<commit_message>
More normalization of ASR alignment output
</commit_message>
<xml_diff>
--- a/results/selected_sessions_normalized.xlsx
+++ b/results/selected_sessions_normalized.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB4"/>
+  <dimension ref="A1:AM4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,107 +471,162 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>Nvidia-Parakeet-ASR</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>norm_human_transcript</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>norm_whisper_asr</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>norm_phi4_asr</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>norm_parakeet_asr</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>norm_whisper_asr_wer</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>norm_whisper_asr_ins</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>norm_whisper_asr_del</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>norm_whisper_asr_sub</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>norm_phi4_asr_wer</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>norm_phi4_asr_ins</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>norm_phi4_asr_del</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>norm_phi4_asr_sub</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>norm_parakeet_asr_wer</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>norm_parakeet_asr_ins</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>norm_parakeet_asr_del</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>norm_parakeet_asr_sub</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>norm_whisper_asr_Deletions</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>norm_whisper_asr_Insertions</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>norm_whisper_asr_Substitutions</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>norm_phi4_asr_Deletions</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>norm_phi4_asr_Insertions</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>norm_phi4_asr_Substitutions</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>norm_parakeet_asr_Deletions</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>norm_parakeet_asr_Insertions</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>norm_parakeet_asr_Substitutions</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>whisper_aligned_df</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>phi4_aligned_df</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>parakeet_aligned_df</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>whisper_reconstructed_ref</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>phi4_reconstructed_ref</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>parakeet_reconstructed_ref</t>
         </is>
       </c>
     </row>
@@ -611,74 +666,111 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>hello can you hear me ok ohh yes i can can you hear me yeah good good so my name is joe i am a doctor um here at babylon can i just confirm your name please uh my names vincent and your date of birth uh uh ninth of may two thousand and sixteen ok great  and are you in a uh a safe place ohh sorry a safe and  confidential place to talk and just  happy to go ahead with the consultation yeah yeah i am yes yes i am great so how can i help yeah so have a  i have been having a cough and a sore throat for about a week and its been causing me problems i have had to stay away from work for about three or four of those days because of how bad is ok i am sorry to hear that so you have had a cough and a sore throat for about a week and what came what what came first yes uh the sore throat came first and then after a day or two the cough ok ok and uh are you coughing up anything no its very dry ok so i am i am just going to ask a few questions about the uh your current symptoms and a little bit about your background um and something else about what we can do a little bit later on in the consultation to help you so before we go on  anything you are particularly concerned about um or have any ideas what might be going on you said that you had a cold ok  well i mean you  you know how we all are once this happens you google it and there seems to be all kinds of bad things it could be it could be could be a cold or flu obviously but it could also be tuberculosis it could be cancer always comes up so it will be good if none of those great so so yeah i can provide a bit of reassurance um and uh we can talk about those a little bit as well and was there anything you were particularly expecting or hoping to get out of this consultation um ok uh uh well uh yeah so reassurance so like hopefully some sense that its not anything too serious but also is there anything you can prescribe me to make it better or any advice or maybe even a sick note so that if i need to stay away from work for a bit longer i can get one sure sure ok all right so well talk a little bit about the symptoms and i am sure we can  get a um those things uh  and some reassurance um about your concerns ok so um you mentioned that you started with sore throat about a week ago developed into bit of a dry cough um  ill just ask a few questions around those so um do you have any shortness of breath no yes yes i have been having shortness of  yeah i have been having shortness of breath yeah you are short of breath and uh do you have any wheeze or chest pain uh yeah a bit of both  you are you are feeling a bit wheezy with some chest pain as well yes ok and how ah when did you start to develop the shortness of breath  so so the sore throat so todays friday sore throat was about last week friday or thursday cough was saturday or sunday so the so the shortness of breath was i think shortly after the cough so maybe a day or two later so three four days ago three or four days ago you started develop  and is the cough worse at nighttime no no its the same throughout the whole day same throughout the day um and uh when you say you are short of breath just need to try and get an idea about how short of breath you are so are you able to so  um so uh like walk up a flight of stairs for example um or or are you short of breath at rest ohh yeah its its like so when i am doing walking um and i do exercises now and then so it it has not been  superbad like has not stopped me from doing any of those things but its been pretty unusual and a little bit worrying and you are a bit concerned about that ok so i just need to ask a few uh things about your background as well so um do you have any other medical conditions or medical history no just no no  past medical history no no  no history of asthma no um and any uh uh history of uh clots on your legs or your lungs so these  uh no one in your familys had those clots on the legs or the lungs  well my mother had lung cancer your mother had lung cancer do you smoke no you ever smoked or been exposed to asbestos that you know of do not know with asbestos ever smoked  i mean once or twice in amsterdam if that counts but not really ok um and uh this so just going back to the your symptoms of shortness of breath with the cough its a dry cough no you are not coughing up any flem um do do you have uh and you do not you say you do not have any chest pain as such um uh are you taking any medications currently at the moment uh no no ok are you allergic to any medications not to any medication but i am allergic to peanuts peanuts ok um and uh you mentioned that your mother had uh lung cancer um any other family history of any significant illnesses uh run running in your family no no that is the only one just lung cancer from my mother just lung cancer ok and you say you have a cold so do you have  sinus congestion or um no it seems to be   entirely with just my throat so like my nose is  like  so  just your just your throat and any recent travel or have you always lived in the uk uh no so i i i have not always lived in the uk like so i was born in the us and moved over well it was twelve years ago but in terms of recent travel just to europe nowhere too exotic ok so no so no recent travel no significant recent travel any anywhere um ok and are you coughing up anything other than  um uh so you you are not coughing up blood or anything like that no no um good and uh are you feeling feverish hot cold sweaty yeah so a little bit feverish uh um at first so the first three or so days of this but then it the fevers gone away ok and in general do you  sorry yeah  yeah i was just going to say also had a bit of a headache but like headaches that come and go rather but like right now its fine uh ok and in general would you say you are feeling you are you are beginning to to feel better worse or or sort of um staying the same  so its like its up and down so so let us see so i  it started last week and i stayed home from work two days this week i think it was maybe tuesday and then thursday so like i felt better and then worse again and then better and then worse again so its been yeah a kind of constant but constant and being variable if that makes  ok and i just  need to ask any other sort of risk factors um that you may have so  um no sort of significant weight loss um or unexplained weight loss any  so no weight loss but i have been have been losing my appetite recently and i mean i usually eat a lot so and i and i enjoy eating as well but like so that is been a bit concerning you have been losing your appetite recently yes and you are a little bit concerned about that but you have not you have not lost any weight that you think of yes no not that  and any um sort of rashes or anything or uh  and you no not  not that not that you can think of ok um so i would ask to examine you now but um i i do not know if i could sort of look inside your throat at least to see if there is a probably there is ohh we can try  ohh no well no its ok i  might think about doing a have you got any lumps or bumps around your neck that you can feel  uh no no that you no ok um and so finally you you were talking about uh  i mean it sounds to me that um you have been a little bit up and down sore throat developed a dry cough um you are slightly short of breath but not too overly concerningly short of breath what i would say were just coming to the end of consultation now  if you feel significantly worse  mmhmm um uh if you get more short of breath or sudden change in your breathlessness um or breathlessness that you are concerned about then i would advise you to see no  go and see a gp um and actually see somebody physically um uh but i think for now i can sort of uh try and reassure you that um if this clears up as i expect it would so i expect this to sort of be getting better in the next four or five days um if its not please get in touch with a medical professional again um and uh i would expect it to and so therefore i would not be concerned about tuberculosis um your concerns about lung cancer are and was that the other thing you are concerned about ohh yeah yeah yeah yeah so so um again if you are not getting better please see somebody again um i have just got four seconds now so nice talking to you and have we got to we got to tidy up yeah ok so uh all right uh and ill provide you with a sick note just to give you a few more days off work um and paracetemol lots of fluids um and uh rest up and as i say if you are not feeling better please get in touch ok  have a good day  thank you bye</t>
+          <t>Hello, can you hear me okay? Hey, yes, I can. Can you hear me? Yeah, good, good. So my name is Joe. I'm a doctor here at Babylon. Can I just confirm your name, please? Hey, my name's Vincent. And your date of birth? 9th of May 2016. Okay, great. And are you in a safe place? Oh, sorry, a safe and confidential place to talk and just have to go ahead with the consultation. Yes, yes, I am. Great. So how can I help? Yeah, so I have a call up. I've been having a cough and a sore throat for about a week and it's been causing me problems. I've had to stay away from work for about three or four of those days because of a bandit. Okay, I'm sorry to hear that. So you've had a cough and a sore throat for about a week. And what came first? The sore throat came first and then after a day or two the cough. Okay, okay. And are you coughing up anything? No, it's very dry. Okay. So I'm just going to ask a few questions about your current symptoms and then a little bit about your background and something else about what we can do a little bit later on in the consultation to help you. But before I go on, anything you're particularly concerned about or have any ideas what might be going on? You said that you had a cold. Well, I mean, you know how we all are. Once this happens, you Google it and it seems to be all kinds of bad things. It could be, it could be, it could be a cold or flu, obviously, but tuberculosis, it could be cancer, always comes up. So it'll be good if none of those. Right. So yeah, I can provide a little bit of reassurance and we can talk about those a little bit as well. And was there anything you were particularly expecting or hoping to get out of this consultation? Well, yeah, so reassurance. So hopefully some sense that it's not anything too serious. But also, if there's anything you can prescribe me to make it better or any advice, or maybe even a sick note. So if I need to stay away from work for a bit longer, I can get one. Sure, sure. Okay. All right. So we'll talk a little bit about the symptoms and I'm sure we can get those things and some reassurance about your concerns. So you mentioned that you started with a sore throat about a week ago, developed into a bit of a dry cough. I'll just ask a few questions around those. So do you have any shortness of breath? Yes, yes. I've been having shortness of breath. Yeah, I've been having shortness of breath. You are short of breath. And do you have any wheeze or chest pain? Yeah, a bit of four attacks. You're feeling a bit wheezy with some chest pain as well. Yes. Okay. And how when did you start to develop the shortness of breath? I think so. So the sore throat, so today is Friday. The sore throat was about last week, Friday or Thursday. Cough was satisfied. So the shortness of breath was, I think, shortly after the cough, so maybe a day or two later, so three, four days ago? Three or four days ago, you started developing. And is the cough worse at night time? No, it's the same throughout the week. Same throughout the day. And when you say you're short of breath, just need to try and get an idea about how short of breath you are. So are you able to get walk up a flight of stairs, for example, or are you short of breath at rest? Oh, yeah, it's like when I'm doing walking and I do exercise now and then. So it hasn't been super bad. Like it hasn't stopped me from doing any of those things, but it's been pretty unusual and a little bit worried. And you're a bit concerned about that, okay? So I just need to ask a few things about your background as well. So do you have any other medical conditions or medical history? No, just no, no past medical history now. No past microgravity. No history of asthma? No. And any history of clots on your legs or your lungs? So these are DVDs or Ps. None in your family's had those clots in the legs or lungs? Well, my mother had lung cancer. Your mother had lung cancer. Do you smoke? No. Have you ever smoked or been exposed to asbestos? You know? Don't know if asbestos ever smoked. I mean, once or twice in Amsterdam, but not really. Okay. And this, just going back to your symptoms of shortness of breath with the cough, it's a dry cough. No, you're not coughing up anyphlem. Do you have, and you say you don't have any chest pain as such? Are you taking any medications currently at the moment? No, no. Okay. Are you allergic to any medications? Not to any medication, but I'm allergic to peanuts. Peanuts, okay. And you mentioned that your mother had lung cancer. Any other family history of any significant illnesses when running in your family? No, no, that's the only one. Just lung cancer from my mother. Just lung cancer. Okay. And you say you have a cold. So do you have sinus congestion or? No, it seems to be all entirely with just my throat. Like my nose is tiny now. Just your throat and any recent travel or have you always lived in the UK? No, so I haven't always lived in the UK. So I was born in the US and moved over 12 years ago, but in terms of recent travel, just to Europe, to exotic. Okay, so no recent travel, no significant recent travel anywhere. Okay. And are you coughing up anything other than, so you're not coughing up blood or anything like that? No. Good. And are you feeling feverish, hot cold, sweaty? Yeah, so a little bit feverish at first. So the first three or so days of this, but then the fever's gone away. Okay. And in general, do you feel? Yeah, I was just going to say also had a bit of a headache. Like headaches that come and go rather, but like right now it's fine. Okay. And in general, would you say you're feeling you're beginning to feel better, worse, or sort of staying the same? So it's like it's up and down. So let's see. So I started last week and I stayed home from work two days this week. I think it was maybe Tuesday and then Thursday. So like I felt better and then worse again and then better and then worse again. So it's been a kind of constant but constant in being variable if that make me. Okay and I just need to ask any other sort of risk factors that you may have. So no sort of significant weight loss or unexplained weight loss? Any waters? So no weight loss but I have been have been losing my appetite recently and I mean I usually eat a lot so I enjoy eating as well but like that's been a bit concerning. You've been losing your appetite recently. Yes. And you're a little bit concerned about that. But you haven't you haven't lost any weight that you think of? No, not that. And any sort of rashes or anything? No rash. Okay. So I would ask to examine you now but I don't know if I could sort of look inside your throat at least to see if there's a probably we can try. Oh no well no it's okay I might think about doing that. Have you got any lumps or bumps around your neck that you can feel? No? No. Okay. And so finally you were talking about I mean it sounds to me that you've been a little bit up and down, sore throat, developed a dry cough. You are slightly short of breath but not too overly concerningly short of breath. What I would say we're just coming to the end of the consultation now is if you feel significantly worse if you get more short of breath or sudden change in your breathlessness or breathlessness that you are concerned about and I would advise you to seek medical tension games here GP and actually see somebody physically but I think for now I can sort of try and reassure you that if this clears up as I expect it would so expect this to sort of be getting better in the next four or five days if it's not please get in touch with the medical professional again and I would expect it too and so therefore I wouldn't be concerned about tuberculosis your concerns about lung cancer are was that the other thing you concerned about yeah oh yeah yeah so so again if you're not getting better please see somebody again I've just got four seconds now so nice talking to you and we've got to tidy up yeah okay so and I'll provide you with a sick note just to give you a few more days off work and paracetamol lots of fluids and rest up and as I say if you're not feeling better please get in touch okay all right thanks a lot have a good day thank you</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>hello can you hear me okay yes i can can you hear me yeah good good so my name is joe i am a doctor here at babylon can i just confirm your name please my name is vincent and your date of birth nineth of may two thousand and sixteen okay great sorry i know you in a uh a safe place oh sorry a safe and confidential place to talk and just i have to go ahead with the consultation yes yes i am great so how can i help yeah so i have a call that i have been having a cough and a sore throat for about a week and its been causing me problems i have had to stay away from work for about three or four of those days because of a bad history okay i am sorry to hear that so you have had a cough and a sore throat for about a week and what came first the sore throat came first and then after a day or two the cough okay and i just want to thank a few questions about your current symptoms and then a little bit about your background and something else about what we can do a little bit later on in the consultation to help you but before we go on anything you are particularly concerned about or have any ideas what might be going on you said that you had a cold well i mean you know how we all are once this happens you google it and it seems to be all kinds of bad things it could be a cold or flu obviously obviously because we tuberculosis the cancer always comes up so it will be good if those right say say yeah i can provide a little bit of reassurance and we can talk about those a little bit as well and was there any you are particularly expecting or hoping to get out of this consultation well yeah so reassurance so hopefully some sense that its not anything too serious but also if there is anything you can prescribe me to make it better or any advice or maybe even a sick note so if i need to stay away from work for a bit longer i can get one sure sure okay all right so well talk a little bit about the symptoms and i am sure we can get those things some secrets and some reassurance thank you about your concerns so you mentioned that you started with a sore throat about a week ago developed into a bit of a dry cough and i just ask a few questions around those those so do you have any shortness of breath yes yes were having shorts oh yeah i have been having shortness of breath you are short of breath and do you have any wheeze or chest pain yeah you are feeling a bit wheezy with some chest pain as well yes okay and when did you start to develop a shortness of breath let us see so the sore throat so today is friday sore throat was about last friday or thursday cough was saturday or sunday so the shortness of breath was i think shortly after the cough so maybe a day or two later so three or four days ago three or four days ago you started developing and is the cough worse at night time no its the same throughout the day and when you say you are short of breath just need to try and get an idea about how short of breath you are so are you able to like walk up flights of stairs for example or are you short breath of rest oh yeah its like when i am doing walking and i do exercise now and then so it has not been super bad like has not stopped me from doing any of those things but its been pretty unusual and a little bit worried and you are a bit concerned about that okay so i just need to ask a few things about your background as well so do you have any other medical conditions or medical history no just no no no history of asthma no and any history of clots on your legs or your lungs these are ddts or ps no one in your familys had those clots on the legs or the lungs well my mother had lung cancer your mother had lung cancer do you smoke no have you ever smoked or been exposed to asbestos i do not know if asbestos ever smoked i mean once or twice in amsterdam in dakar but not really okay and this just going back to your symptoms of shortness of breath with the cough its a dry cough not cough cap flem do you have and you say you do not have any chest pain as such are you taking any medications currently at the moment no i am not okay are you allergic to any medications not to any medication but i am allergic to peanuts peanuts okay and you mentioned that your mother had lung cancer any other family history of any significant illnesses when running into family no no that is the only one just lung cancer from my mother okay and you say you have a cold so do you have sinus congestion or no it seems to be all entirely with just my throat like my nose is just running out just your throat and any recent travel or have you always lived in the uk no so i i have not always lived in the uk like so i was born in the us and twelve years ago but its a recent travel just to europe nowhere to exotic okay so no so no recent travel no significant recent travel anywhere um okay and are you coughing up anything other than um so you are not coughing up blood or anything like that um good and uh are you feeling feverish hot cold sweaty so a little bit feverish at first so the first three or so days of this but then the fevers gone away ok and in general do you feel better sorry yeah yeah i was just going to say i also had a bit of a headache like headaches that come and go rather but right now its fine ok and in general would you say you are beginning to feel better worse or sort of staying the same so its like its up and down so let us see so i started last week and i stayed home from work two days this week i think it was maybe tuesday and then thursday so like i felt better and then worse again and then better and then worse again so its been a kind of constant but constant in being variable okay and i just need to ask any other sort of risk factors um that you may have so um no sort of significant weight loss um or unexplained weight loss any so no no weight loss but i have been losing my appetite recently and i mean i usually eat a lot so i enjoy eating as well but that is been a bit concerning you have been losing your appetite recently yes and you are a little bit concerned about that but you have not lost any weight lost any weight that you think no not that and any um sort of rashes or anything uh and you no no okay um so i would ask to examine you now but um i i do not know if i could sort of look inside your throat at least see if there is a probably we can try oh no well no its okay i might think about doing have you got any lumps or bumps around your neck that you could feel no not the no okay and and so finally you were talking about i it sounds to me that you have been a little bit up and down sore throat developed a dry cough you are slightly short of breath but not too overly concerningly short of breath what i would say were just coming to the end of the consultation now is if you feel significantly worse if you get more short of breath or sudden change in your breathlessness or breathlessness that you are concerned about and i would advise you to see a gp and actually see something physically but i think for now i can sort of try and reassure you that if this clears up as i expect it would so expect this to sort of be getting better in the next four or five days if its not please get in touch with the medical professional again and i would expect it to and so therefore i would not be concerned about tuberculosis your concerns about lung cancer are was that the other thing you were concerned about oh yeah yeah so again if you are not getting better please see somebody again i have just got four seconds now so nice talking to you and we have got to tidy up yeah okay okay so and ill provide you with a sick note just to give you a few more days of work and paracetamol lots of fluids and rest up and as i say if you are not feeling better please get in touch okay all right thank you</t>
+          <t>hello can you hear me okay oh yes i can can you hear me yeah good good so my name is joe i am a doctor  here at babylon can i just confirm your name please  my names vincent and your date of birth   ninth of may two thousand and sixteen okay great and are you in a  a safe place oh sorry a safe and confidential place to talk and just happy to go ahead with the consultation yeah yeah i am yes yes i am great so how can i help yeah so have a i have been having a cough and a sore throat for about a week and it is been causing me problems i have had to stay away from work for about three or four of those days because of how bad is okay i am sorry to hear that so you have had a cough and a sore throat for about a week and what came what what came first yes  the sore throat came first and then after a day or two the cough okay okay and  are you coughing up anything no it is very dry okay so i am i am just going to ask a few questions about the  your current symptoms and a little bit about your background  and something else about what we can do a little bit later on in the consultation to help you so before we go on anything you are particularly concerned about  or have any ideas what might be going on you said that you had a cold okay well i mean you you know how we all are once this happens you google it and there seems to be all kinds of bad things it could be it could be could be a cold or flu obviously but it could also be tuberculosis it could be cancer always comes up so it will be good if none of those great so so yeah i can provide a bit of reassurance  and  we can talk about those a little bit as well and was there anything you were particularly expecting or hoping to get out of this consultation  okay   well  yeah so reassurance so like hopefully some sense that it is not anything too serious but also is there anything you can prescribe me to make it better or any advice or maybe even a sick note so that if i need to stay away from work for a bit longer i can get one sure sure okay all right so we will talk a little bit about the symptoms and i am sure we can get a  those things  and some reassurance  about your concerns okay so  you mentioned that you started with sore throat about a week ago developed into bit of a dry cough  i will just ask a few questions around those so  do you have any shortness of breath no yes yes i have been having shortness of yeah i have been having shortness of breath yeah you are short of breath and  do you have any wheeze or chest pain  yeah a bit of both you are you are feeling a bit wheezy with some chest pain as well yes okay and how  when did you start to develop the shortness of breath so so the sore throat so todays friday sore throat was about last week friday or thursday cough was saturday or sunday so the so the shortness of breath was i think shortly after the cough so maybe a day or two later so three four days ago three or four days ago you started develop and is the cough worse at nighttime no no it is the same throughout the whole day same throughout the day  and  when you say you are short of breath just need to try and get an idea about how short of breath you are so are you able to so  so  like walk up a flight of stairs for example  or or are you short of breath at rest oh yeah it is it is like so when i am doing walking  and i do exercises now and then so it it has not been superbad like has not stopped me from doing any of those things but it is been pretty unusual and a little bit worrying and you are a bit concerned about that okay so i just need to ask a few  things about your background as well so  do you have any other medical conditions or medical history no just no no past medical history no no no history of asthma no  and any   history of  clots on your legs or your lungs so these  no one in your familys had those clots on the legs or the lungs well my mother had lung cancer your mother had lung cancer do you smoke no you ever smoked or been exposed to asbestos that you know of do not know with asbestos ever smoked i mean once or twice in amsterdam if that counts but not really okay  and  this so just going back to the your symptoms of shortness of breath with the cough it is a dry cough no you are not coughing up any flem  do do you have  and you do not you say you do not have any chest pain as such   are you taking any medications currently at the moment  no no okay are you allergic to any medications not to any medication but i am allergic to peanuts peanuts okay  and  you mentioned that your mother had  lung cancer  any other family history of any significant illnesses  run running in your family no no that is the only one just lung cancer from my mother just lung cancer okay and you say you have a cold so do you have sinus congestion or  no it seems to be entirely with just my throat so like my nose is like so just your just your throat and any recent travel or have you always lived in the uk  no so i i i have not always lived in the uk like so i was born in the us and moved over well it was twelve years ago but in terms of recent travel just to europe nowhere too exotic okay so no so no recent travel no significant recent travel any anywhere  okay and are you coughing up anything other than   so you you are not coughing up blood or anything like that no no  good and  are you feeling feverish hot cold sweaty yeah so a little bit feverish   at first so the first three or so days of this but then it the fevers gone away okay and in general do you sorry yeah yeah i was just going to say also had a bit of a headache but like headaches that come and go rather but like right now it is fine  okay and in general would you say you are feeling you are you are beginning to to feel better worse or or sort of  staying the same so it is like it is up and down so so let us see so i it started last week and i stayed home from work two days this week i think it was maybe tuesday and then thursday so like i felt better and then worse again and then better and then worse again so it is been yeah a kind of constant but constant and being variable if that makes okay and i just need to ask any other sort of risk factors  that you may have so  no sort of significant weight loss  or unexplained weight loss any so no weight loss but i have been have been losing my appetite recently and i mean i usually eat a lot so and i and i enjoy eating as well but like so that is been a bit concerning you have been losing your appetite recently yes and you are a little bit concerned about that but you have not you have not lost any weight that you think of yes no not that and any  sort of rashes or anything or  and you no not not that not that you can think of okay  so i would ask to examine you now but  i i do not know if i could sort of look inside your throat at least to see if there is a probably there is oh we can try oh no well no it is okay i might think about doing a have you got any lumps or bumps around your neck that you can feel  no no that you no okay  and so finally you you were talking about  i mean it sounds to me that  you have been a little bit up and down sore throat developed a dry cough  you are slightly short of breath but not too overly concerningly short of breath what i would say we are just coming to the end of consultation now if you feel significantly worse    if you get more short of breath or sudden change in your breathlessness  or breathlessness that you are concerned about then i would advise you to see no go and see a gp  and actually see somebody physically   but i think for now i can sort of  try and reassure you that  if this clears up as i expect it would so i expect this to sort of be getting better in the next four or five days  if it is not please get in touch with a medical professional again  and  i would expect it to and so therefore i would not be concerned about tuberculosis  your concerns about lung cancer are and was that the other thing you are concerned about oh yeah yeah yeah yeah so so  again if you are not getting better please see somebody again  i have just got four seconds now so nice talking to you and have we got to we got to tidy up yeah okay so  all right  and i will provide you with a sick note just to give you a few more days off work  and paracetemol lots of fluids  and  rest up and as i say if you are not feeling better please get in touch okay have a good day thank you bye</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>hello can you hear me okay hey yes i can can you hear me yeah good good so my name is joe i am a doctor here at babylon can i just confirm your name please hey my name is vincent and your date of birth ah nine of may two thousand and sixteen okay great sorry and are you in a be a safe place oh sorry a safe and confidential place to talk and discuss yeah i am happy to go ahead with the consultation yes yes i am great so how can i help yeah so i have a call up i have been having a cough and a sore throat for about a week and its been causing me problems i have had to stay away from work for about three or four of those days because of it okay i am sorry to hear that so you have had a cough and a sore throat for about a week and what came what came first the sore throat came first and then after a day or two the cough okay and are you coughing up anything no its very dry okay so i am just going to ask a few questions about the your current symptoms and then a little bit about your background and something else about what we can do a little bit later on in the consultation to help you but before we go on anything you are particularly concerned about or have any right so so yeah i can provide a little bit of reassurance um and uh we can talk about those a little bit as well was there anything you were particularly expecting or hoping to get out of this consultation well yeah so reassurance so like hopefully in some sense that is not anything too serious but also is there anything you can prescribe me to make it better or any advice or maybe even a sick note so that if i need to stay away from work for a bit longer i can get one sure sure okay all right so well talk a little bit about the symptoms and i am sure we can get a those things sorted and some reassurance thank you about your concerns so um you mentioned that you started with a sore throat about a week ago developed into a bit of a dry cough and ill just ask a few questions around those so um do you have any shortness of breath yes yes i have been having shortness of oh yeah i have been having shortness of breath yeah you are short of breath and uh do you have any wheeze or chest pain yeah you are feeling a bit wheezy with some chest pain as well yes okay and how when did you start to develop the shortness of breath so the sore throat so today is friday sore throat was about friday or thursday cough was saturday or sunday so the shortness of breath was i think shortly after the cough so maybe a day or two later so three or four days ago two or four days ago you start to develop symptoms and is the cough worse at night time no no its the same throughout the day same throughout the day and when you say you are short of breath just need to try and get an idea about how short of breath you are so are you able to like walk up a flight of stairs for example or are you short of breath at rest oh yeah its like when i am doing walking and i do exercise now and then so it it has not been super bad like has not stopped me from doing any of those things but its been pretty unusual and a little bit worrying and you are a bit concerned about that okay so i just need to ask a few things about your background as well so do you have any other medical conditions or medical history no just no no past medical history no no history of asthma no and any history of clots on your legs or your lungs so these are ddps or ps and none of your families had those clots in the legs or lungs well my mother had lung cancer your mother had lung cancer do you smoke no you ever smoked or been exposed to asbestos you know do not know if asbestos ever smoked i mean once or twice in amsterdam with that car but not really okay um and ah this so just going back to the your symptoms of shortness of breath with the cough its a dry cough no you are not coughing up any phlegm um do you do you have and you say you do not have any chest pain as such um are you taking any medications currently at the moment no i am not okay are you allergic to any medications not any medication but i am allergic to peanuts peanuts okay and and you mentioned that your mother had lung cancer and any other family history of any significant illnesses when running in your family no no that is the only one just lung cancer from my mother just lung cancer okay and you say you have a cold so do you have sinus congestion or um no it seems to be almost entirely just my throat like j just your just your throat and any recent travel or have you always lived in the you k uh no so i i have not always lived in the you k like so i was born in the you s and moved over about twelve years ago but in terms of recent travel just to europe nowhere to exotic okay so no so no recent travel no significant recent travel anywhere um okay and are you coughing up anything other than um so you are not coughing up blood or anything like that no um good and are you feeling feverish hot cold sweaty yeah so a little bit feverish um at first so the first three or so days of this but then the fevers gone away okay and in general do you sorry yeah i was just going to say also had a bit of a headache like headaches that come and go rather but like right now its fine okay and in general would you say you are feeling you are you are beginning to to feel better worse or or sort of staying the same so its like its up and down so so let us see so i started last week and i stayed home from work two days this week i think it was maybe tuesday and then thursday so like i felt better and then worse again and then better and then worse again so its been yeah a kind of constant but constant in being variable but okay and i just really need to ask any other sort of risk factors um that you may have so um no sort of significant weight loss um or unexplained weight loss any so no weight loss but i have been have been losing my appetite recently and i mean i usually eat a lot so i enjoy eating as well but like that is been a bit concerning you have been losing your appetite recently yes and you are a little bit concerned about that but you have not you have not lost any weight that you think no not that and any um sort of rashes or anything uh and you no rash no you can go okay um so i would ask to examine you now but um i i do not know if i could sort of look inside your throat at least to see if there is a probably there is oh we can try it on oh no well no its okay i might think about doing it have you got any lumps or bumps around your neck that you can feel ah no not the no okay and and so finally you you were talking about i mean it sounds to me that um you have been a little bit up and down sore throat developed a dry cough and you are slightly short of breath but not too overly concerningly short of breath what i would say were just coming to the end so consultation hours is if you feel significantly worse um uh if you get more short of breath or sudden change in your breathlessness um or breathlessness that you are concerned about and i would advise you to see your gp and actually see somebody physically um uh but i think for now i can sort of try and reassure you that um if this clears up as i expected it would so expect this to sort of be getting better in the next four or five days if its not please get in touch with the medical professional again and ill expect it to and so therefore i would not be concerned about tuberculosis your concerns about lung cancer was that the other thing you were concerned about yeah yeah so so um again if you are not getting better please see somebody again i have just got four seconds now so nice talking to you and we have got to we have got to tidy up yeah okay so and ill provide you with a sick note just to give you a few more days off work and paracetamol lots of fluids and rest up and as i say if you are not feeling better please get in touch okay alright have a good day thank you alright</t>
-        </is>
-      </c>
-      <c r="K2" t="n">
-        <v>0.2046204620462046</v>
-      </c>
-      <c r="L2" t="n">
-        <v>30</v>
+          <t>hello can you hear me okay yes i can can you hear me yeah good good so my name is joe i am a doctor here at babylon can i just confirm your name please my name is vincent and your date of birth nineth of may two thousand and sixteen okay great sorry i know you in a  a safe place oh sorry a safe and confidential place to talk and just i have to go ahead with the consultation yes yes i am great so how can i help yeah so i have a call that i have been having a cough and a sore throat for about a week and it is been causing me problems i have had to stay away from work for about three or four of those days because of a bad history okay i am sorry to hear that so you have had a cough and a sore throat for about a week and what came first the sore throat came first and then after a day or two the cough okay and i just want to thank a few questions about your current symptoms and then a little bit about your background and something else about what we can do a little bit later on in the consultation to help you but before we go on anything you are particularly concerned about or have any ideas what might be going on you said that you had a cold well i mean you know how we all are once this happens you google it and it seems to be all kinds of bad things it could be a cold or flu obviously obviously because we tuberculosis the cancer always comes up so it will be good if those right say say yeah i can provide a little bit of reassurance and we can talk about those a little bit as well and was there any you are particularly expecting or hoping to get out of this consultation well yeah so reassurance so hopefully some sense that it is not anything too serious but also if there is anything you can prescribe me to make it better or any advice or maybe even a sick note so if i need to stay away from work for a bit longer i can get one sure sure okay all right so we will talk a little bit about the symptoms and i am sure we can get those things some secrets and some reassurance thank you about your concerns so you mentioned that you started with a sore throat about a week ago developed into a bit of a dry cough and i just ask a few questions around those those so do you have any shortness of breath yes yes we are having shorts oh yeah i have been having shortness of breath you are short of breath and do you have any wheeze or chest pain yeah you are feeling a bit wheezy with some chest pain as well yes okay and when did you start to develop a shortness of breath let us see so the sore throat so today is friday sore throat was about last friday or thursday cough was saturday or sunday so the shortness of breath was i think shortly after the cough so maybe a day or two later so three or four days ago three or four days ago you started developing and is the cough worse at night time no it is the same throughout the day and when you say you are short of breath just need to try and get an idea about how short of breath you are so are you able to like walk up flights of stairs for example or are you short breath of rest oh yeah it is like when i am doing walking and i do exercise now and then so it has not been super bad like has not stopped me from doing any of those things but it is been pretty unusual and a little bit worried and you are a bit concerned about that okay so i just need to ask a few things about your background as well so do you have any other medical conditions or medical history no just no no no history of asthma no and any history of clots on your legs or your lungs these are ddts or ps no one in your familys had those clots on the legs or the lungs well my mother had lung cancer your mother had lung cancer do you smoke no have you ever smoked or been exposed to asbestos i do not know if asbestos ever smoked i mean once or twice in amsterdam in dakar but not really okay and this just going back to your symptoms of shortness of breath with the cough it is a dry cough not cough cap flem do you have and you say you do not have any chest pain as such are you taking any medications currently at the moment no i am not okay are you allergic to any medications not to any medication but i am allergic to peanuts peanuts okay and you mentioned that your mother had lung cancer any other family history of any significant illnesses when running into family no no that is the only one just lung cancer from my mother okay and you say you have a cold so do you have sinus congestion or no it seems to be all entirely with just my throat like my nose is just running out just your throat and any recent travel or have you always lived in the uk no so i i have not always lived in the uk like so i was born in the us and twelve years ago but it is a recent travel just to europe nowhere to exotic okay so no so no recent travel no significant recent travel anywhere  okay and are you coughing up anything other than  so you are not coughing up blood or anything like that  good and  are you feeling feverish hot cold sweaty so a little bit feverish at first so the first three or so days of this but then the fevers gone away okay and in general do you feel better sorry yeah yeah i was just going to say i also had a bit of a headache like headaches that come and go rather but right now it is fine okay and in general would you say you are beginning to feel better worse or sort of staying the same so it is like it is up and down so let us see so i started last week and i stayed home from work two days this week i think it was maybe tuesday and then thursday so like i felt better and then worse again and then better and then worse again so it is been a kind of constant but constant in being variable okay and i just need to ask any other sort of risk factors  that you may have so  no sort of significant weight loss  or unexplained weight loss any so no no weight loss but i have been losing my appetite recently and i mean i usually eat a lot so i enjoy eating as well but that is been a bit concerning you have been losing your appetite recently yes and you are a little bit concerned about that but you have not lost any weight lost any weight that you think no not that and any  sort of rashes or anything  and you no no okay  so i would ask to examine you now but  i i do not know if i could sort of look inside your throat at least see if there is a probably we can try oh no well no it is okay i might think about doing have you got any lumps or bumps around your neck that you could feel no not the no okay and and so finally you were talking about i it sounds to me that you have been a little bit up and down sore throat developed a dry cough you are slightly short of breath but not too overly concerningly short of breath what i would say we are just coming to the end of the consultation now is if you feel significantly worse if you get more short of breath or sudden change in your breathlessness or breathlessness that you are concerned about and i would advise you to see a gp and actually see something physically but i think for now i can sort of try and reassure you that if this clears up as i expect it would so expect this to sort of be getting better in the next four or five days if it is not please get in touch with the medical professional again and i would expect it to and so therefore i would not be concerned about tuberculosis your concerns about lung cancer are was that the other thing you were concerned about oh yeah yeah so again if you are not getting better please see somebody again i have just got four seconds now so nice talking to you and we have got to tidy up yeah okay okay so and i will provide you with a sick note just to give you a few more days of work and paracetamol lots of fluids and rest up and as i say if you are not feeling better please get in touch okay all right thank you</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>hello can you hear me okay hey yes i can can you hear me yeah good good so my name is joe i am a doctor here at babylon can i just confirm your name please hey my name is vincent and your date of birth  nine of may two thousand and sixteen okay great sorry and are you in a be a safe place oh sorry a safe and confidential place to talk and discuss yeah i am happy to go ahead with the consultation yes yes i am great so how can i help yeah so i have a call up i have been having a cough and a sore throat for about a week and it is been causing me problems i have had to stay away from work for about three or four of those days because of it okay i am sorry to hear that so you have had a cough and a sore throat for about a week and what came what came first the sore throat came first and then after a day or two the cough okay and are you coughing up anything no it is very dry okay so i am just going to ask a few questions about the your current symptoms and then a little bit about your background and something else about what we can do a little bit later on in the consultation to help you but before we go on anything you are particularly concerned about or have any right so so yeah i can provide a little bit of reassurance  and  we can talk about those a little bit as well was there anything you were particularly expecting or hoping to get out of this consultation well yeah so reassurance so like hopefully in some sense that is not anything too serious but also is there anything you can prescribe me to make it better or any advice or maybe even a sick note so that if i need to stay away from work for a bit longer i can get one sure sure okay all right so we will talk a little bit about the symptoms and i am sure we can get a those things sorted and some reassurance thank you about your concerns so  you mentioned that you started with a sore throat about a week ago developed into a bit of a dry cough and i will just ask a few questions around those so  do you have any shortness of breath yes yes i have been having shortness of oh yeah i have been having shortness of breath yeah you are short of breath and  do you have any wheeze or chest pain yeah you are feeling a bit wheezy with some chest pain as well yes okay and how when did you start to develop the shortness of breath so the sore throat so today is friday sore throat was about friday or thursday cough was saturday or sunday so the shortness of breath was i think shortly after the cough so maybe a day or two later so three or four days ago two or four days ago you start to develop symptoms and is the cough worse at night time no no it is the same throughout the day same throughout the day and when you say you are short of breath just need to try and get an idea about how short of breath you are so are you able to like walk up a flight of stairs for example or are you short of breath at rest oh yeah it is like when i am doing walking and i do exercise now and then so it it has not been super bad like has not stopped me from doing any of those things but it is been pretty unusual and a little bit worrying and you are a bit concerned about that okay so i just need to ask a few things about your background as well so do you have any other medical conditions or medical history no just no no past medical history no no history of asthma no and any history of clots on your legs or your lungs so these are ddps or ps and none of your families had those clots in the legs or lungs well my mother had lung cancer your mother had lung cancer do you smoke no you ever smoked or been exposed to asbestos you know do not know if asbestos ever smoked i mean once or twice in amsterdam with that car but not really okay  and  this so just going back to the your symptoms of shortness of breath with the cough it is a dry cough no you are not coughing up any phlegm  do you do you have and you say you do not have any chest pain as such  are you taking any medications currently at the moment no i am not okay are you allergic to any medications not any medication but i am allergic to peanuts peanuts okay and and you mentioned that your mother had lung cancer and any other family history of any significant illnesses when running in your family no no that is the only one just lung cancer from my mother just lung cancer okay and you say you have a cold so do you have sinus congestion or  no it seems to be almost entirely just my throat like j just your just your throat and any recent travel or have you always lived in the you k  no so i i have not always lived in the you k like so i was born in the you s and moved over about twelve years ago but in terms of recent travel just to europe nowhere to exotic okay so no so no recent travel no significant recent travel anywhere  okay and are you coughing up anything other than  so you are not coughing up blood or anything like that no  good and are you feeling feverish hot cold sweaty yeah so a little bit feverish  at first so the first three or so days of this but then the fevers gone away okay and in general do you sorry yeah i was just going to say also had a bit of a headache like headaches that come and go rather but like right now it is fine okay and in general would you say you are feeling you are you are beginning to to feel better worse or or sort of staying the same so it is like it is up and down so so let us see so i started last week and i stayed home from work two days this week i think it was maybe tuesday and then thursday so like i felt better and then worse again and then better and then worse again so it is been yeah a kind of constant but constant in being variable but okay and i just really need to ask any other sort of risk factors  that you may have so  no sort of significant weight loss  or unexplained weight loss any so no weight loss but i have been have been losing my appetite recently and i mean i usually eat a lot so i enjoy eating as well but like that is been a bit concerning you have been losing your appetite recently yes and you are a little bit concerned about that but you have not you have not lost any weight that you think no not that and any  sort of rashes or anything  and you no rash no you can go okay  so i would ask to examine you now but  i i do not know if i could sort of look inside your throat at least to see if there is a probably there is oh we can try it on oh no well no it is okay i might think about doing it have you got any lumps or bumps around your neck that you can feel  no not the no okay and and so finally you you were talking about i mean it sounds to me that  you have been a little bit up and down sore throat developed a dry cough and you are slightly short of breath but not too overly concerningly short of breath what i would say we are just coming to the end so consultation hours is if you feel significantly worse   if you get more short of breath or sudden change in your breathlessness  or breathlessness that you are concerned about and i would advise you to see your gp and actually see somebody physically   but i think for now i can sort of try and reassure you that  if this clears up as i expected it would so expect this to sort of be getting better in the next four or five days if it is not please get in touch with the medical professional again and i will expect it to and so therefore i would not be concerned about tuberculosis your concerns about lung cancer was that the other thing you were concerned about yeah yeah so so  again if you are not getting better please see somebody again i have just got four seconds now so nice talking to you and we have got to we have got to tidy up yeah okay so and i will provide you with a sick note just to give you a few more days off work and paracetamol lots of fluids and rest up and as i say if you are not feeling better please get in touch okay alright have a good day thank you alright</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>hello can you hear me okay hey yes i can can you hear me yeah good good so my name is joe i am a doctor here at babylon can i just confirm your name please hey my names vincent and your date of birth nineth of may two thousand and sixteen okay great and are you in a safe place oh sorry a safe and confidential place to talk and just have to go ahead with the consultation yes yes i am great so how can i help yeah so i have a call up i have been having a cough and a sore throat for about a week and it is been causing me problems i have had to stay away from work for about three or four of those days because of a bandit okay i am sorry to hear that so you have had a cough and a sore throat for about a week and what came first the sore throat came first and then after a day or two the cough okay okay and are you coughing up anything no it is very dry okay so i am just going to ask a few questions about your current symptoms and then a little bit about your background and something else about what we can do a little bit later on in the consultation to help you but before i go on anything you are particularly concerned about or have any ideas what might be going on you said that you had a cold well i mean you know how we all are once this happens you google it and it seems to be all kinds of bad things it could be it could be it could be a cold or flu obviously but tuberculosis it could be cancer always comes up so it will be good if none of those right so yeah i can provide a little bit of reassurance and we can talk about those a little bit as well and was there anything you were particularly expecting or hoping to get out of this consultation well yeah so reassurance so hopefully some sense that it is not anything too serious but also if there is anything you can prescribe me to make it better or any advice or maybe even a sick note so if i need to stay away from work for a bit longer i can get one sure sure okay all right so we will talk a little bit about the symptoms and i am sure we can get those things and some reassurance about your concerns so you mentioned that you started with a sore throat about a week ago developed into a bit of a dry cough i will just ask a few questions around those so do you have any shortness of breath yes yes i have been having shortness of breath yeah i have been having shortness of breath you are short of breath and do you have any wheeze or chest pain yeah a bit of four attacks you are feeling a bit wheezy with some chest pain as well yes okay and how when did you start to develop the shortness of breath i think so so the sore throat so today is friday the sore throat was about last week friday or thursday cough was satisfied so the shortness of breath was i think shortly after the cough so maybe a day or two later so three four days ago three or four days ago you started developing and is the cough worse at night time no it is the same throughout the week same throughout the day and when you say you are short of breath just need to try and get an idea about how short of breath you are so are you able to get walk up a flight of stairs for example or are you short of breath at rest oh yeah it is like when i am doing walking and i do exercise now and then so it has not been super bad like it has not stopped me from doing any of those things but it is been pretty unusual and a little bit worried and you are a bit concerned about that okay so i just need to ask a few things about your background as well so do you have any other medical conditions or medical history no just no no past medical history now no past microgravity no history of asthma no and any history of clots on your legs or your lungs so these are dvds or ps none in your familys had those clots in the legs or lungs well my mother had lung cancer your mother had lung cancer do you smoke no have you ever smoked or been exposed to asbestos you know do not know if asbestos ever smoked i mean once or twice in amsterdam but not really okay and this just going back to your symptoms of shortness of breath with the cough it is a dry cough no you are not coughing up anyphlem do you have and you say you do not have any chest pain as such are you taking any medications currently at the moment no no okay are you allergic to any medications not to any medication but i am allergic to peanuts peanuts okay and you mentioned that your mother had lung cancer any other family history of any significant illnesses when running in your family no no that is the only one just lung cancer from my mother just lung cancer okay and you say you have a cold so do you have sinus congestion or no it seems to be all entirely with just my throat like my nose is tiny now just your throat and any recent travel or have you always lived in the uk no so i have not always lived in the uk so i was born in the us and moved over twelve years ago but in terms of recent travel just to europe to exotic okay so no recent travel no significant recent travel anywhere okay and are you coughing up anything other than so you are not coughing up blood or anything like that no good and are you feeling feverish hot cold sweaty yeah so a little bit feverish at first so the first three or so days of this but then the fevers gone away okay and in general do you feel yeah i was just going to say also had a bit of a headache like headaches that come and go rather but like right now it is fine okay and in general would you say you are feeling you are beginning to feel better worse or sort of staying the same so it is like it is up and down so let us see so i started last week and i stayed home from work two days this week i think it was maybe tuesday and then thursday so like i felt better and then worse again and then better and then worse again so it is been a kind of constant but constant in being variable if that make me okay and i just need to ask any other sort of risk factors that you may have so no sort of significant weight loss or unexplained weight loss any waters so no weight loss but i have been have been losing my appetite recently and i mean i usually eat a lot so i enjoy eating as well but like that is been a bit concerning you have been losing your appetite recently yes and you are a little bit concerned about that but you have not you have not lost any weight that you think of no not that and any sort of rashes or anything no rash okay so i would ask to examine you now but i do not know if i could sort of look inside your throat at least to see if there is a probably we can try oh no well no it is okay i might think about doing that have you got any lumps or bumps around your neck that you can feel no no okay and so finally you were talking about i mean it sounds to me that you have been a little bit up and down sore throat developed a dry cough you are slightly short of breath but not too overly concerningly short of breath what i would say we are just coming to the end of the consultation now is if you feel significantly worse if you get more short of breath or sudden change in your breathlessness or breathlessness that you are concerned about and i would advise you to seek medical tension games here gp and actually see somebody physically but i think for now i can sort of try and reassure you that if this clears up as i expect it would so expect this to sort of be getting better in the next four or five days if it is not please get in touch with the medical professional again and i would expect it too and so therefore i would not be concerned about tuberculosis your concerns about lung cancer are was that the other thing you concerned about yeah oh yeah yeah so so again if you are not getting better please see somebody again i have just got four seconds now so nice talking to you and we have got to tidy up yeah okay so and i will provide you with a sick note just to give you a few more days off work and paracetamol lots of fluids and rest up and as i say if you are not feeling better please get in touch okay all right thanks a lot have a good day thank you</t>
+        </is>
       </c>
       <c r="M2" t="n">
-        <v>240</v>
+        <v>0.1577739529546758</v>
       </c>
       <c r="N2" t="n">
-        <v>102</v>
+        <v>37</v>
       </c>
       <c r="O2" t="n">
-        <v>0.1848184818481848</v>
+        <v>167</v>
       </c>
       <c r="P2" t="n">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="Q2" t="n">
-        <v>209</v>
+        <v>0.146873207114171</v>
       </c>
       <c r="R2" t="n">
-        <v>90</v>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>['ohh', 'um', 'uh', 'ninth', 'yeah', 'yeah', 'i', 'am', 'what', 'what', 'came', 'yes', 'uh', 'ok', 'uh', 'are', 'you', 'coughing', 'up', 'anything', 'no', 'its', 'very', 'dry', 'ok', 'so', 'am', 'i', 'am', 'the', 'uh', 'um', 'um', 'ok', 'you', 'it', 'could', 'be', 'could', 'be', 'also', 'be', 'could', 'be', 'none', 'of', 'um', 'uh', 'um', 'ok', 'uh', 'uh', 'uh', 'like', 'that', 'a', 'um', 'ok', 'um', 'um', 'no', 'have', 'been', 'yeah', 'uh', 'uh', 'a', 'bit', 'of', 'both', 'you', 'are', 'how', 'ah', 'week', 'so', 'the', 'whole', 'same', 'throughout', 'the', 'day', 'um', 'uh', 'so', 'um', 'so', 'uh', 'flight', 'um', 'or', 'of', 'its', 'so', 'um', 'it', 'uh', 'um', 'past', 'medical', 'history', 'no', 'no', 'um', 'uh', 'uh', 'uh', 'you', 'know', 'of', 'counts', 'um', 'uh', 'so', 'the', 'no', 'you', 'are', 'any', 'um', 'do', 'uh', 'do', 'not', 'you', 'um', 'uh', 'um', 'uh', 'uh', 'um', 'run', 'your', 'lung', 'cancer', 'ok', 'um', 'so', 'your', 'uh', 'i', 'moved', 'over', 'well', 'it', 'was', 'of', 'any', 'uh', 'you', 'no', 'no', 'yeah', 'uh', 'um', 'it', 'but', 'like', 'uh', 'feeling', 'you', 'are', 'you', 'are', 'to', 'or', 'um', 'so', 'it', 'yeah', 'that', 'makes', 'ok', 'have', 'been', 'and', 'and', 'i', 'like', 'so', 'of', 'yes', 'or', 'that', 'not', 'that', 'you', 'can', 'think', 'of', 'ok', 'to', 'there', 'is', 'ohh', 'a', 'uh', 'you', 'you', 'uh', 'mean', 'um', 'um', 'mmhmm', 'um', 'uh', 'um', 'no', 'go', 'and', 'see', 'um', 'um', 'uh', 'uh', 'um', 'i', 'um', 'um', 'uh', 'um', 'and', 'yeah', 'yeah', 'so', 'um', 'um', 'have', 'to', 'we', 'uh', 'all', 'right', 'uh', 'um', 'um', 'uh', 'good', 'day', 'bye']</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>['sorry', 'i', 'i', 'call', 'that', 'then', 'little', 'is', 'some', 'thank', 'a', 'a', 'those', 'let', 'us', 'today', 'or', 'super', 'these', 'are', 'have', 'no', 'all', 'feel', 'better', 'i', 'no', 'the', 'is', 'okay']</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>['ok', 'uh', 'my', 'names', 'uh', 'ok', 'and', 'are', 'ohh', 'happy', 'how', 'is', 'ok', 'ok', 'going', 'ask', 'so', 'there', 'but', 'it', 'could', 'it', 'great', 'so', 'so', 'anything', 'were', 'is', 'ok', 'uh', 'um', 'um', 'ill', 'i', 'shortness', 'of', 'ok', 'the', 'so', 'todays', 'develop', 'nighttime', 'no', 'a', 'at', 'ohh', 'exercises', 'superbad', 'worrying', 'ok', 'so', 'these', 'uh', 'that', 'with', 'if', 'that', 'ok', 'coughing', 'up', 'uh', 'no', 'no', 'ok', 'ok', 'uh', 'in', 'just', 'like', 'so', 'just', 'in', 'terms', 'too', 'ok', 'ok', 'and', 'if', 'you', 'have', 'not', 'not', 'not', 'ohh', 'ok', 'can', 'no', 'that', 'ok', 'um', 'then', 'somebody', 'a', 'are', 'ohh', 'got', 'ok', 'off', 'paracetemol', 'ok', 'have', 'a']</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>['um', 'ninth', 'yeah', 'yeah', 'i', 'am', 'is', 'ok', 'what', 'yes', 'uh', 'ok', 'uh', 'i', 'am', 'uh', 'um', 'um', 'what', 'might', 'be', 'going', 'on', 'you', 'said', 'that', 'you', 'had', 'a', 'cold', 'ok', 'well', 'i', 'mean', 'you', 'you', 'know', 'how', 'we', 'all', 'are', 'once', 'this', 'happens', 'you', 'google', 'it', 'and', 'there', 'seems', 'to', 'be', 'all', 'kinds', 'of', 'bad', 'things', 'it', 'could', 'be', 'it', 'could', 'be', 'could', 'be', 'a', 'cold', 'or', 'flu', 'obviously', 'but', 'it', 'could', 'also', 'be', 'tuberculosis', 'it', 'could', 'be', 'cancer', 'always', 'comes', 'up', 'it', 'will', 'be', 'good', 'if', 'none', 'of', 'those', 'great', 'so', 'and', 'um', 'ok', 'uh', 'uh', 'uh', 'um', 'ok', 'no', 'uh', 'a', 'bit', 'of', 'both', 'you', 'are', 'ah', 'so', 'last', 'week', 'so', 'the', 'whole', 'um', 'uh', 'so', 'um', 'so', 'uh', 'um', 'or', 'its', 'so', 'um', 'uh', 'um', 'no', 'um', 'uh', 'uh', 'uh', 'the', 'that', 'of', 'uh', 'do', 'not', 'you', 'uh', 'to', 'uh', 'uh', 'run', 'with', 'so', 'nose', 'is', 'like', 'so', 'i', 'it', 'was', 'any', 'uh', 'you', 'no', 'uh', 'uh', 'it', 'yeah', 'but', 'ok', 'um', 'it', 'makes', 'ok', 'and', 'and', 'i', 'so', 'of', 'yes', 'or', 'that', 'not', 'that', 'ok', 'you', 'uh', 'mmhmm', 'go', 'and', 'see', 'a', 'um', 'uh', 'i', 'um', 'um', 'i', 'would', 'um', 'are', 'and', 'ohh', 'yeah', 'yeah', 'um', 'we', 'uh', 'all', 'right', 'uh', 'um', 'um', 'uh']</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>['name', 'sorry', 'discuss', 'yeah', 'i', 'i', 'call', 'up', 'then', 'little', 'in', 'thank', 'a', 'a', 'oh', 'today', 'or', 'start', 'symptoms', 'night', 'super', 'are', 'ddps', 'or', 'you', 'no', 'almost', 'you', 'you', 'you', 'really', 'it', 'on', 'hours', 'we', 'have', 'okay']</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>['ok', 'ohh', 'uh', 'names', 'uh', 'uh', 'ok', 'uh', 'ohh', 'just', 'how', 'bad', 'ok', 'ok', 'so', 'ideas', 'its', 'ok', 'uh', 'um', 'um', 'ok', 'todays', 'three', 'started', 'nighttime', 'ohh', 'exercises', 'superbad', 'ok', 'uh', 'no', 'one', 'in', 'familys', 'on', 'with', 'if', 'counts', 'ok', 'uh', 'flem', 'uh', 'no', 'no', 'ok', 'ok', 'um', 'um', 'uh', 'ok', 'my', 'uk', 'uk', 'us', 'well', 'too', 'ok', 'ok', 'ok', 'uh', 'and', 'if', 'that', 'not', 'not', 'think', 'of', 'ohh', 'ohh', 'ok', 'a', 'uh', 'no', 'that', 'ok', 'um', 'um', 'of', 'now', 'then', 'no', 'expect', 'a', 'uh', 'are', 'ok', 'paracetemol', 'ok', 'bye']</t>
-        </is>
+        <v>48</v>
+      </c>
+      <c r="S2" t="n">
+        <v>160</v>
+      </c>
+      <c r="T2" t="n">
+        <v>48</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.1113023522662077</v>
+      </c>
+      <c r="V2" t="n">
+        <v>33</v>
+      </c>
+      <c r="W2" t="n">
+        <v>113</v>
+      </c>
+      <c r="X2" t="n">
+        <v>48</v>
       </c>
       <c r="Y2" t="inlineStr">
+        <is>
+          <t>['oh', 'yeah', 'yeah', 'i', 'am', 'what', 'what', 'came', 'yes', 'okay', 'are', 'you', 'coughing', 'up', 'anything', 'no', 'it', 'is', 'very', 'dry', 'okay', 'so', 'am', 'i', 'am', 'the', 'okay', 'you', 'it', 'could', 'be', 'could', 'be', 'also', 'be', 'could', 'be', 'none', 'of', 'okay', 'like', 'that', 'a', 'okay', 'will', 'no', 'been', 'yeah', 'a', 'bit', 'of', 'both', 'you', 'are', 'how', 'week', 'so', 'the', 'whole', 'same', 'throughout', 'the', 'day', 'so', 'so', 'flight', 'or', 'of', 'it', 'is', 'so', 'it', 'past', 'medical', 'history', 'no', 'no', 'you', 'know', 'of', 'counts', 'so', 'the', 'no', 'you', 'are', 'any', 'do', 'do', 'not', 'you', 'your', 'just', 'lung', 'cancer', 'so', 'your', 'i', 'moved', 'over', 'well', 'it', 'was', 'any', 'you', 'no', 'no', 'yeah', 'it', 'but', 'like', 'feeling', 'you', 'are', 'you', 'are', 'to', 'or', 'so', 'it', 'yeah', 'if', 'that', 'makes', 'have', 'been', 'and', 'and', 'i', 'like', 'so', 'of', 'yes', 'or', 'not', 'that', 'not', 'that', 'you', 'can', 'think', 'of', 'to', 'there', 'is', 'oh', 'a', 'you', 'you', 'mean', 'no', 'go', 'and', 'see', 'i', 'and', 'yeah', 'yeah', 'so', 'have', 'to', 'we', 'all', 'right', 'good', 'day', 'bye']</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>['name', 'sorry', 'i', 'i', 'call', 'that', 'then', 'little', 'is', 'some', 'secrets', 'thank', 'you', 'a', 'a', 'and', 'those', 'let', 'us', 'today', 'or', 'super', 'these', 'are', 'ddts', 'have', 'i', 'am', 'all', 'feel', 'better', 'i', 'no', 'and', 'the', 'is', 'okay']</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>['names', 'ninth', 'and', 'are', 'happy', 'how', 'is', 'going', 'ask', 'so', 'there', 'but', 'it', 'could', 'it', 'great', 'so', 'so', 'anything', 'were', 'is', 'i', 'have', 'shortness', 'of', 'the', 'so', 'todays', 'develop', 'nighttime', 'no', 'a', 'at', 'exercises', 'superbad', 'worrying', 'so', 'these', 'that', 'with', 'if', 'that', 'coughing', 'up', 'no', 'run', 'in', 'like', 'so', 'just', 'in', 'terms', 'of', 'too', 'and', 'you', 'have', 'not', 'not', 'can', 'no', 'that', 'then', 'somebody', 'a', 'are', 'got', 'off', 'paracetemol', 'have', 'a']</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>['yeah', 'yeah', 'i', 'am', 'bad', 'is', 'what', 'yes', 'okay', 'i', 'am', 'what', 'might', 'be', 'going', 'on', 'you', 'said', 'that', 'you', 'had', 'a', 'cold', 'okay', 'well', 'i', 'mean', 'you', 'you', 'know', 'how', 'we', 'all', 'are', 'once', 'this', 'happens', 'you', 'google', 'it', 'and', 'there', 'seems', 'to', 'be', 'all', 'kinds', 'of', 'bad', 'things', 'it', 'could', 'be', 'it', 'could', 'be', 'could', 'be', 'a', 'cold', 'or', 'flu', 'obviously', 'but', 'it', 'could', 'also', 'be', 'tuberculosis', 'it', 'could', 'be', 'cancer', 'always', 'comes', 'up', 'it', 'will', 'be', 'good', 'if', 'none', 'of', 'those', 'great', 'so', 'and', 'okay', 'it', 'okay', 'no', 'a', 'bit', 'of', 'both', 'you', 'are', 'so', 'last', 'week', 'so', 'the', 'whole', 'so', 'so', 'or', 'it', 'is', 'so', 'no', 'the', 'that', 'of', 'do', 'not', 'you', 'to', 'with', 'so', 'nose', 'is', 'like', 'so', 'i', 'it', 'was', 'any', 'you', 'no', 'it', 'yeah', 'but', 'it', 'that', 'makes', 'and', 'and', 'i', 'so', 'of', 'yes', 'or', 'that', 'not', 'that', 'of', 'you', 'go', 'and', 'see', 'a', 'i', 'are', 'and', 'oh', 'yeah', 'yeah', 'we', 'all', 'right']</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>['hey', 'name', 'sorry', 'be', 'discuss', 'yeah', 'i', 'i', 'call', 'up', 'then', 'little', 'in', 'sorted', 'thank', 'you', 'a', 'a', 'and', 'oh', 'today', 'or', 'start', 'symptoms', 'night', 'super', 'are', 'ddps', 'or', 'ps', 'you', 'i', 'am', 'and', 'and', 'almost', 'you', 'you', 'you', 'really', 'it', 'on', 'and', 'and', 'hours', 'we', 'have', 'alright']</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>['oh', 'names', 'ninth', 'just', 'how', 'so', 'ideas', 'todays', 'three', 'started', 'nighttime', 'exercises', 'superbad', 'no', 'one', 'in', 'familys', 'on', 'with', 'if', 'counts', 'flem', 'no', 'run', 'my', 'uk', 'uk', 'us', 'well', 'too', 'and', 'if', 'not', 'not', 'think', 'a', 'no', 'that', 'of', 'now', 'then', 'no', 'expect', 'a', 'would', 'are', 'paracetemol', 'bye']</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>['a', 'yeah', 'yeah', 'i', 'am', 'is', 'what', 'what', 'came', 'yes', 'i', 'am', 'the', 'okay', 'you', 'it', 'could', 'also', 'be', 'so', 'okay', 'like', 'that', 'a', 'okay', 'no', 'yeah', 'are', 'or', 'sunday', 'so', 'the', 'day', 'so', 'like', 'or', 'it', 'is', 'so', 'it', 'the', 'that', 'of', 'if', 'that', 'counts', 'so', 'the', 'flem', 'do', 'do', 'not', 'you', 'so', 'just', 'your', 'i', 'i', 'like', 'well', 'it', 'was', 'too', 'so', 'no', 'any', 'you', 'no', 'it', 'yeah', 'but', 'you', 'are', 'to', 'or', 'so', 'it', 'yeah', 'and', 'and', 'i', 'so', 'yes', 'or', 'and', 'you', 'not', 'that', 'not', 'that', 'you', 'can', 'think', 'of', 'i', 'there', 'is', 'oh', 'that', 'you', 'no', 'you', 'a', 'i', 'and', 'are', 'oh', 'have', 'to', 'we', 'all', 'right', 'bye']</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>['hey', 'i', 'call', 'up', 'then', 'it', 'little', 'is', 'a', 'a', 'breath', 'i', 'think', 'today', 'the', 'super', 'it', 'now', 'past', 'are', 'dvds', 'or', 'have', 'all', 'make', 'waters', 'the', 'is', 'all', 'right', 'thanks', 'a', 'lot']</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>['oh', 'ninth', 'happy', 'how', 'bad', 'so', 'we', 'there', 'great', 'is', 'both', 'you', 'todays', 'saturday', 'develop', 'nighttime', 'no', 'whole', 'so', 'exercises', 'superbad', 'worrying', 'no', 'no', 'one', 'on', 'with', 'any', 'run', 'like', 'so', 'nowhere', 'sorry', 'and', 'makes', 'not', 'a', 'then', 'see', 'no', 'go', 'and', 'see', 'a', 'to', 'yeah', 'got', 'paracetemol']</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
         <is>
           <t xml:space="preserve">      ref_ix  hyp_ix reference hypothesis operation  index_edit_ops
 0          0       0     hello      hello         =            &lt;NA&gt;
@@ -687,15 +779,15 @@
 3          3       3      hear       hear         =            &lt;NA&gt;
 4          4       4        me         me         =            &lt;NA&gt;
 ...      ...     ...       ...        ...       ...             ...
-1843    1813    &lt;NA&gt;      good          _       del             369
-1844    1814    &lt;NA&gt;       day          _       del             370
-1845    1815    1606     thank      thank         =            &lt;NA&gt;
-1846    1816    1607       you        you         =            &lt;NA&gt;
-1847    1817    &lt;NA&gt;       bye          _       del             371
-[1848 rows x 6 columns]</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
+1775    1738    &lt;NA&gt;      good          _       del             272
+1776    1739    &lt;NA&gt;       day          _       del             273
+1777    1740    1611     thank      thank         =            &lt;NA&gt;
+1778    1741    1612       you        you         =            &lt;NA&gt;
+1779    1742    &lt;NA&gt;       bye          _       del             274
+[1780 rows x 6 columns]</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
         <is>
           <t xml:space="preserve">      ref_ix  hyp_ix reference hypothesis operation  index_edit_ops
 0          0       0     hello      hello         =            &lt;NA&gt;
@@ -704,22 +796,44 @@
 3          3       3      hear       hear         =            &lt;NA&gt;
 4          4       4        me         me         =            &lt;NA&gt;
 ...      ...     ...       ...        ...       ...             ...
-1850    1813    1641      good       good         =            &lt;NA&gt;
-1851    1814    1642       day        day         =            &lt;NA&gt;
-1852    1815    1643     thank      thank         =            &lt;NA&gt;
-1853    1816    1644       you        you         =            &lt;NA&gt;
-1854    1817    1645       bye    alright       sub             335
-[1855 rows x 6 columns]</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>hello can you hear me [SUB:ok-&gt;okay] [DEL:ohh] yes i can can you hear me yeah good good so my name is joe i am a doctor [DEL:um] here at babylon can i just confirm your name please [SUB:uh-&gt;my] [SUB:my-&gt;name] [SUB:names-&gt;is] vincent and your date of birth [SUB:uh-&gt;nineth] [DEL:uh] [DEL:ninth] of may two thousand and sixteen [SUB:ok-&gt;okay] great [INS:sorry] [SUB:and-&gt;i] [SUB:are-&gt;know] you in a uh a safe place [SUB:ohh-&gt;oh] sorry a safe and confidential place to talk and just [INS:i] [SUB:happy-&gt;have] to go ahead with the consultation [DEL:yeah] [DEL:yeah] [DEL:i] [DEL:am] yes yes i am great so how can i help yeah so [INS:i] have a [INS:call] [INS:that] i have been having a cough and a sore throat for about a week and its been causing me problems i have had to stay away from work for about three or four of those days because of [SUB:how-&gt;a] bad [SUB:is-&gt;history] [SUB:ok-&gt;okay] i am sorry to hear that so you have had a cough and a sore throat for about a week and what came [DEL:what] [DEL:what] [DEL:came] first [DEL:yes] [DEL:uh] the sore throat came first and then after a day or two the cough [SUB:ok-&gt;okay] [DEL:ok] and [DEL:uh] [DEL:are] [DEL:you] [DEL:coughing] [DEL:up] [DEL:anything] [DEL:no] [DEL:its] [DEL:very] [DEL:dry] [DEL:ok] [DEL:so] i [DEL:am] [DEL:i] [DEL:am] just [SUB:going-&gt;want] to [SUB:ask-&gt;thank] a few questions about [DEL:the] [DEL:uh] your current symptoms and [INS:then] a little bit about your background [DEL:um] and something else about what we can do a little bit later on in the consultation to help you [SUB:so-&gt;but] before we go on anything you are particularly concerned about [DEL:um] or have any ideas what might be going on you said that you had a cold [DEL:ok] well i mean you [DEL:you] know how we all are once this happens you google it and [SUB:there-&gt;it] seems to be all kinds of bad things it could be [DEL:it] [DEL:could] [DEL:be] [DEL:could] [DEL:be] a cold or flu obviously [SUB:but-&gt;obviously] [SUB:it-&gt;because] [SUB:could-&gt;we] [DEL:also] [DEL:be] tuberculosis [SUB:it-&gt;the] [DEL:could] [DEL:be] cancer always comes up so it will be good if [DEL:none] [DEL:of] those [SUB:great-&gt;right] [SUB:so-&gt;say] [SUB:so-&gt;say] yeah i can provide a [INS:little] bit of reassurance [DEL:um] and [DEL:uh] we can talk about those a little bit as well and was there [SUB:anything-&gt;any] you [SUB:were-&gt;are] particularly expecting or hoping to get out of this consultation [DEL:um] [DEL:ok] [DEL:uh] [DEL:uh] well [DEL:uh] yeah so reassurance so [DEL:like] hopefully some sense that its not anything too serious but also [SUB:is-&gt;if] there [INS:is] anything you can prescribe me to make it better or any advice or maybe even a sick note so [DEL:that] if i need to stay away from work for a bit longer i can get one sure sure [SUB:ok-&gt;okay] all right so well talk a little bit about the symptoms and i am sure we can get [DEL:a] [DEL:um] those things [INS:some] [SUB:uh-&gt;secrets] and some reassurance [INS:thank] [SUB:um-&gt;you] about your concerns [DEL:ok] so [DEL:um] you mentioned that you started with [INS:a] sore throat about a week ago developed into [INS:a] bit of a dry cough [SUB:um-&gt;and] [SUB:ill-&gt;i] just ask a few questions around those [INS:those] so [DEL:um] do you have any shortness of breath [DEL:no] yes yes [SUB:i-&gt;were] [DEL:have] [DEL:been] having [SUB:shortness-&gt;shorts] [SUB:of-&gt;oh] yeah i have been having shortness of breath [DEL:yeah] you are short of breath and [DEL:uh] do you have any wheeze or chest pain [DEL:uh] yeah [DEL:a] [DEL:bit] [DEL:of] [DEL:both] you are [DEL:you] [DEL:are] feeling a bit wheezy with some chest pain as well yes [SUB:ok-&gt;okay] and [DEL:how] [DEL:ah] when did you start to develop [SUB:the-&gt;a] shortness of breath [INS:let] [INS:us] [SUB:so-&gt;see] so the sore throat so [INS:today] [SUB:todays-&gt;is] friday sore throat was about last [DEL:week] friday or thursday cough was saturday or sunday so the [DEL:so] [DEL:the] shortness of breath was i think shortly after the cough so maybe a day or two later so three [INS:or] four days ago three or four days ago you started [SUB:develop-&gt;developing] and is the cough worse at [SUB:nighttime-&gt;night] [SUB:no-&gt;time] no its the same throughout the [DEL:whole] day [DEL:same] [DEL:throughout] [DEL:the] [DEL:day] [DEL:um] and [DEL:uh] when you say you are short of breath just need to try and get an idea about how short of breath you are so are you able to [DEL:so] [DEL:um] [DEL:so] [DEL:uh] like walk up [SUB:a-&gt;flights] [DEL:flight] of stairs for example [DEL:um] or [DEL:or] are you short [DEL:of] breath [SUB:at-&gt;of] rest [SUB:ohh-&gt;oh] yeah its [DEL:its] like [DEL:so] when i am doing walking [DEL:um] and i do [SUB:exercises-&gt;exercise] now and then so it [DEL:it] has not been [INS:super] [SUB:superbad-&gt;bad] like has not stopped me from doing any of those things but its been pretty unusual and a little bit [SUB:worrying-&gt;worried] and you are a bit concerned about that [SUB:ok-&gt;okay] so i just need to ask a few [DEL:uh] things about your background as well so [DEL:um] do you have any other medical conditions or medical history no just no no [DEL:past] [DEL:medical] [DEL:history] no [DEL:no] [DEL:no] history of asthma no [DEL:um] and any [DEL:uh] [DEL:uh] history of [DEL:uh] clots on your legs or your lungs [INS:these] [INS:are] [SUB:so-&gt;ddts] [SUB:these-&gt;or] [SUB:uh-&gt;ps] no one in your familys had those clots on the legs or the lungs well my mother had lung cancer your mother had lung cancer do you smoke no [INS:have] you ever smoked or been exposed to asbestos [SUB:that-&gt;i] [DEL:you] [DEL:know] [DEL:of] do not know [SUB:with-&gt;if] asbestos ever smoked i mean once or twice in amsterdam [SUB:if-&gt;in] [SUB:that-&gt;dakar] [DEL:counts] but not really [SUB:ok-&gt;okay] [DEL:um] and [DEL:uh] this [DEL:so] just going back to [DEL:the] your symptoms of shortness of breath with the cough its a dry cough [DEL:no] [DEL:you] [DEL:are] not [SUB:coughing-&gt;cough] [SUB:up-&gt;cap] [DEL:any] flem [DEL:um] do [DEL:do] you have [DEL:uh] and you [DEL:do] [DEL:not] [DEL:you] say you do not have any chest pain as such [DEL:um] [DEL:uh] are you taking any medications currently at the moment [INS:no] [SUB:uh-&gt;i] [SUB:no-&gt;am] [SUB:no-&gt;not] [SUB:ok-&gt;okay] are you allergic to any medications not to any medication but i am allergic to peanuts peanuts [SUB:ok-&gt;okay] [DEL:um] and [DEL:uh] you mentioned that your mother had [DEL:uh] lung cancer [DEL:um] any other family history of any significant illnesses [SUB:uh-&gt;when] [DEL:run] running [SUB:in-&gt;into] [DEL:your] family no no that is the only one just lung cancer from my mother [SUB:just-&gt;okay] [DEL:lung] [DEL:cancer] [DEL:ok] and you say you have a cold so do you have sinus congestion or [DEL:um] no it seems to be [INS:all] entirely with just my throat [DEL:so] like my nose is [SUB:like-&gt;just] [SUB:so-&gt;running] [SUB:just-&gt;out] [DEL:your] just your throat and any recent travel or have you always lived in the uk [DEL:uh] no so i i [DEL:i] have not always lived in the uk like so i was born in the us and [DEL:moved] [DEL:over] [DEL:well] [DEL:it] [DEL:was] twelve years ago but [SUB:in-&gt;its] [SUB:terms-&gt;a] [DEL:of] recent travel just to europe nowhere [SUB:too-&gt;to] exotic [SUB:ok-&gt;okay] so no so no recent travel no significant recent travel [DEL:any] anywhere um [SUB:ok-&gt;okay] and are you coughing up anything other than um [DEL:uh] so you [DEL:you] are not coughing up blood or anything like that [DEL:no] [DEL:no] um good and uh are you feeling feverish hot cold sweaty [DEL:yeah] so a little bit feverish [DEL:uh] [DEL:um] at first so the first three or so days of this but then [DEL:it] the fevers gone away ok and in general do you [INS:feel] [INS:better] sorry yeah yeah i was just going to say [INS:i] also had a bit of a headache [DEL:but] like headaches that come and go rather but [DEL:like] right now its fine [DEL:uh] ok and in general would you say you are [DEL:feeling] [DEL:you] [DEL:are] [DEL:you] [DEL:are] beginning to [DEL:to] feel better worse or [DEL:or] sort of [DEL:um] staying the same so its like its up and down so [DEL:so] let us see so i [DEL:it] started last week and i stayed home from work two days this week i think it was maybe tuesday and then thursday so like i felt better and then worse again and then better and then worse again so its been [DEL:yeah] a kind of constant but constant [SUB:and-&gt;in] being variable [SUB:if-&gt;okay] [DEL:that] [DEL:makes] [DEL:ok] and i just need to ask any other sort of risk factors um that you may have so um no sort of significant weight loss um or unexplained weight loss any so no [INS:no] weight loss but i have been [DEL:have] [DEL:been] losing my appetite recently and i mean i usually eat a lot so [DEL:and] i [DEL:and] [DEL:i] enjoy eating as well but [DEL:like] [DEL:so] that is been a bit concerning you have been losing your appetite recently yes and you are a little bit concerned about that but you have not [SUB:you-&gt;lost] [SUB:have-&gt;any] [SUB:not-&gt;weight] lost any weight that you think [DEL:of] [DEL:yes] no not that and any um sort of rashes or anything [DEL:or] uh and you no [SUB:not-&gt;no] [SUB:not-&gt;okay] [DEL:that] [DEL:not] [DEL:that] [DEL:you] [DEL:can] [DEL:think] [DEL:of] [DEL:ok] um so i would ask to examine you now but um i i do not know if i could sort of look inside your throat at least [DEL:to] see if there is a probably [DEL:there] [DEL:is] [DEL:ohh] we can try [SUB:ohh-&gt;oh] no well no its [SUB:ok-&gt;okay] i might think about doing [DEL:a] have you got any lumps or bumps around your neck that you [SUB:can-&gt;could] feel [DEL:uh] no [SUB:no-&gt;not] [SUB:that-&gt;the] [DEL:you] no [SUB:ok-&gt;okay] [SUB:um-&gt;and] and so finally you [DEL:you] were talking about [DEL:uh] i [DEL:mean] it sounds to me that [DEL:um] you have been a little bit up and down sore throat developed a dry cough [DEL:um] you are slightly short of breath but not too overly concerningly short of breath what i would say were just coming to the end of [INS:the] consultation now [INS:is] if you feel significantly worse [DEL:mmhmm] [DEL:um] [DEL:uh] if you get more short of breath or sudden change in your breathlessness [DEL:um] or breathlessness that you are concerned about [SUB:then-&gt;and] i would advise you to see [DEL:no] [DEL:go] [DEL:and] [DEL:see] a gp [DEL:um] and actually see [SUB:somebody-&gt;something] physically [DEL:um] [DEL:uh] but i think for now i can sort of [DEL:uh] try and reassure you that [DEL:um] if this clears up as i expect it would so [DEL:i] expect this to sort of be getting better in the next four or five days [DEL:um] if its not please get in touch with [SUB:a-&gt;the] medical professional again [DEL:um] and [DEL:uh] i would expect it to and so therefore i would not be concerned about tuberculosis [DEL:um] your concerns about lung cancer are [DEL:and] was that the other thing you [SUB:are-&gt;were] concerned about [SUB:ohh-&gt;oh] yeah yeah [DEL:yeah] [DEL:yeah] so [DEL:so] [DEL:um] again if you are not getting better please see somebody again [DEL:um] i have just got four seconds now so nice talking to you and [DEL:have] we [SUB:got-&gt;have] [DEL:to] [DEL:we] got to tidy up yeah [INS:okay] [SUB:ok-&gt;okay] so [DEL:uh] [DEL:all] [DEL:right] [DEL:uh] and ill provide you with a sick note just to give you a few more days [SUB:off-&gt;of] work [DEL:um] and [SUB:paracetemol-&gt;paracetamol] lots of fluids [DEL:um] and [DEL:uh] rest up and as i say if you are not feeling better please get in touch [SUB:ok-&gt;okay] [SUB:have-&gt;all] [SUB:a-&gt;right] [DEL:good] [DEL:day] thank you [DEL:bye]</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>hello can you hear me [SUB:ok-&gt;okay] [SUB:ohh-&gt;hey] yes i can can you hear me yeah good good so my name is joe i am a doctor [DEL:um] here at babylon can i just confirm your name please [SUB:uh-&gt;hey] my [INS:name] [SUB:names-&gt;is] vincent and your date of birth [SUB:uh-&gt;ah] [SUB:uh-&gt;nine] [DEL:ninth] of may two thousand and sixteen [SUB:ok-&gt;okay] great [INS:sorry] and are you in a [SUB:uh-&gt;be] a safe place [SUB:ohh-&gt;oh] sorry a safe and confidential place to talk and [INS:discuss] [INS:yeah] [INS:i] [SUB:just-&gt;am] happy to go ahead with the consultation [DEL:yeah] [DEL:yeah] [DEL:i] [DEL:am] yes yes i am great so how can i help yeah so [INS:i] have a [INS:call] [INS:up] i have been having a cough and a sore throat for about a week and its been causing me problems i have had to stay away from work for about three or four of those days because of [SUB:how-&gt;it] [SUB:bad-&gt;okay] [DEL:is] [DEL:ok] i am sorry to hear that so you have had a cough and a sore throat for about a week and what came what [DEL:what] came first [DEL:yes] [DEL:uh] the sore throat came first and then after a day or two the cough [SUB:ok-&gt;okay] [DEL:ok] and [DEL:uh] are you coughing up anything no its very dry [SUB:ok-&gt;okay] so i am [DEL:i] [DEL:am] just going to ask a few questions about the [DEL:uh] your current symptoms and [INS:then] a little bit about your background [DEL:um] and something else about what we can do a little bit later on in the consultation to help you [SUB:so-&gt;but] before we go on anything you are particularly concerned about [DEL:um] or have any [SUB:ideas-&gt;right] [DEL:what] [DEL:might] [DEL:be] [DEL:going] [DEL:on] [DEL:you] [DEL:said] [DEL:that] [DEL:you] [DEL:had] [DEL:a] [DEL:cold] [DEL:ok] [DEL:well] [DEL:i] [DEL:mean] [DEL:you] [DEL:you] [DEL:know] [DEL:how] [DEL:we] [DEL:all] [DEL:are] [DEL:once] [DEL:this] [DEL:happens] [DEL:you] [DEL:google] [DEL:it] [DEL:and] [DEL:there] [DEL:seems] [DEL:to] [DEL:be] [DEL:all] [DEL:kinds] [DEL:of] [DEL:bad] [DEL:things] [DEL:it] [DEL:could] [DEL:be] [DEL:it] [DEL:could] [DEL:be] [DEL:could] [DEL:be] [DEL:a] [DEL:cold] [DEL:or] [DEL:flu] [DEL:obviously] [DEL:but] [DEL:it] [DEL:could] [DEL:also] [DEL:be] [DEL:tuberculosis] [DEL:it] [DEL:could] [DEL:be] [DEL:cancer] [DEL:always] [DEL:comes] [DEL:up] so [DEL:it] [DEL:will] [DEL:be] [DEL:good] [DEL:if] [DEL:none] [DEL:of] [DEL:those] [DEL:great] so [DEL:so] yeah i can provide a [INS:little] bit of reassurance um and uh we can talk about those a little bit as well [DEL:and] was there anything you were particularly expecting or hoping to get out of this consultation [DEL:um] [DEL:ok] [DEL:uh] [DEL:uh] well [DEL:uh] yeah so reassurance so like hopefully [INS:in] some sense that [SUB:its-&gt;is] not anything too serious but also is there anything you can prescribe me to make it better or any advice or maybe even a sick note so that if i need to stay away from work for a bit longer i can get one sure sure [SUB:ok-&gt;okay] all right so well talk a little bit about the symptoms and i am sure we can get a [DEL:um] those things [SUB:uh-&gt;sorted] and some reassurance [INS:thank] [SUB:um-&gt;you] about your concerns [DEL:ok] so um you mentioned that you started with [INS:a] sore throat about a week ago developed into [INS:a] bit of a dry cough [SUB:um-&gt;and] ill just ask a few questions around those so um do you have any shortness of breath [DEL:no] yes yes i have been having shortness of [INS:oh] yeah i have been having shortness of breath yeah you are short of breath and uh do you have any wheeze or chest pain [DEL:uh] yeah [DEL:a] [DEL:bit] [DEL:of] [DEL:both] you are [DEL:you] [DEL:are] feeling a bit wheezy with some chest pain as well yes [SUB:ok-&gt;okay] and how [DEL:ah] when did you start to develop the shortness of breath so [DEL:so] the sore throat so [INS:today] [SUB:todays-&gt;is] friday sore throat was about [DEL:last] [DEL:week] friday or thursday cough was saturday or sunday so the [DEL:so] [DEL:the] shortness of breath was i think shortly after the cough so maybe a day or two later so three [INS:or] four days ago [SUB:three-&gt;two] or four days ago you [INS:start] [SUB:started-&gt;to] develop [INS:symptoms] and is the cough worse at [INS:night] [SUB:nighttime-&gt;time] no no its the same throughout the [DEL:whole] day same throughout the day [DEL:um] and [DEL:uh] when you say you are short of breath just need to try and get an idea about how short of breath you are so are you able to [DEL:so] [DEL:um] [DEL:so] [DEL:uh] like walk up a flight of stairs for example [DEL:um] or [DEL:or] are you short of breath at rest [SUB:ohh-&gt;oh] yeah its [DEL:its] like [DEL:so] when i am doing walking [DEL:um] and i do [SUB:exercises-&gt;exercise] now and then so it it has not been [INS:super] [SUB:superbad-&gt;bad] like has not stopped me from doing any of those things but its been pretty unusual and a little bit worrying and you are a bit concerned about that [SUB:ok-&gt;okay] so i just need to ask a few [DEL:uh] things about your background as well so [DEL:um] do you have any other medical conditions or medical history no just no no past medical history no no [DEL:no] history of asthma no [DEL:um] and any [DEL:uh] [DEL:uh] history of [DEL:uh] clots on your legs or your lungs so these [INS:are] [INS:ddps] [INS:or] [SUB:uh-&gt;ps] [SUB:no-&gt;and] [SUB:one-&gt;none] [SUB:in-&gt;of] your [SUB:familys-&gt;families] had those clots [SUB:on-&gt;in] the legs or [DEL:the] lungs well my mother had lung cancer your mother had lung cancer do you smoke no you ever smoked or been exposed to asbestos [DEL:that] you know [DEL:of] do not know [SUB:with-&gt;if] asbestos ever smoked i mean once or twice in amsterdam [SUB:if-&gt;with] that [SUB:counts-&gt;car] but not really [SUB:ok-&gt;okay] um and [SUB:uh-&gt;ah] this so just going back to the your symptoms of shortness of breath with the cough its a dry cough no you are not coughing up any [SUB:flem-&gt;phlegm] um do [INS:you] do you have [DEL:uh] and you [DEL:do] [DEL:not] [DEL:you] say you do not have any chest pain as such um [DEL:uh] are you taking any medications currently at the moment [INS:no] [SUB:uh-&gt;i] [SUB:no-&gt;am] [SUB:no-&gt;not] [SUB:ok-&gt;okay] are you allergic to any medications not [DEL:to] any medication but i am allergic to peanuts peanuts [SUB:ok-&gt;okay] [SUB:um-&gt;and] and [DEL:uh] you mentioned that your mother had [DEL:uh] lung cancer [SUB:um-&gt;and] any other family history of any significant illnesses [SUB:uh-&gt;when] [DEL:run] running in your family no no that is the only one just lung cancer from my mother just lung cancer [SUB:ok-&gt;okay] and you say you have a cold so do you have sinus congestion or um no it seems to be [INS:almost] entirely [DEL:with] just my throat [DEL:so] like [SUB:my-&gt;j] [DEL:nose] [DEL:is] [DEL:like] [DEL:so] just your just your throat and any recent travel or have you always lived in the [INS:you] [SUB:uk-&gt;k] uh no so i i [DEL:i] have not always lived in the [INS:you] [SUB:uk-&gt;k] like so i was born in the [INS:you] [SUB:us-&gt;s] and moved over [SUB:well-&gt;about] [DEL:it] [DEL:was] twelve years ago but in terms of recent travel just to europe nowhere [SUB:too-&gt;to] exotic [SUB:ok-&gt;okay] so no so no recent travel no significant recent travel [DEL:any] anywhere um [SUB:ok-&gt;okay] and are you coughing up anything other than um [DEL:uh] so you [DEL:you] are not coughing up blood or anything like that no [DEL:no] um good and [DEL:uh] are you feeling feverish hot cold sweaty yeah so a little bit feverish [DEL:uh] um at first so the first three or so days of this but then [DEL:it] the fevers gone away [SUB:ok-&gt;okay] and in general do you sorry yeah [DEL:yeah] i was just going to say also had a bit of a headache [DEL:but] like headaches that come and go rather but like right now its fine [SUB:uh-&gt;okay] [DEL:ok] and in general would you say you are feeling you are you are beginning to to feel better worse or or sort of [DEL:um] staying the same so its like its up and down so so let us see so i [DEL:it] started last week and i stayed home from work two days this week i think it was maybe tuesday and then thursday so like i felt better and then worse again and then better and then worse again so its been yeah a kind of constant but constant [SUB:and-&gt;in] being variable [SUB:if-&gt;but] [SUB:that-&gt;okay] [DEL:makes] [DEL:ok] and i just [INS:really] need to ask any other sort of risk factors um that you may have so um no sort of significant weight loss um or unexplained weight loss any so no weight loss but i have been have been losing my appetite recently and i mean i usually eat a lot so [DEL:and] i [DEL:and] [DEL:i] enjoy eating as well but like [DEL:so] that is been a bit concerning you have been losing your appetite recently yes and you are a little bit concerned about that but you have not you have not lost any weight that you think [DEL:of] [DEL:yes] no not that and any um sort of rashes or anything [DEL:or] uh and you no [SUB:not-&gt;rash] [SUB:not-&gt;no] [DEL:that] [DEL:not] [DEL:that] you can [SUB:think-&gt;go] [SUB:of-&gt;okay] [DEL:ok] um so i would ask to examine you now but um i i do not know if i could sort of look inside your throat at least to see if there is a probably there is [SUB:ohh-&gt;oh] we can try [INS:it] [INS:on] [SUB:ohh-&gt;oh] no well no its [SUB:ok-&gt;okay] i might think about doing [SUB:a-&gt;it] have you got any lumps or bumps around your neck that you can feel [SUB:uh-&gt;ah] no [SUB:no-&gt;not] [SUB:that-&gt;the] [DEL:you] no [SUB:ok-&gt;okay] [SUB:um-&gt;and] and so finally you you were talking about [DEL:uh] i mean it sounds to me that um you have been a little bit up and down sore throat developed a dry cough [SUB:um-&gt;and] you are slightly short of breath but not too overly concerningly short of breath what i would say were just coming to the end [SUB:of-&gt;so] consultation [INS:hours] [SUB:now-&gt;is] if you feel significantly worse [DEL:mmhmm] um uh if you get more short of breath or sudden change in your breathlessness um or breathlessness that you are concerned about [SUB:then-&gt;and] i would advise you to see [SUB:no-&gt;your] [DEL:go] [DEL:and] [DEL:see] [DEL:a] gp [DEL:um] and actually see somebody physically um uh but i think for now i can sort of [DEL:uh] try and reassure you that um if this clears up as i [SUB:expect-&gt;expected] it would so [DEL:i] expect this to sort of be getting better in the next four or five days [DEL:um] if its not please get in touch with [SUB:a-&gt;the] medical professional again [DEL:um] and [SUB:uh-&gt;ill] [DEL:i] [DEL:would] expect it to and so therefore i would not be concerned about tuberculosis [DEL:um] your concerns about lung cancer [DEL:are] [DEL:and] was that the other thing you [SUB:are-&gt;were] concerned about [DEL:ohh] yeah yeah [DEL:yeah] [DEL:yeah] so so um again if you are not getting better please see somebody again [DEL:um] i have just got four seconds now so nice talking to you and [INS:we] have [DEL:we] got to we [INS:have] got to tidy up yeah [SUB:ok-&gt;okay] so [DEL:uh] [DEL:all] [DEL:right] [DEL:uh] and ill provide you with a sick note just to give you a few more days off work [DEL:um] and [SUB:paracetemol-&gt;paracetamol] lots of fluids [DEL:um] and [DEL:uh] rest up and as i say if you are not feeling better please get in touch [INS:okay] [SUB:ok-&gt;alright] have a good day thank you [SUB:bye-&gt;alright]</t>
+1786    1738    1626      good       good         =            &lt;NA&gt;
+1787    1739    1627       day        day         =            &lt;NA&gt;
+1788    1740    1628     thank      thank         =            &lt;NA&gt;
+1789    1741    1629       you        you         =            &lt;NA&gt;
+1790    1742    1630       bye    alright       sub             255
+[1791 rows x 6 columns]</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      ref_ix  hyp_ix reference hypothesis operation  index_edit_ops
+0          0       0     hello      hello         =            &lt;NA&gt;
+1          1       1       can        can         =            &lt;NA&gt;
+2          2       2       you        you         =            &lt;NA&gt;
+3          3       3      hear       hear         =            &lt;NA&gt;
+4          4       4        me         me         =            &lt;NA&gt;
+...      ...     ...       ...        ...       ...             ...
+1771    1738    1659      good       good         =            &lt;NA&gt;
+1772    1739    1660       day        day         =            &lt;NA&gt;
+1773    1740    1661     thank      thank         =            &lt;NA&gt;
+1774    1741    1662       you        you         =            &lt;NA&gt;
+1775    1742    &lt;NA&gt;       bye          _       del             193
+[1776 rows x 6 columns]</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>hello can you hear me okay [DEL:oh] yes i can can you hear me yeah good good so my name is joe i am a doctor here at babylon can i just confirm your name please my [INS:name] [SUB:names-&gt;is] vincent and your date of birth [SUB:ninth-&gt;nineth] of may two thousand and sixteen okay great [INS:sorry] [SUB:and-&gt;i] [SUB:are-&gt;know] you in a a safe place oh sorry a safe and confidential place to talk and just [INS:i] [SUB:happy-&gt;have] to go ahead with the consultation [DEL:yeah] [DEL:yeah] [DEL:i] [DEL:am] yes yes i am great so how can i help yeah so [INS:i] have a [INS:call] [INS:that] i have been having a cough and a sore throat for about a week and it is been causing me problems i have had to stay away from work for about three or four of those days because of [SUB:how-&gt;a] bad [SUB:is-&gt;history] okay i am sorry to hear that so you have had a cough and a sore throat for about a week and what came [DEL:what] [DEL:what] [DEL:came] first [DEL:yes] the sore throat came first and then after a day or two the cough okay [DEL:okay] and [DEL:are] [DEL:you] [DEL:coughing] [DEL:up] [DEL:anything] [DEL:no] [DEL:it] [DEL:is] [DEL:very] [DEL:dry] [DEL:okay] [DEL:so] i [DEL:am] [DEL:i] [DEL:am] just [SUB:going-&gt;want] to [SUB:ask-&gt;thank] a few questions about [DEL:the] your current symptoms and [INS:then] a little bit about your background and something else about what we can do a little bit later on in the consultation to help you [SUB:so-&gt;but] before we go on anything you are particularly concerned about or have any ideas what might be going on you said that you had a cold [DEL:okay] well i mean you [DEL:you] know how we all are once this happens you google it and [SUB:there-&gt;it] seems to be all kinds of bad things it could be [DEL:it] [DEL:could] [DEL:be] [DEL:could] [DEL:be] a cold or flu obviously [SUB:but-&gt;obviously] [SUB:it-&gt;because] [SUB:could-&gt;we] [DEL:also] [DEL:be] tuberculosis [SUB:it-&gt;the] [DEL:could] [DEL:be] cancer always comes up so it will be good if [DEL:none] [DEL:of] those [SUB:great-&gt;right] [SUB:so-&gt;say] [SUB:so-&gt;say] yeah i can provide a [INS:little] bit of reassurance and we can talk about those a little bit as well and was there [SUB:anything-&gt;any] you [SUB:were-&gt;are] particularly expecting or hoping to get out of this consultation [DEL:okay] well yeah so reassurance so [DEL:like] hopefully some sense that it is not anything too serious but also [SUB:is-&gt;if] there [INS:is] anything you can prescribe me to make it better or any advice or maybe even a sick note so [DEL:that] if i need to stay away from work for a bit longer i can get one sure sure okay all right so we will talk a little bit about the symptoms and i am sure we can get [DEL:a] those things [INS:some] [INS:secrets] and some reassurance [INS:thank] [INS:you] about your concerns [DEL:okay] so you mentioned that you started with [INS:a] sore throat about a week ago developed into [INS:a] bit of a dry cough [INS:and] i [DEL:will] just ask a few questions around those [INS:those] so do you have any shortness of breath [DEL:no] yes yes [SUB:i-&gt;we] [SUB:have-&gt;are] [DEL:been] having [SUB:shortness-&gt;shorts] [SUB:of-&gt;oh] yeah i have been having shortness of breath [DEL:yeah] you are short of breath and do you have any wheeze or chest pain yeah [DEL:a] [DEL:bit] [DEL:of] [DEL:both] you are [DEL:you] [DEL:are] feeling a bit wheezy with some chest pain as well yes okay and [DEL:how] when did you start to develop [SUB:the-&gt;a] shortness of breath [INS:let] [INS:us] [SUB:so-&gt;see] so the sore throat so [INS:today] [SUB:todays-&gt;is] friday sore throat was about last [DEL:week] friday or thursday cough was saturday or sunday so the [DEL:so] [DEL:the] shortness of breath was i think shortly after the cough so maybe a day or two later so three [INS:or] four days ago three or four days ago you started [SUB:develop-&gt;developing] and is the cough worse at [SUB:nighttime-&gt;night] [SUB:no-&gt;time] no it is the same throughout the [DEL:whole] day [DEL:same] [DEL:throughout] [DEL:the] [DEL:day] and when you say you are short of breath just need to try and get an idea about how short of breath you are so are you able to [DEL:so] [DEL:so] like walk up [SUB:a-&gt;flights] [DEL:flight] of stairs for example or [DEL:or] are you short [DEL:of] breath [SUB:at-&gt;of] rest oh yeah it is [DEL:it] [DEL:is] like [DEL:so] when i am doing walking and i do [SUB:exercises-&gt;exercise] now and then so it [DEL:it] has not been [INS:super] [SUB:superbad-&gt;bad] like has not stopped me from doing any of those things but it is been pretty unusual and a little bit [SUB:worrying-&gt;worried] and you are a bit concerned about that okay so i just need to ask a few things about your background as well so do you have any other medical conditions or medical history no just no no [DEL:past] [DEL:medical] [DEL:history] no [DEL:no] [DEL:no] history of asthma no and any history of clots on your legs or your lungs [INS:these] [INS:are] [INS:ddts] [SUB:so-&gt;or] [SUB:these-&gt;ps] no one in your familys had those clots on the legs or the lungs well my mother had lung cancer your mother had lung cancer do you smoke no [INS:have] you ever smoked or been exposed to asbestos [SUB:that-&gt;i] [DEL:you] [DEL:know] [DEL:of] do not know [SUB:with-&gt;if] asbestos ever smoked i mean once or twice in amsterdam [SUB:if-&gt;in] [SUB:that-&gt;dakar] [DEL:counts] but not really okay and this [DEL:so] just going back to [DEL:the] your symptoms of shortness of breath with the cough it is a dry cough [DEL:no] [DEL:you] [DEL:are] not [SUB:coughing-&gt;cough] [SUB:up-&gt;cap] [DEL:any] flem do [DEL:do] you have and you [DEL:do] [DEL:not] [DEL:you] say you do not have any chest pain as such are you taking any medications currently at the moment no [INS:i] [INS:am] [SUB:no-&gt;not] okay are you allergic to any medications not to any medication but i am allergic to peanuts peanuts okay and you mentioned that your mother had lung cancer any other family history of any significant illnesses [SUB:run-&gt;when] running [SUB:in-&gt;into] [DEL:your] family no no that is the only one just lung cancer from my mother [DEL:just] [DEL:lung] [DEL:cancer] okay and you say you have a cold so do you have sinus congestion or no it seems to be [INS:all] entirely with just my throat [DEL:so] like my nose is [SUB:like-&gt;just] [SUB:so-&gt;running] [SUB:just-&gt;out] [DEL:your] just your throat and any recent travel or have you always lived in the uk no so i i [DEL:i] have not always lived in the uk like so i was born in the us and [DEL:moved] [DEL:over] [DEL:well] [DEL:it] [DEL:was] twelve years ago but [SUB:in-&gt;it] [SUB:terms-&gt;is] [SUB:of-&gt;a] recent travel just to europe nowhere [SUB:too-&gt;to] exotic okay so no so no recent travel no significant recent travel [DEL:any] anywhere okay and are you coughing up anything other than so you [DEL:you] are not coughing up blood or anything like that [DEL:no] [DEL:no] good and are you feeling feverish hot cold sweaty [DEL:yeah] so a little bit feverish at first so the first three or so days of this but then [DEL:it] the fevers gone away okay and in general do you [INS:feel] [INS:better] sorry yeah yeah i was just going to say [INS:i] also had a bit of a headache [DEL:but] like headaches that come and go rather but [DEL:like] right now it is fine okay and in general would you say you are [DEL:feeling] [DEL:you] [DEL:are] [DEL:you] [DEL:are] beginning to [DEL:to] feel better worse or [DEL:or] sort of staying the same so it is like it is up and down so [DEL:so] let us see so i [DEL:it] started last week and i stayed home from work two days this week i think it was maybe tuesday and then thursday so like i felt better and then worse again and then better and then worse again so it is been [DEL:yeah] a kind of constant but constant [SUB:and-&gt;in] being variable [DEL:if] [DEL:that] [DEL:makes] okay and i just need to ask any other sort of risk factors that you may have so no sort of significant weight loss or unexplained weight loss any so no [INS:no] weight loss but i have been [DEL:have] [DEL:been] losing my appetite recently and i mean i usually eat a lot so [DEL:and] i [DEL:and] [DEL:i] enjoy eating as well but [DEL:like] [DEL:so] that is been a bit concerning you have been losing your appetite recently yes and you are a little bit concerned about that but you have not [SUB:you-&gt;lost] [SUB:have-&gt;any] [SUB:not-&gt;weight] lost any weight that you think [DEL:of] [DEL:yes] no not that and any sort of rashes or anything [DEL:or] and you no [SUB:not-&gt;no] [DEL:not] [DEL:that] [DEL:not] [DEL:that] [DEL:you] [DEL:can] [DEL:think] [DEL:of] okay so i would ask to examine you now but i i do not know if i could sort of look inside your throat at least [DEL:to] see if there is a probably [DEL:there] [DEL:is] [DEL:oh] we can try oh no well no it is okay i might think about doing [DEL:a] have you got any lumps or bumps around your neck that you [SUB:can-&gt;could] feel no [SUB:no-&gt;not] [SUB:that-&gt;the] [DEL:you] no okay and [INS:and] so finally you [DEL:you] were talking about i [DEL:mean] it sounds to me that you have been a little bit up and down sore throat developed a dry cough you are slightly short of breath but not too overly concerningly short of breath what i would say we are just coming to the end of [INS:the] consultation now [INS:is] if you feel significantly worse if you get more short of breath or sudden change in your breathlessness or breathlessness that you are concerned about [SUB:then-&gt;and] i would advise you to see [DEL:no] [DEL:go] [DEL:and] [DEL:see] a gp and actually see [SUB:somebody-&gt;something] physically but i think for now i can sort of try and reassure you that if this clears up as i expect it would so [DEL:i] expect this to sort of be getting better in the next four or five days if it is not please get in touch with [SUB:a-&gt;the] medical professional again and i would expect it to and so therefore i would not be concerned about tuberculosis your concerns about lung cancer are [DEL:and] was that the other thing you [SUB:are-&gt;were] concerned about oh yeah yeah [DEL:yeah] [DEL:yeah] so [DEL:so] again if you are not getting better please see somebody again i have just got four seconds now so nice talking to you and [DEL:have] we [SUB:got-&gt;have] [DEL:to] [DEL:we] got to tidy up yeah okay [INS:okay] so [DEL:all] [DEL:right] and i will provide you with a sick note just to give you a few more days [SUB:off-&gt;of] work and [SUB:paracetemol-&gt;paracetamol] lots of fluids and rest up and as i say if you are not feeling better please get in touch okay [SUB:have-&gt;all] [SUB:a-&gt;right] [DEL:good] [DEL:day] thank you [DEL:bye]</t>
+        </is>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>hello can you hear me okay [SUB:oh-&gt;hey] yes i can can you hear me yeah good good so my name is joe i am a doctor here at babylon can i just confirm your name please [INS:hey] my [INS:name] [SUB:names-&gt;is] vincent and your date of birth [SUB:ninth-&gt;nine] of may two thousand and sixteen okay great [INS:sorry] and are you in a [INS:be] a safe place oh sorry a safe and confidential place to talk and [INS:discuss] [INS:yeah] [INS:i] [SUB:just-&gt;am] happy to go ahead with the consultation [DEL:yeah] [DEL:yeah] [DEL:i] [DEL:am] yes yes i am great so how can i help yeah so [INS:i] have a [INS:call] [INS:up] i have been having a cough and a sore throat for about a week and it is been causing me problems i have had to stay away from work for about three or four of those days because of [SUB:how-&gt;it] [DEL:bad] [DEL:is] okay i am sorry to hear that so you have had a cough and a sore throat for about a week and what came what [DEL:what] came first [DEL:yes] the sore throat came first and then after a day or two the cough okay [DEL:okay] and are you coughing up anything no it is very dry okay so i am [DEL:i] [DEL:am] just going to ask a few questions about the your current symptoms and [INS:then] a little bit about your background and something else about what we can do a little bit later on in the consultation to help you [SUB:so-&gt;but] before we go on anything you are particularly concerned about or have any [SUB:ideas-&gt;right] [DEL:what] [DEL:might] [DEL:be] [DEL:going] [DEL:on] [DEL:you] [DEL:said] [DEL:that] [DEL:you] [DEL:had] [DEL:a] [DEL:cold] [DEL:okay] [DEL:well] [DEL:i] [DEL:mean] [DEL:you] [DEL:you] [DEL:know] [DEL:how] [DEL:we] [DEL:all] [DEL:are] [DEL:once] [DEL:this] [DEL:happens] [DEL:you] [DEL:google] [DEL:it] [DEL:and] [DEL:there] [DEL:seems] [DEL:to] [DEL:be] [DEL:all] [DEL:kinds] [DEL:of] [DEL:bad] [DEL:things] [DEL:it] [DEL:could] [DEL:be] [DEL:it] [DEL:could] [DEL:be] [DEL:could] [DEL:be] [DEL:a] [DEL:cold] [DEL:or] [DEL:flu] [DEL:obviously] [DEL:but] [DEL:it] [DEL:could] [DEL:also] [DEL:be] [DEL:tuberculosis] [DEL:it] [DEL:could] [DEL:be] [DEL:cancer] [DEL:always] [DEL:comes] [DEL:up] so [DEL:it] [DEL:will] [DEL:be] [DEL:good] [DEL:if] [DEL:none] [DEL:of] [DEL:those] [DEL:great] so [DEL:so] yeah i can provide a [INS:little] bit of reassurance and we can talk about those a little bit as well [DEL:and] was there anything you were particularly expecting or hoping to get out of this consultation [DEL:okay] well yeah so reassurance so like hopefully [INS:in] some sense that [DEL:it] is not anything too serious but also is there anything you can prescribe me to make it better or any advice or maybe even a sick note so that if i need to stay away from work for a bit longer i can get one sure sure okay all right so we will talk a little bit about the symptoms and i am sure we can get a those things [INS:sorted] and some reassurance [INS:thank] [INS:you] about your concerns [DEL:okay] so you mentioned that you started with [INS:a] sore throat about a week ago developed into [INS:a] bit of a dry cough [INS:and] i will just ask a few questions around those so do you have any shortness of breath [DEL:no] yes yes i have been having shortness of [INS:oh] yeah i have been having shortness of breath yeah you are short of breath and do you have any wheeze or chest pain yeah [DEL:a] [DEL:bit] [DEL:of] [DEL:both] you are [DEL:you] [DEL:are] feeling a bit wheezy with some chest pain as well yes okay and how when did you start to develop the shortness of breath so [DEL:so] the sore throat so [INS:today] [SUB:todays-&gt;is] friday sore throat was about [DEL:last] [DEL:week] friday or thursday cough was saturday or sunday so the [DEL:so] [DEL:the] shortness of breath was i think shortly after the cough so maybe a day or two later so three [INS:or] four days ago [SUB:three-&gt;two] or four days ago you [INS:start] [SUB:started-&gt;to] develop [INS:symptoms] and is the cough worse at [INS:night] [SUB:nighttime-&gt;time] no no it is the same throughout the [DEL:whole] day same throughout the day and when you say you are short of breath just need to try and get an idea about how short of breath you are so are you able to [DEL:so] [DEL:so] like walk up a flight of stairs for example or [DEL:or] are you short of breath at rest oh yeah it is [DEL:it] [DEL:is] like [DEL:so] when i am doing walking and i do [SUB:exercises-&gt;exercise] now and then so it it has not been [INS:super] [SUB:superbad-&gt;bad] like has not stopped me from doing any of those things but it is been pretty unusual and a little bit worrying and you are a bit concerned about that okay so i just need to ask a few things about your background as well so do you have any other medical conditions or medical history no just no no past medical history no no [DEL:no] history of asthma no and any history of clots on your legs or your lungs so these [INS:are] [INS:ddps] [INS:or] [INS:ps] [SUB:no-&gt;and] [SUB:one-&gt;none] [SUB:in-&gt;of] your [SUB:familys-&gt;families] had those clots [SUB:on-&gt;in] the legs or [DEL:the] lungs well my mother had lung cancer your mother had lung cancer do you smoke no you ever smoked or been exposed to asbestos [DEL:that] you know [DEL:of] do not know [SUB:with-&gt;if] asbestos ever smoked i mean once or twice in amsterdam [SUB:if-&gt;with] that [SUB:counts-&gt;car] but not really okay and this so just going back to the your symptoms of shortness of breath with the cough it is a dry cough no you are not coughing up any [SUB:flem-&gt;phlegm] do [INS:you] do you have and you [DEL:do] [DEL:not] [DEL:you] say you do not have any chest pain as such are you taking any medications currently at the moment no [INS:i] [INS:am] [SUB:no-&gt;not] okay are you allergic to any medications not [DEL:to] any medication but i am allergic to peanuts peanuts okay and [INS:and] you mentioned that your mother had lung cancer [INS:and] any other family history of any significant illnesses [SUB:run-&gt;when] running in your family no no that is the only one just lung cancer from my mother just lung cancer okay and you say you have a cold so do you have sinus congestion or no it seems to be [INS:almost] entirely [DEL:with] just my throat [DEL:so] like [SUB:my-&gt;j] [DEL:nose] [DEL:is] [DEL:like] [DEL:so] just your just your throat and any recent travel or have you always lived in the [INS:you] [SUB:uk-&gt;k] no so i i [DEL:i] have not always lived in the [INS:you] [SUB:uk-&gt;k] like so i was born in the [INS:you] [SUB:us-&gt;s] and moved over [SUB:well-&gt;about] [DEL:it] [DEL:was] twelve years ago but in terms of recent travel just to europe nowhere [SUB:too-&gt;to] exotic okay so no so no recent travel no significant recent travel [DEL:any] anywhere okay and are you coughing up anything other than so you [DEL:you] are not coughing up blood or anything like that no [DEL:no] good and are you feeling feverish hot cold sweaty yeah so a little bit feverish at first so the first three or so days of this but then [DEL:it] the fevers gone away okay and in general do you sorry yeah [DEL:yeah] i was just going to say also had a bit of a headache [DEL:but] like headaches that come and go rather but like right now it is fine okay and in general would you say you are feeling you are you are beginning to to feel better worse or or sort of staying the same so it is like it is up and down so so let us see so i [DEL:it] started last week and i stayed home from work two days this week i think it was maybe tuesday and then thursday so like i felt better and then worse again and then better and then worse again so it is been yeah a kind of constant but constant [SUB:and-&gt;in] being variable [SUB:if-&gt;but] [DEL:that] [DEL:makes] okay and i just [INS:really] need to ask any other sort of risk factors that you may have so no sort of significant weight loss or unexplained weight loss any so no weight loss but i have been have been losing my appetite recently and i mean i usually eat a lot so [DEL:and] i [DEL:and] [DEL:i] enjoy eating as well but like [DEL:so] that is been a bit concerning you have been losing your appetite recently yes and you are a little bit concerned about that but you have not you have not lost any weight that you think [DEL:of] [DEL:yes] no not that and any sort of rashes or anything [DEL:or] and you no [SUB:not-&gt;rash] [SUB:not-&gt;no] [DEL:that] [DEL:not] [DEL:that] you can [SUB:think-&gt;go] [DEL:of] okay so i would ask to examine you now but i i do not know if i could sort of look inside your throat at least to see if there is a probably there is oh we can try [INS:it] [INS:on] oh no well no it is okay i might think about doing [SUB:a-&gt;it] have you got any lumps or bumps around your neck that you can feel no [SUB:no-&gt;not] [SUB:that-&gt;the] [DEL:you] no okay and [INS:and] so finally you you were talking about i mean it sounds to me that you have been a little bit up and down sore throat developed a dry cough [INS:and] you are slightly short of breath but not too overly concerningly short of breath what i would say we are just coming to the end [SUB:of-&gt;so] consultation [INS:hours] [SUB:now-&gt;is] if you feel significantly worse if you get more short of breath or sudden change in your breathlessness or breathlessness that you are concerned about [SUB:then-&gt;and] i would advise you to see [SUB:no-&gt;your] [DEL:go] [DEL:and] [DEL:see] [DEL:a] gp and actually see somebody physically but i think for now i can sort of try and reassure you that if this clears up as i [SUB:expect-&gt;expected] it would so [DEL:i] expect this to sort of be getting better in the next four or five days if it is not please get in touch with [SUB:a-&gt;the] medical professional again and i [SUB:would-&gt;will] expect it to and so therefore i would not be concerned about tuberculosis your concerns about lung cancer [DEL:are] [DEL:and] was that the other thing you [SUB:are-&gt;were] concerned about [DEL:oh] yeah yeah [DEL:yeah] [DEL:yeah] so so again if you are not getting better please see somebody again i have just got four seconds now so nice talking to you and [INS:we] have [DEL:we] got to we [INS:have] got to tidy up yeah okay so [DEL:all] [DEL:right] and i will provide you with a sick note just to give you a few more days off work and [SUB:paracetemol-&gt;paracetamol] lots of fluids and rest up and as i say if you are not feeling better please get in touch okay [INS:alright] have a good day thank you [SUB:bye-&gt;alright]</t>
+        </is>
+      </c>
+      <c r="AM2" t="inlineStr">
+        <is>
+          <t>hello can you hear me okay [SUB:oh-&gt;hey] yes i can can you hear me yeah good good so my name is joe i am a doctor here at babylon can i just confirm your name please [INS:hey] my names vincent and your date of birth [SUB:ninth-&gt;nineth] of may two thousand and sixteen okay great and are you in a [DEL:a] safe place oh sorry a safe and confidential place to talk and just [SUB:happy-&gt;have] to go ahead with the consultation [DEL:yeah] [DEL:yeah] [DEL:i] [DEL:am] yes yes i am great so how can i help yeah so [INS:i] have a [INS:call] [INS:up] i have been having a cough and a sore throat for about a week and it is been causing me problems i have had to stay away from work for about three or four of those days because of [SUB:how-&gt;a] [SUB:bad-&gt;bandit] [DEL:is] okay i am sorry to hear that so you have had a cough and a sore throat for about a week and what came [DEL:what] [DEL:what] [DEL:came] first [DEL:yes] the sore throat came first and then after a day or two the cough okay okay and are you coughing up anything no it is very dry okay so i am [DEL:i] [DEL:am] just going to ask a few questions about [DEL:the] your current symptoms and [INS:then] a little bit about your background and something else about what we can do a little bit later on in the consultation to help you [SUB:so-&gt;but] before [SUB:we-&gt;i] go on anything you are particularly concerned about or have any ideas what might be going on you said that you had a cold [DEL:okay] well i mean you [DEL:you] know how we all are once this happens you google it and [SUB:there-&gt;it] seems to be all kinds of bad things it could be it could be [INS:it] could be a cold or flu obviously but [DEL:it] [DEL:could] [DEL:also] [DEL:be] tuberculosis it could be cancer always comes up so it will be good if none of those [SUB:great-&gt;right] so [DEL:so] yeah i can provide a [INS:little] bit of reassurance and we can talk about those a little bit as well and was there anything you were particularly expecting or hoping to get out of this consultation [DEL:okay] well yeah so reassurance so [DEL:like] hopefully some sense that it is not anything too serious but also [SUB:is-&gt;if] there [INS:is] anything you can prescribe me to make it better or any advice or maybe even a sick note so [DEL:that] if i need to stay away from work for a bit longer i can get one sure sure okay all right so we will talk a little bit about the symptoms and i am sure we can get [DEL:a] those things and some reassurance about your concerns [DEL:okay] so you mentioned that you started with [INS:a] sore throat about a week ago developed into [INS:a] bit of a dry cough i will just ask a few questions around those so do you have any shortness of breath [DEL:no] yes yes i have been having shortness of [INS:breath] yeah i have been having shortness of breath [DEL:yeah] you are short of breath and do you have any wheeze or chest pain yeah a bit of [SUB:both-&gt;four] [SUB:you-&gt;attacks] [DEL:are] you are feeling a bit wheezy with some chest pain as well yes okay and how when did you start to develop the shortness of breath [INS:i] [INS:think] so so the sore throat so [INS:today] [SUB:todays-&gt;is] friday [INS:the] sore throat was about last week friday or thursday cough was [SUB:saturday-&gt;satisfied] [DEL:or] [DEL:sunday] so the [DEL:so] [DEL:the] shortness of breath was i think shortly after the cough so maybe a day or two later so three four days ago three or four days ago you started [SUB:develop-&gt;developing] and is the cough worse at [SUB:nighttime-&gt;night] [SUB:no-&gt;time] no it is the same throughout the [SUB:whole-&gt;week] [DEL:day] same throughout the day and when you say you are short of breath just need to try and get an idea about how short of breath you are so are you able to [SUB:so-&gt;get] [DEL:so] [DEL:like] walk up a flight of stairs for example or [DEL:or] are you short of breath at rest oh yeah it is [DEL:it] [DEL:is] like [DEL:so] when i am doing walking and i do [SUB:exercises-&gt;exercise] now and then so it [DEL:it] has not been [INS:super] [SUB:superbad-&gt;bad] like [INS:it] has not stopped me from doing any of those things but it is been pretty unusual and a little bit [SUB:worrying-&gt;worried] and you are a bit concerned about that okay so i just need to ask a few things about your background as well so do you have any other medical conditions or medical history no just no no past medical history [INS:now] no [INS:past] [SUB:no-&gt;microgravity] no history of asthma no and any history of clots on your legs or your lungs so these [INS:are] [INS:dvds] [INS:or] [SUB:no-&gt;ps] [SUB:one-&gt;none] in your familys had those clots [SUB:on-&gt;in] the legs or [DEL:the] lungs well my mother had lung cancer your mother had lung cancer do you smoke no [INS:have] you ever smoked or been exposed to asbestos [DEL:that] you know [DEL:of] do not know [SUB:with-&gt;if] asbestos ever smoked i mean once or twice in amsterdam [DEL:if] [DEL:that] [DEL:counts] but not really okay and this [DEL:so] just going back to [DEL:the] your symptoms of shortness of breath with the cough it is a dry cough no you are not coughing up [SUB:any-&gt;anyphlem] [DEL:flem] do [DEL:do] you have and you [DEL:do] [DEL:not] [DEL:you] say you do not have any chest pain as such are you taking any medications currently at the moment no no okay are you allergic to any medications not to any medication but i am allergic to peanuts peanuts okay and you mentioned that your mother had lung cancer any other family history of any significant illnesses [SUB:run-&gt;when] running in your family no no that is the only one just lung cancer from my mother just lung cancer okay and you say you have a cold so do you have sinus congestion or no it seems to be [INS:all] entirely with just my throat [DEL:so] like my nose is [SUB:like-&gt;tiny] [SUB:so-&gt;now] just your [DEL:just] [DEL:your] throat and any recent travel or have you always lived in the uk no so i [DEL:i] [DEL:i] have not always lived in the uk [DEL:like] so i was born in the us and moved over [DEL:well] [DEL:it] [DEL:was] twelve years ago but in terms of recent travel just to europe [SUB:nowhere-&gt;to] [DEL:too] exotic okay so no [DEL:so] [DEL:no] recent travel no significant recent travel [DEL:any] anywhere okay and are you coughing up anything other than so you [DEL:you] are not coughing up blood or anything like that no [DEL:no] good and are you feeling feverish hot cold sweaty yeah so a little bit feverish at first so the first three or so days of this but then [DEL:it] the fevers gone away okay and in general do you [SUB:sorry-&gt;feel] yeah [DEL:yeah] i was just going to say also had a bit of a headache [DEL:but] like headaches that come and go rather but like right now it is fine okay and in general would you say you are feeling you are [DEL:you] [DEL:are] beginning to [DEL:to] feel better worse or [DEL:or] sort of staying the same so it is like it is up and down so [DEL:so] let us see so i [DEL:it] started last week and i stayed home from work two days this week i think it was maybe tuesday and then thursday so like i felt better and then worse again and then better and then worse again so it is been [DEL:yeah] a kind of constant but constant [SUB:and-&gt;in] being variable if that [INS:make] [SUB:makes-&gt;me] okay and i just need to ask any other sort of risk factors that you may have so no sort of significant weight loss or unexplained weight loss any [INS:waters] so no weight loss but i have been have been losing my appetite recently and i mean i usually eat a lot so [DEL:and] i [DEL:and] [DEL:i] enjoy eating as well but like [DEL:so] that is been a bit concerning you have been losing your appetite recently yes and you are a little bit concerned about that but you have not you have not lost any weight that you think of [DEL:yes] no not that and any sort of rashes or anything [DEL:or] [DEL:and] [DEL:you] no [SUB:not-&gt;rash] [DEL:not] [DEL:that] [DEL:not] [DEL:that] [DEL:you] [DEL:can] [DEL:think] [DEL:of] okay so i would ask to examine you now but i [DEL:i] do not know if i could sort of look inside your throat at least to see if there is a probably [DEL:there] [DEL:is] [DEL:oh] we can try oh no well no it is okay i might think about doing [SUB:a-&gt;that] have you got any lumps or bumps around your neck that you can feel no no [DEL:that] [DEL:you] [DEL:no] okay and so finally you [DEL:you] were talking about i mean it sounds to me that you have been a little bit up and down sore throat developed a dry cough you are slightly short of breath but not too overly concerningly short of breath what i would say we are just coming to the end of [INS:the] consultation now [INS:is] if you feel significantly worse if you get more short of breath or sudden change in your breathlessness or breathlessness that you are concerned about [SUB:then-&gt;and] i would advise you to [SUB:see-&gt;seek] [SUB:no-&gt;medical] [SUB:go-&gt;tension] [SUB:and-&gt;games] [SUB:see-&gt;here] [DEL:a] gp and actually see somebody physically but i think for now i can sort of try and reassure you that if this clears up as i expect it would so [DEL:i] expect this to sort of be getting better in the next four or five days if it is not please get in touch with [SUB:a-&gt;the] medical professional again and i would expect it [SUB:to-&gt;too] and so therefore i would not be concerned about tuberculosis your concerns about lung cancer are [DEL:and] was that the other thing you [DEL:are] concerned about [DEL:oh] yeah [SUB:yeah-&gt;oh] yeah yeah so so again if you are not getting better please see somebody again i have just got four seconds now so nice talking to you and [DEL:have] we [SUB:got-&gt;have] [DEL:to] [DEL:we] got to tidy up yeah okay so [DEL:all] [DEL:right] and i will provide you with a sick note just to give you a few more days off work and [SUB:paracetemol-&gt;paracetamol] lots of fluids and rest up and as i say if you are not feeling better please get in touch okay [INS:all] [INS:right] [INS:thanks] [INS:a] [INS:lot] have a good day thank you [DEL:bye]</t>
         </is>
       </c>
     </row>
@@ -759,74 +873,111 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>hello hello good afternoon good afternoon i am doctor yemi and ill be the one attending to you this afternoon all right so can you tell me what brought you to the hospital i have been havingerm my body has been feeling hot for a while now as in very hot oh i am so sorry to hear about that so id like to know more about this so i would know how best to you know help you so when did it start started a week ago was is sudden in onset or it was gradual it was gradual and how has it been since then has it progressed has it gotten better or it has gotten worse it has gotten worse ok aside from this high body temperature do you have any other associated symptom yes i have been having this very bad headache ok body pains ok ok ok so all these symptoms now did it starts with the high body temperature yes and it especially it gets worse at night at night ok ok so you feel like what of during the day how how do you feel during the day during the day erm i vomit like i vomited for example today now i vomited like four times ok this morning ok so the headache what part of your head are you have having this headache the my front part of my head front part of your head i will do you describe it like any associated eye pain no ok hmm last month ok so you have not you have not had a missed yeah ok alright thank you very much so aside from this id like to ermso what have you done since it started so far i have not done i have i have only taken paracetamol you have only taken para and any any any relief with paracetamol just for a short while ok ok ok so erm id just like to ask some other systemic questions to be sure that everything is fine with other systems so from any uhm neck pain or stiffness no any cough or chest pain no have you been going to have you any urinary symptoms no any diarrhea no ok so like from what you told me so far you said you have been having high body temperature yes there was headache and body pain and you shiver for about a week now am i correct and also this happens more in the evenings ok and there is also been vomiting how about your appetite has your appetite been fine it has reduced reduced appetite ok ok so are you being erm i would like to ask for your past medical history now are you been managed for any medical condition no in the past are you on any routine medications no do you drink alcohol no do you smoke cigarettes no have you had surgery before in the past no have you ever been admitted in the hospital no have you ever been transfused with blood no ok erm are you married no ok are you sexually active no ok that is that is that is that is ok and what do you do for work i am a student oh ok where do you school unilag ok now i am most i would like to ask for this erm consultation are you paying out of pocket or you are under insurance i am paying out of pocket and how are your finances like you know well depend i am depending on my parents ok ok ok alright that is that is very good so erm asides this is there any other thing that you think its important that i might have missed out in the course of this conversation none for now ok alright thank you very much so id like to examine you now ill do a general examination and for and focus and systemic examinations so well from what you have told me so far let us just you know do a quick recap you said you have been having headache body pains and fever for about a week with vomiting so and this it occurs more in the evenings so i am thinking you are having a condition you are having malaria so but what what would need to do is well need to confirm well take blood samples to the lab well do erm malaria parasite test so if it comes out positive well give you medications for malaria but for now wed give you paracetamol for the fever and the erm headache and the body pains so wed also like you to you know bed rest if you need erm notes for school to maybe exempt you from school we can also issue that for you do you have any other thing you would like you know like me to help with so ill direct you to the lab where they will do the test and while we await the test results alright have any other thing no alright thank you so much for your time thank you very much alright have a lovely day you too bye</t>
+          <t>Hello. Hello. Good afternoon. Good afternoon. I'm Dr. Yemi and I'll be the one attending to you this afternoon. Alright, so can you tell me what brought you to the hospital? I've been having my body has been feeling hot for a while now. It's very hot. Oh, I'm so sorry to hear about that. So I'd like to know more about this so I'd know how best to you know help you. So when did it start? Started a week ago. Was it suddenly also that it was gradual? It was gradual. And how has it been since then? Has it progressed? Has it gotten better? It has gotten worse. It has gotten worse. Okay. Aside from this high body temperature, do you have any other associated symptoms? Yes, I've been having this very bad headache. Okay. Body pains. Okay. And sometimes I shiver. Okay, okay. So all these symptoms now, this starts with the high body temperature. Yes, and it especially gets worse at night. At night, okay, okay. So you feel like what of during the day? How do you feel during the day? During the day, I vomit. Like I've vomited, for example, today I vomited like four times this morning. Okay. So the headache, what part of your head are you having this headache? The front part of my head. Front part of your head. Did you describe it like in any associated eye pain? No. Okay. I would like to ask you, when was your last menstrual period? Last morning. Okay, so you've not had a missed period. Yes. Okay, all right. Thank you very much. So aside from this, I'd like to. So what have you done since it started so far? I haven't done. I won't take parasitomol. If you need any relief with paracetamol, just for a short while. Okay, okay, okay. So I'd just like to ask some other systemic questions to be sure that everything is fine with other systems. So from any neck pain or stiffness? No. Any cough or chest pain? No. Have you been going to have you any urinary symptoms? No. Any diarrhea? No. Okay. So like from what you told me so far, you said you've been having high body temperature. Yes. There was headache and body pain and you shiver for about a week now. Am I correct? And also this happens more in the evenings. Okay, and there's also been vomiting. How about appetite? Appetite's been fine? Reduced. Reduced appetite. Okay, okay. So are you being I would like to ask for your past medical history now? Have you been married for any medical condition in the past? Are you on any routine medications? No. Do you drink alcohol? No. Do you smoke cigarettes? Have you had surgery before in the past? No. Have you ever been admitted in the hospital? No. Have you ever been transfused with blood? No. Okay. Are you married? No. Okay. Are you sexually active? No. Okay, that's that's that's that's okay. And what do you do for work? I'm a student. Okay, where do you school? Um you know, okay. Now, um, who's I would like to ask for this um consultation. Are you paying out of pocket or yeah under insurance? I'm paying out of pocket. And how are your finances? Like, you know, um, well, depend, I'm depending on my parents. Okay, okay, okay, all right. That's that's very good. So, um, aside, is there any other thing that you think is important that I must have missed out in the course of this um conversation? None for now. Okay, all right, thank you very much. So, I'd like to um examine you now. I'll do a general examination and focus and systemic examinations. So, um, well, from what you've told me so far, let's just you know, do a quick recap. You said you've been having headache, body pains, and fever for about a week. You're vomiting, so and this cause more in the evenings. So, I'm thinking you are having a condition, you're having malaria. So, but what we would need to do is we'll need to confirm. We'll take um blood samples to the lab, we'll do malaria parasite tests. So, if it comes out positive, we'll give you medications for malaria. But for now, we'll give you um paracetamol for the fever and the um headache and the body pains. So, um, also like you to you know, bed rest if you need notes for school to maybe exempt you from school. We can also issue that for you. Do you have any other thing would like you know, like me to help with? So, I'll direct you to the lab where you'll do the test and while we await the test results. All right, have any other thing? No, all right, thank you so much for your time. Thank you, all right. Have a lovely day. Bye.</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>hello hello good afternoon good afternoon i am doctor yemi and ill be the one attending to you this afternoon alright so can you tell me what brought you to the hospital i have been having my body has been feeling hot for a while now its very hot oh i am so sorry to hear about that so id like to know more about this so id know how best to help you when did it start it started a week ago sorry to hear about that so id like to know more about this so id know how best to you know help you so when did it start started a week ago was this sudden onset it was gradual it was gradual and how has it been since then has it progressed has it gotten better it has gotten worse it has gotten worse okay aside from this high body temperature do you have any other associated dead yes i have been having this very bad headache okay body pains okay and sometimes i shiver okay okay so all these symptoms do they start with the high body temperature yes and it especially gets worse at night at night okay okay so you feel like what during the day how do you feel during the day during the day um i vomit like i vomited for example today and i vomited like four times okay okay so the headache what part of your head are you having this headache my front part of my front part of your head i will describe it like in any actual eye pain no okay id like to ask you um when was your last menstrual period um last morning okay so you have done you have all had the missed period yeah okay all right thank you very much so aside from this id like to um so what have you done since it started so far i have not done i am i will not take you first with paracetamol just for a short while okay okay okay so um id just like to ask some other systemic questions to be sure that everything is fine with our systems so from um any um neck pain or stiffness no any cough or chest pain have pain no have you been going to have you any urinary symptoms no any diarrhea no okay so like from what you told me so far you said you have been having high body temperature yes there was headache and body pain and you shivered for about a week now am i correct i correct and also this happens more in the evenings okay and there is also been vomiting how about your appetite are you ever tired of being fine uh that is reduced reduced appetite okay okay so are you being me um id like to ask for your past medical history now i have been married to any medical condition in the past are you on any routine medications um do you drink alcohol do you smoke cigarettes have you had surgery before in the past have you ever been addicted in the hospital no you have been transfused with blood okay um are you married no okay are you sexually active no okay that is that is that is okay and what do you do for work i am a student oh okay where do you school um you know okay now um i would like to ask for this um consultation are you paying out of pocket or yeah under insurance i am paying out of pocket and how are your finances like you know um well depend i am depending on my parents okay okay okay all right that is that is very good so um is there any other thing that you think is important that i must have missed out in the course of this um conversation none for now okay all right thank you very much so id like to um examine you now ill do a general examination and and systemic examinations so um well from what you have told me so far let us just you know do a quick recap he said you have been having headache body pains and fever for about a week you are vomiting so and its your because more in the evenings so i am thinking you are having a condition you are having malaria so but what we need to do is we need to confirm we take blood samples to the lab well do a malaria parasite test so if it comes out positive well give you medications for malaria but for now well give you um paracetamol for the fever and the headache and the body pains so i would also like you to you know bed rest if you need notes for school to maybe exempt you from school we can also issue that for you do you have any other thing would like you know like me to help with so ill direct you to the lab where they will do the test and well which the test results all right have any other thing no all right thank you so much for your time all right have a lovely day bye</t>
+          <t>hello hello good afternoon good afternoon i am doctor yemi and i will be the one attending to you this afternoon all right so can you tell me what brought you to the hospital i have been havingerm my body has been feeling hot for a while now as in very hot oh i am so sorry to hear about that so i would like to know more about this so i would know how best to you know help you so when did it start started a week ago was is sudden in onset or it was gradual it was gradual and how has it been since then has it progressed has it gotten better or it has gotten worse it has gotten worse okay aside from this high body temperature do you have any other associated symptom yes i have been having this very bad headache okay body pains okay okay okay so all these symptoms now did it starts with the high body temperature yes and it especially it gets worse at night at night okay okay so you feel like what of during the day how how do you feel during the day during the day  i vomit like i vomited for example today now i vomited like four times okay this morning okay so the headache what part of your head are you have having this headache the my front part of my head front part of your head i will do you describe it like any associated eye pain no okay hmm last month okay so you have not you have not had a missed yeah okay alright thank you very much so aside from this i would like to ermso what have you done since it started so far i have not done i have i have only taken paracetamol you have only taken para and any any any relief with paracetamol just for a short while okay okay okay so  i would just like to ask some other systemic questions to be sure that everything is fine with other systems so from any  neck pain or stiffness no any cough or chest pain no have you been going to have you any urinary symptoms no any diarrhea no okay so like from what you told me so far you said you have been having high body temperature yes there was headache and body pain and you shiver for about a week now am i correct and also this happens more in the evenings okay and there is also been vomiting how about your appetite has your appetite been fine it has reduced reduced appetite okay okay so are you being  i would like to ask for your past medical history now are you been managed for any medical condition no in the past are you on any routine medications no do you drink alcohol no do you smoke cigarettes no have you had surgery before in the past no have you ever been admitted in the hospital no have you ever been transfused with blood no okay  are you married no okay are you sexually active no okay that is that is that is that is okay and what do you do for work i am a student oh okay where do you school unilag okay now i am most i would like to ask for this  consultation are you paying out of pocket or you are under insurance i am paying out of pocket and how are your finances like you know well depend i am depending on my parents okay okay okay alright that is that is very good so  asides this is there any other thing that you think it is important that i might have missed out in the course of this conversation none for now okay alright thank you very much so i would like to examine you now i will do a general examination and for and focus and systemic examinations so well from what you have told me so far let us just you know do a quick recap you said you have been having headache body pains and fever for about a week with vomiting so and this it occurs more in the evenings so i am thinking you are having a condition you are having malaria so but what what would need to do is we will need to confirm we will take blood samples to the lab we will do  malaria parasite test so if it comes out positive we will give you medications for malaria but for now we would give you paracetamol for the fever and the  headache and the body pains so we would also like you to you know bed rest if you need  notes for school to maybe exempt you from school we can also issue that for you do you have any other thing you would like you know like me to help with so i will direct you to the lab where they will do the test and while we await the test results alright have any other thing no alright thank you so much for your time thank you very much alright have a lovely day you too bye</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t xml:space="preserve">hello hello good afternoon good afternoon i am dr yemi and ill be the one attending to you this afternoon all right so can you tell me what brought you to the hospital i have been having um my body has been feeling hot for a while now its very hot oh i am so sorry to hear about that so id like to know more about this so i know how best to you know help you so when did it start started a week ago was this sudden or was it gradual it was gradual and how has it been since then has it progressed has it gotten better it has gotten worse it has gotten worse okay aside from this high body temperature do you have any other associated symptom yes i have been having this very bad headache okay body pains okay and sometimes i shiver okay okay so all these symptoms are do they start with the high body temperature yes and it especially gets worse at night at night okay okay so you feel like what of during the day how how do you feel during the day during the day um i vomit okay i vomited for example today and i vomited like four times this morning okay so the headache what part of your head are you having this headache my front part of my head front part of your head are you describing it like in any as your eye pain no okay i would like to ask you when was your last menstrual period last month okay so you have had a missed period yeah okay alright thank you very much so aside from this id like to so what have you done since it started so far i have not done i have not taken any paracetamol any relief with paracetamol just for a short while okay okay okay so id just like to ask some other systemic questions to be sure that everything is fine with our systems so from any any neck pain or stiffness no any cough or chest pain no have you been um going to have you any urinary symptoms no any diarrhea no okay so like from what you told me so far you said you have been having um high body temperature yes there was headache and um body pain and you shiver for about a week now am i correct and also this happens more in the evenings okay and there is also been vomiting how about appetite i your appetites been fine it does reduced reduced appetite okay okay so are you being me i would like to ask for your past medical history now have you been married for any medical condition no in the past are you on any routine medications no do you drink alcohol no do you smoke cigarettes no have you had surgery before in the past no have you ever been admitted in the hospital no you have been transfused with blood no okay are you married no okay are you sexually active no okay that is that is that is it and what do you do for work i am a student okay where do you go you know i okay now i am most i would like to ask for this consultation are you paying out of pocket or are you under insurance i am paying out of pocket and how are your finances like you know well depend i am depending on my okay okay okay alright that sounds very good so um aside to is it is there any other thing that you think is important that i must have missed out in the because of this conversation none for now okay alright thank you very much so id like to examine you now ill do a general examination and systemic examinations so um well from what you have told me so far let us just you know do a quick recap said you have been having headache body pains and fever for about week were vomiting so and its causing more in the evenings so i am thinking you are having a condition you are having malaria so but what we need to do is we need to confirm well take um blood samples to the lab well do malaria parasite tests so if it comes out positive well give you medications for malaria but for now well give you um paracetamol for the fever and the um headache and the body pains so also like you to you know bed rest if you need um notes for school to maybe exempt you from school we can also issue that for you do you have any other thing would like you know like me to help with so ill direct you to the lab and well do the test and well i wish the test results alright have any other thing no alright thank you so much for your time thank you very much alright have a lovely day you too bye </t>
-        </is>
-      </c>
-      <c r="K3" t="n">
-        <v>0.2537313432835821</v>
-      </c>
-      <c r="L3" t="n">
-        <v>68</v>
+          <t>hello hello good afternoon good afternoon i am doctor yemi and i will be the one attending to you this afternoon alright so can you tell me what brought you to the hospital i have been having my body has been feeling hot for a while now it is very hot oh i am so sorry to hear about that so i would like to know more about this so i would know how best to help you when did it start it started a week ago sorry to hear about that so i would like to know more about this so i would know how best to you know help you so when did it start started a week ago was this sudden onset it was gradual it was gradual and how has it been since then has it progressed has it gotten better it has gotten worse it has gotten worse okay aside from this high body temperature do you have any other associated dead yes i have been having this very bad headache okay body pains okay and sometimes i shiver okay okay so all these symptoms do they start with the high body temperature yes and it especially gets worse at night at night okay okay so you feel like what during the day how do you feel during the day during the day  i vomit like i vomited for example today and i vomited like four times okay okay so the headache what part of your head are you having this headache my front part of my front part of your head i will describe it like in any actual eye pain no okay i would like to ask you  when was your last menstrual period  last morning okay so you have done you have all had the missed period yeah okay all right thank you very much so aside from this i would like to  so what have you done since it started so far i have not done i am i will not take you first with paracetamol just for a short while okay okay okay so  i would just like to ask some other systemic questions to be sure that everything is fine with our systems so from  any  neck pain or stiffness no any cough or chest pain have pain no have you been going to have you any urinary symptoms no any diarrhea no okay so like from what you told me so far you said you have been having high body temperature yes there was headache and body pain and you shivered for about a week now am i correct i correct and also this happens more in the evenings okay and there is also been vomiting how about your appetite are you ever tired of being fine  that is reduced reduced appetite okay okay so are you being me  i would like to ask for your past medical history now i have been married to any medical condition in the past are you on any routine medications  do you drink alcohol do you smoke cigarettes have you had surgery before in the past have you ever been addicted in the hospital no you have been transfused with blood okay  are you married no okay are you sexually active no okay that is that is that is okay and what do you do for work i am a student oh okay where do you school  you know okay now  i would like to ask for this  consultation are you paying out of pocket or yeah under insurance i am paying out of pocket and how are your finances like you know  well depend i am depending on my parents okay okay okay all right that is that is very good so  is there any other thing that you think is important that i must have missed out in the course of this  conversation none for now okay all right thank you very much so i would like to  examine you now i will do a general examination and and systemic examinations so  well from what you have told me so far let us just you know do a quick recap he said you have been having headache body pains and fever for about a week you are vomiting so and it is your because more in the evenings so i am thinking you are having a condition you are having malaria so but what we need to do is we need to confirm we take blood samples to the lab we will do a malaria parasite test so if it comes out positive we will give you medications for malaria but for now we will give you  paracetamol for the fever and the headache and the body pains so i would also like you to you know bed rest if you need notes for school to maybe exempt you from school we can also issue that for you do you have any other thing would like you know like me to help with so i will direct you to the lab where they will do the test and well which the test results all right have any other thing no all right thank you so much for your time all right have a lovely day bye</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>hello hello good afternoon good afternoon i am doctor yemi and i will be the one attending to you this afternoon all right so can you tell me what brought you to the hospital i have been having  my body has been feeling hot for a while now it is very hot oh i am so sorry to hear about that so i would like to know more about this so i know how best to you know help you so when did it start started a week ago was this sudden or was it gradual it was gradual and how has it been since then has it progressed has it gotten better it has gotten worse it has gotten worse okay aside from this high body temperature do you have any other associated symptom yes i have been having this very bad headache okay body pains okay and sometimes i shiver okay okay so all these symptoms are do they start with the high body temperature yes and it especially gets worse at night at night okay okay so you feel like what of during the day how how do you feel during the day during the day  i vomit okay i vomited for example today and i vomited like four times this morning okay so the headache what part of your head are you having this headache my front part of my head front part of your head are you describing it like in any as your eye pain no okay i would like to ask you when was your last menstrual period last month okay so you have had a missed period yeah okay alright thank you very much so aside from this i would like to so what have you done since it started so far i have not done i have not taken any paracetamol any relief with paracetamol just for a short while okay okay okay so i would just like to ask some other systemic questions to be sure that everything is fine with our systems so from any any neck pain or stiffness no any cough or chest pain no have you been  going to have you any urinary symptoms no any diarrhea no okay so like from what you told me so far you said you have been having  high body temperature yes there was headache and  body pain and you shiver for about a week now am i correct and also this happens more in the evenings okay and there is also been vomiting how about appetite i your appetites been fine it does reduced reduced appetite okay okay so are you being me i would like to ask for your past medical history now have you been married for any medical condition no in the past are you on any routine medications no do you drink alcohol no do you smoke cigarettes no have you had surgery before in the past no have you ever been admitted in the hospital no you have been transfused with blood no okay are you married no okay are you sexually active no okay that is that is that is it and what do you do for work i am a student okay where do you go you know i okay now i am most i would like to ask for this consultation are you paying out of pocket or are you under insurance i am paying out of pocket and how are your finances like you know well depend i am depending on my okay okay okay alright that sounds very good so  aside to is it is there any other thing that you think is important that i must have missed out in the because of this conversation none for now okay alright thank you very much so i would like to examine you now i will do a general examination and systemic examinations so  well from what you have told me so far let us just you know do a quick recap said you have been having headache body pains and fever for about week we are vomiting so and it is causing more in the evenings so i am thinking you are having a condition you are having malaria so but what we need to do is we need to confirm we will take  blood samples to the lab we will do malaria parasite tests so if it comes out positive we will give you medications for malaria but for now we will give you  paracetamol for the fever and the  headache and the body pains so also like you to you know bed rest if you need  notes for school to maybe exempt you from school we can also issue that for you do you have any other thing would like you know like me to help with so i will direct you to the lab and we will do the test and well i wish the test results alright have any other thing no alright thank you so much for your time thank you very much alright have a lovely day you too bye</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>hello hello good afternoon good afternoon i am doctor yemi and i will be the one attending to you this afternoon alright so can you tell me what brought you to the hospital i have been having my body has been feeling hot for a while now it is very hot oh i am so sorry to hear about that so i would like to know more about this so i would know how best to you know help you so when did it start started a week ago was it suddenly also that it was gradual it was gradual and how has it been since then has it progressed has it gotten better it has gotten worse it has gotten worse okay aside from this high body temperature do you have any other associated symptoms yes i have been having this very bad headache okay body pains okay and sometimes i shiver okay okay so all these symptoms now this starts with the high body temperature yes and it especially gets worse at night at night okay okay so you feel like what of during the day how do you feel during the day during the day i vomit like i have vomited for example today i vomited like four times this morning okay so the headache what part of your head are you having this headache the front part of my head front part of your head did you describe it like in any associated eye pain no okay i would like to ask you when was your last menstrual period last morning okay so you have not had a missed period yes okay all right thank you very much so aside from this i would like to so what have you done since it started so far i have not done i will not take parasitomol if you need any relief with paracetamol just for a short while okay okay okay so i would just like to ask some other systemic questions to be sure that everything is fine with other systems so from any neck pain or stiffness no any cough or chest pain no have you been going to have you any urinary symptoms no any diarrhea no okay so like from what you told me so far you said you have been having high body temperature yes there was headache and body pain and you shiver for about a week now am i correct and also this happens more in the evenings okay and there is also been vomiting how about appetite appetites been fine reduced reduced appetite okay okay so are you being i would like to ask for your past medical history now have you been married for any medical condition in the past are you on any routine medications no do you drink alcohol no do you smoke cigarettes have you had surgery before in the past no have you ever been admitted in the hospital no have you ever been transfused with blood no okay are you married no okay are you sexually active no okay that is that is that is that is okay and what do you do for work i am a student okay where do you school  you know okay now  who is i would like to ask for this  consultation are you paying out of pocket or yeah under insurance i am paying out of pocket and how are your finances like you know  well depend i am depending on my parents okay okay okay all right that is that is very good so  aside is there any other thing that you think is important that i must have missed out in the course of this  conversation none for now okay all right thank you very much so i would like to  examine you now i will do a general examination and focus and systemic examinations so  well from what you have told me so far let us just you know do a quick recap you said you have been having headache body pains and fever for about a week you are vomiting so and this because more in the evenings so i am thinking you are having a condition you are having malaria so but what we would need to do is we will need to confirm we will take  blood samples to the lab we will do malaria parasite tests so if it comes out positive we will give you medications for malaria but for now we will give you  paracetamol for the fever and the  headache and the body pains so  also like you to you know bed rest if you need notes for school to maybe exempt you from school we can also issue that for you do you have any other thing would like you know like me to help with so i will direct you to the lab where you will do the test and while we await the test results all right have any other thing no all right thank you so much for your time thank you all right have a lovely day bye</t>
+        </is>
       </c>
       <c r="M3" t="n">
-        <v>49</v>
+        <v>0.1988571428571428</v>
       </c>
       <c r="N3" t="n">
-        <v>104</v>
+        <v>65</v>
       </c>
       <c r="O3" t="n">
-        <v>0.1802525832376579</v>
+        <v>53</v>
       </c>
       <c r="P3" t="n">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="Q3" t="n">
-        <v>45</v>
+        <v>0.1325714285714286</v>
       </c>
       <c r="R3" t="n">
-        <v>85</v>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>['right', 'in', 'in', 'or', 'or', 'starts', 'it', 'of', 'how', 'morning', 'ok', 'have', 'the', 'head', 'do', 'you', 'paracetamol', 'only', 'taken', 'para', 'and', 'any', 'any', 'any', 'relief', 'no', 'no', 'no', 'no', 'have', 'erm', 'is', 'ok', 'are', 'asides', 'this', 'for', 'focus', 'and', 'would', 'erm', 'erm', 'you', 'await', 'very', 'much', 'alright', 'you', 'too']</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>['id', 'know', 'how', 'best', 'to', 'help', 'you', 'when', 'did', 'it', 'start', 'it', 'started', 'a', 'week', 'ago', 'sorry', 'to', 'hear', 'about', 'that', 'so', 'id', 'more', 'about', 'this', 'so', 'id', 'know', 'okay', 'and', 'sometimes', 'i', 'in', 'okay', 'id', 'like', 'to', 'ask', 'you', 'um', 'when', 'menstrual', 'period', 'um', 'last', 'period', 'okay', 'um', 'um', 'have', 'pain', 'i', 'correct', 'are', 'you', 'uh', 'um', 'okay', 'um', 'okay', 'um', 'um', 'you', 'um', 'i', 'all', 'all']</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>['all', 'havingerm', 'as', 'i', 'would', 'is', 'ok', 'symptom', 'ok', 'ok', 'ok', 'ok', 'now', 'did', 'it', 'ok', 'ok', 'erm', 'now', 'ok', 'this', 'associated', 'ok', 'hmm', 'month', 'ok', 'not', 'not', 'a', 'ok', 'alright', 'ermso', 'have', 'have', 'only', 'taken', 'have', 'ok', 'ok', 'ok', 'erm', 'other', 'uhm', 'ok', 'shiver', 'ok', 'has', 'your', 'appetite', 'been', 'it', 'has', 'ok', 'ok', 'erm', 'i', 'would', 'are', 'you', 'managed', 'for', 'no', 'admitted', 'ever', 'no', 'ok', 'ok', 'ok', 'that', 'ok', 'unilag', 'ok', 'now', 'i', 'am', 'most', 'erm', 'you', 'ok', 'ok', 'ok', 'alright', 'erm', 'its', 'might', 'ok', 'alright', 'you', 'with', 'this', 'it', 'occurs', 'what', 'well', 'well', 'erm', 'wed', 'wed', 'while', 'we', 'alright', 'alright', 'thank', 'you']</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>['in', 'would', 'or', 'was', 'or', 'it', 'ok', 'have', 'the', 'will', 'do', 'not', 'have', 'only', 'paracetamol', 'you', 'have', 'only', 'taken', 'para', 'and', 'erm', 'your', 'have', 'erm', 'is', 'ok', 'ok', 'erm', 'are', 'ok', 'that', 'is', 'for', 'and', 'focus', 'and', 'you', 'a', 'occurs', 'would', 'erm', 'wed', 'you', 'will']</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>['having', 'okay', 'and', 'sometimes', 'i', 'in', 'as', 'okay', 'i', 'would', 'like', 'to', 'ask', 'you', 'when', 'period', 'um', 'um', 'um', 'go', 'you', 'are', 'it', 'is', 'um', 'um', 'um']</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>['doctor', 'havingerm', 'as', 'is', 'in', 'onset', 'ok', 'ok', 'ok', 'ok', 'ok', 'now', 'did', 'it', 'starts', 'ok', 'ok', 'erm', 'like', 'now', 'ok', 'i', 'describe', 'associated', 'ok', 'hmm', 'month', 'ok', 'so', 'you', 'have', 'not', 'ok', 'ermso', 'i', 'any', 'ok', 'ok', 'ok', 'other', 'uhm', 'ok', 'ok', 'has', 'appetite', 'has', 'ok', 'ok', 'erm', 'are', 'managed', 'ever', 'ok', 'ok', 'ok', 'that', 'oh', 'school', 'unilag', 'ok', 'parents', 'ok', 'ok', 'is', 'erm', 'asides', 'this', 'its', 'might', 'course', 'ok', 'with', 'this', 'it', 'what', 'well', 'test', 'wed', 'erm', 'erm', 'where', 'they', 'while', 'we', 'await']</t>
-        </is>
+        <v>25</v>
+      </c>
+      <c r="S3" t="n">
+        <v>43</v>
+      </c>
+      <c r="T3" t="n">
+        <v>48</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.1257142857142857</v>
+      </c>
+      <c r="V3" t="n">
+        <v>22</v>
+      </c>
+      <c r="W3" t="n">
+        <v>40</v>
+      </c>
+      <c r="X3" t="n">
+        <v>48</v>
       </c>
       <c r="Y3" t="inlineStr">
+        <is>
+          <t>['right', 'in', 'or', 'or', 'starts', 'it', 'of', 'how', 'this', 'morning', 'have', 'the', 'head', 'do', 'you', 'paracetamol', 'only', 'taken', 'para', 'and', 'any', 'any', 'any', 'relief', 'no', 'no', 'no', 'no', 'no', 'have', 'no', 'that', 'is', 'am', 'most', 'i', 'are', 'asides', 'this', 'it', 'for', 'focus', 'and', 'would', 'will', 'will', 'you', 'await', 'very', 'much', 'alright', 'you', 'too']</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>['help', 'when', 'did', 'it', 'start', 'it', 'started', 'a', 'week', 'ago', 'sorry', 'to', 'hear', 'about', 'that', 'so', 'i', 'would', 'like', 'to', 'more', 'about', 'this', 'so', 'i', 'would', 'know', 'how', 'best', 'to', 'you', 'know', 'and', 'sometimes', 'i', 'shiver', 'in', 'i', 'would', 'like', 'to', 'ask', 'you', 'when', 'was', 'menstrual', 'period', 'last', 'period', 'all', 'have', 'pain', 'i', 'correct', 'are', 'you', 'me', 'you', 'all', 'all', 'you', 'it', 'a', 'all', 'all']</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>['all', 'havingerm', 'as', 'in', 'is', 'symptom', 'now', 'did', 'it', 'now', 'associated', 'hmm', 'month', 'not', 'not', 'a', 'alright', 'ermso', 'have', 'have', 'only', 'taken', 'have', 'other', 'shiver', 'has', 'your', 'appetite', 'been', 'it', 'has', 'are', 'you', 'managed', 'for', 'admitted', 'ever', 'unilag', 'you', 'alright', 'might', 'alright', 'you', 'with', 'this', 'it', 'occurs', 'what', 'would', 'we', 'while', 'we', 'alright', 'alright', 'thank', 'you']</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>['would', 'or', 'was', 'or', 'it', 'okay', 'have', 'the', 'will', 'do', 'not', 'you', 'have', 'not', 'have', 'only', 'paracetamol', 'you', 'have', 'only', 'taken', 'para', 'and', 'your', 'have', 'is', 'okay', 'oh', 'are', 'parents', 'that', 'is', 'it', 'for', 'and', 'focus', 'and', 'you', 'would', 'will', 'we', 'would', 'you']</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>['and', 'sometimes', 'i', 'shiver', 'in', 'as', 'i', 'would', 'like', 'to', 'ask', 'you', 'when', 'was', 'menstrual', 'period', 'last', 'period', 'any', 'me', 'go', 'you', 'are', 'it', 'is']</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>['havingerm', 'as', 'in', 'is', 'in', 'onset', 'now', 'did', 'it', 'starts', 'like', 'now', 'i', 'describe', 'associated', 'hmm', 'ermso', 'i', 'any', 'other', 'has', 'appetite', 'has', 'are', 'managed', 'ever', 'that', 'school', 'unilag', 'is', 'asides', 'this', 'might', 'course', 'a', 'week', 'with', 'this', 'it', 'occurs', 'what', 'test', 'would', 'where', 'they', 'while', 'we', 'await']</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>['right', 'or', 'or', 'it', 'it', 'how', 'now', 'okay', 'have', 'my', 'will', 'do', 'paracetamol', 'only', 'taken', 'para', 'and', 'any', 'any', 'your', 'your', 'appetite', 'it', 'has', 'no', 'no', 'oh', 'most', 'are', 'this', 'it', 'for', 'and', 'occurs', 'we', 'would', 'you', 'alright', 'you', 'too']</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>['and', 'sometimes', 'i', 'shiver', 'have', 'in', 'i', 'would', 'like', 'to', 'ask', 'you', 'when', 'was', 'period', 'all', 'you', 'all', 'all', 'you', 'all', 'all']</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>['all', 'havingerm', 'as', 'in', 'is', 'sudden', 'in', 'onset', 'symptom', 'did', 'i', 'hmm', 'month', 'okay', 'so', 'you', 'have', 'not', 'yeah', 'alright', 'ermso', 'have', 'i', 'have', 'only', 'taken', 'have', 'has', 'are', 'managed', 'unilag', 'i', 'am', 'you', 'alright', 'asides', 'might', 'alright', 'with', 'it', 'what', 'test', 'would', 'they', 'alright', 'alright', 'very', 'much']</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
         <is>
           <t xml:space="preserve">     ref_ix  hyp_ix  reference hypothesis operation  index_edit_ops
 0         0       0      hello      hello         =            &lt;NA&gt;
@@ -835,15 +986,15 @@
 3         3       3  afternoon  afternoon         =            &lt;NA&gt;
 4         4       4       good       good         =            &lt;NA&gt;
 ..      ...     ...        ...        ...       ...             ...
-934     866     887     lovely     lovely         =            &lt;NA&gt;
-935     867     888        day        day         =            &lt;NA&gt;
-936     868    &lt;NA&gt;        you          _       del             219
-937     869    &lt;NA&gt;        too          _       del             220
-938     870     889        bye        bye         =            &lt;NA&gt;
-[939 rows x 6 columns]</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
+935     870     884     lovely     lovely         =            &lt;NA&gt;
+936     871     885        day        day         =            &lt;NA&gt;
+937     872    &lt;NA&gt;        you          _       del             172
+938     873    &lt;NA&gt;        too          _       del             173
+939     874     886        bye        bye         =            &lt;NA&gt;
+[940 rows x 6 columns]</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
         <is>
           <t xml:space="preserve">     ref_ix  hyp_ix  reference hypothesis operation  index_edit_ops
 0         0       0      hello      hello         =            &lt;NA&gt;
@@ -852,22 +1003,44 @@
 3         3       3  afternoon  afternoon         =            &lt;NA&gt;
 4         4       4       good       good         =            &lt;NA&gt;
 ..      ...     ...        ...        ...       ...             ...
-893     866     848     lovely     lovely         =            &lt;NA&gt;
-894     867     849        day        day         =            &lt;NA&gt;
-895     868     850        you        you         =            &lt;NA&gt;
-896     869     851        too        too         =            &lt;NA&gt;
-897     870     852        bye        bye         =            &lt;NA&gt;
-[898 rows x 6 columns]</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>hello hello good afternoon good afternoon i am doctor yemi and ill be the one attending to you this afternoon [SUB:all-&gt;alright] [DEL:right] so can you tell me what brought you to the hospital i have been [SUB:havingerm-&gt;having] my body has been feeling hot for a while now [SUB:as-&gt;its] [DEL:in] very hot oh i am so sorry to hear about that so id like to know more about this so [INS:id] [INS:know] [INS:how] [INS:best] [INS:to] [INS:help] [INS:you] [INS:when] [INS:did] [INS:it] [INS:start] [INS:it] [INS:started] [INS:a] [INS:week] [INS:ago] [INS:sorry] [INS:to] [INS:hear] [INS:about] [INS:that] [INS:so] [INS:id] [SUB:i-&gt;like] [SUB:would-&gt;to] know [INS:more] [INS:about] [INS:this] [INS:so] [INS:id] [INS:know] how best to you know help you so when did it start started a week ago was [SUB:is-&gt;this] sudden [DEL:in] onset [DEL:or] it was gradual it was gradual and how has it been since then has it progressed has it gotten better [DEL:or] it has gotten worse it has gotten worse [SUB:ok-&gt;okay] aside from this high body temperature do you have any other associated [SUB:symptom-&gt;dead] yes i have been having this very bad headache [SUB:ok-&gt;okay] body pains [INS:okay] [INS:and] [INS:sometimes] [INS:i] [SUB:ok-&gt;shiver] [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] so all these symptoms [SUB:now-&gt;do] [SUB:did-&gt;they] [SUB:it-&gt;start] [DEL:starts] with the high body temperature yes and it especially [DEL:it] gets worse at night at night [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] so you feel like what [DEL:of] during the day how [DEL:how] do you feel during the day during the day [SUB:erm-&gt;um] i vomit like i vomited for example today [SUB:now-&gt;and] i vomited like four times [SUB:ok-&gt;okay] [SUB:this-&gt;okay] [DEL:morning] [DEL:ok] so the headache what part of your head are you [DEL:have] having this headache [DEL:the] my front part of my [DEL:head] front part of your head i will [DEL:do] [DEL:you] describe it like [INS:in] any [SUB:associated-&gt;actual] eye pain no [INS:okay] [INS:id] [INS:like] [INS:to] [INS:ask] [INS:you] [INS:um] [INS:when] [SUB:ok-&gt;was] [SUB:hmm-&gt;your] last [INS:menstrual] [INS:period] [INS:um] [INS:last] [SUB:month-&gt;morning] [SUB:ok-&gt;okay] so you have [SUB:not-&gt;done] you have [SUB:not-&gt;all] had [SUB:a-&gt;the] missed [INS:period] yeah [INS:okay] [SUB:ok-&gt;all] [SUB:alright-&gt;right] thank you very much so aside from this id like to [INS:um] [SUB:ermso-&gt;so] what have you done since it started so far i have not done i [SUB:have-&gt;am] i [SUB:have-&gt;will] [SUB:only-&gt;not] [SUB:taken-&gt;take] [DEL:paracetamol] you [SUB:have-&gt;first] [DEL:only] [DEL:taken] [DEL:para] [DEL:and] [DEL:any] [DEL:any] [DEL:any] [DEL:relief] with paracetamol just for a short while [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] so [SUB:erm-&gt;um] id just like to ask some other systemic questions to be sure that everything is fine with [SUB:other-&gt;our] systems so from [INS:um] any [SUB:uhm-&gt;um] neck pain or stiffness no any cough or chest pain [INS:have] [INS:pain] no have you been going to have you any urinary symptoms no any diarrhea no [SUB:ok-&gt;okay] so like from what you told me so far you said you have been having high body temperature yes there was headache and body pain and you [SUB:shiver-&gt;shivered] for about a week now am i correct [INS:i] [INS:correct] and also this happens more in the evenings [SUB:ok-&gt;okay] and there is also been vomiting how about your appetite [INS:are] [INS:you] [SUB:has-&gt;ever] [SUB:your-&gt;tired] [SUB:appetite-&gt;of] [SUB:been-&gt;being] fine [INS:uh] [SUB:it-&gt;that] [SUB:has-&gt;is] reduced reduced appetite [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] so are you being [SUB:erm-&gt;me] [SUB:i-&gt;um] [SUB:would-&gt;id] like to ask for your past medical history now [SUB:are-&gt;i] [SUB:you-&gt;have] been [SUB:managed-&gt;married] [SUB:for-&gt;to] any medical condition [DEL:no] in the past are you on any routine medications [SUB:no-&gt;um] do you drink alcohol [DEL:no] do you smoke cigarettes [DEL:no] have you had surgery before in the past [DEL:no] have you ever been [SUB:admitted-&gt;addicted] in the hospital no [DEL:have] you [SUB:ever-&gt;have] been transfused with blood [SUB:no-&gt;okay] [SUB:ok-&gt;um] [DEL:erm] are you married no [SUB:ok-&gt;okay] are you sexually active no [SUB:ok-&gt;okay] that is that is that is [SUB:that-&gt;okay] [DEL:is] [DEL:ok] and what do you do for work i am a student oh [SUB:ok-&gt;okay] where do you school [SUB:unilag-&gt;um] [SUB:ok-&gt;you] [SUB:now-&gt;know] [SUB:i-&gt;okay] [SUB:am-&gt;now] [SUB:most-&gt;um] i would like to ask for this [SUB:erm-&gt;um] consultation are you paying out of pocket or [SUB:you-&gt;yeah] [DEL:are] under insurance i am paying out of pocket and how are your finances like you know [INS:um] well depend i am depending on my parents [INS:okay] [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] [SUB:ok-&gt;all] [SUB:alright-&gt;right] that is that is very good so [SUB:erm-&gt;um] [DEL:asides] [DEL:this] is there any other thing that you think [SUB:its-&gt;is] important that i [SUB:might-&gt;must] have missed out in the course of this [INS:um] conversation none for now [INS:okay] [SUB:ok-&gt;all] [SUB:alright-&gt;right] thank you very much so id like to [INS:um] examine you now ill do a general examination and [DEL:for] and [DEL:focus] [DEL:and] systemic examinations so [INS:um] well from what you have told me so far let us just you know do a quick recap [SUB:you-&gt;he] said you have been having headache body pains and fever for about a week [INS:you] [SUB:with-&gt;are] vomiting so and [SUB:this-&gt;its] [SUB:it-&gt;your] [SUB:occurs-&gt;because] more in the evenings so i am thinking you are having a condition you are having malaria so but what [SUB:what-&gt;we] [DEL:would] need to do is [SUB:well-&gt;we] need to confirm [SUB:well-&gt;we] take blood samples to the lab well do [SUB:erm-&gt;a] malaria parasite test so if it comes out positive well give you medications for malaria but for now [SUB:wed-&gt;well] give you [INS:um] paracetamol for the fever and the [DEL:erm] headache and the body pains so [INS:i] [SUB:wed-&gt;would] also like you to you know bed rest if you need [DEL:erm] notes for school to maybe exempt you from school we can also issue that for you do you have any other thing [DEL:you] would like you know like me to help with so ill direct you to the lab where they will do the test and [SUB:while-&gt;well] [SUB:we-&gt;which] [DEL:await] the test results [INS:all] [SUB:alright-&gt;right] have any other thing no [INS:all] [SUB:alright-&gt;right] thank you so much for your time [SUB:thank-&gt;all] [SUB:you-&gt;right] [DEL:very] [DEL:much] [DEL:alright] have a lovely day [DEL:you] [DEL:too] bye</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>hello hello good afternoon good afternoon i am [SUB:doctor-&gt;dr] yemi and ill be the one attending to you this afternoon all right so can you tell me what brought you to the hospital i have been [INS:having] [SUB:havingerm-&gt;um] my body has been feeling hot for a while now [SUB:as-&gt;its] [DEL:in] very hot oh i am so sorry to hear about that so id like to know more about this so i [DEL:would] know how best to you know help you so when did it start started a week ago was [SUB:is-&gt;this] sudden [SUB:in-&gt;or] [SUB:onset-&gt;was] [DEL:or] it [DEL:was] gradual it was gradual and how has it been since then has it progressed has it gotten better [DEL:or] it has gotten worse it has gotten worse [SUB:ok-&gt;okay] aside from this high body temperature do you have any other associated symptom yes i have been having this very bad headache [SUB:ok-&gt;okay] body pains [INS:okay] [INS:and] [INS:sometimes] [INS:i] [SUB:ok-&gt;shiver] [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] so all these symptoms [SUB:now-&gt;are] [SUB:did-&gt;do] [SUB:it-&gt;they] [SUB:starts-&gt;start] with the high body temperature yes and it especially [DEL:it] gets worse at night at night [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] so you feel like what of during the day how how do you feel during the day during the day [SUB:erm-&gt;um] i vomit [SUB:like-&gt;okay] i vomited for example today [SUB:now-&gt;and] i vomited like four times [DEL:ok] this morning [SUB:ok-&gt;okay] so the headache what part of your head are you [DEL:have] having this headache [DEL:the] my front part of my head front part of your head [SUB:i-&gt;are] [DEL:will] [DEL:do] you [SUB:describe-&gt;describing] it like [INS:in] any [INS:as] [SUB:associated-&gt;your] eye pain no [INS:okay] [INS:i] [INS:would] [INS:like] [INS:to] [INS:ask] [INS:you] [INS:when] [SUB:ok-&gt;was] [SUB:hmm-&gt;your] last [SUB:month-&gt;menstrual] [SUB:ok-&gt;period] [SUB:so-&gt;last] [SUB:you-&gt;month] [SUB:have-&gt;okay] [SUB:not-&gt;so] you have [DEL:not] had a missed [INS:period] yeah [SUB:ok-&gt;okay] alright thank you very much so aside from this id like to [SUB:ermso-&gt;so] what have you done since it started so far i have not done i have [SUB:i-&gt;not] [DEL:have] [DEL:only] taken [DEL:paracetamol] [DEL:you] [DEL:have] [DEL:only] [DEL:taken] [DEL:para] [DEL:and] any [SUB:any-&gt;paracetamol] any relief with paracetamol just for a short while [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] so [DEL:erm] id just like to ask some other systemic questions to be sure that everything is fine with [SUB:other-&gt;our] systems so from any [SUB:uhm-&gt;any] neck pain or stiffness no any cough or chest pain no have you been [INS:um] going to have you any urinary symptoms no any diarrhea no [SUB:ok-&gt;okay] so like from what you told me so far you said you have been having [INS:um] high body temperature yes there was headache and [INS:um] body pain and you shiver for about a week now am i correct and also this happens more in the evenings [SUB:ok-&gt;okay] and there is also been vomiting how about [DEL:your] appetite [SUB:has-&gt;i] your [SUB:appetite-&gt;appetites] been fine it [SUB:has-&gt;does] reduced reduced appetite [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] so are you being [SUB:erm-&gt;me] i would like to ask for your past medical history now [SUB:are-&gt;have] you been [SUB:managed-&gt;married] for any medical condition no in the past are you on any routine medications no do you drink alcohol no do you smoke cigarettes no have you had surgery before in the past no have you ever been admitted in the hospital no [DEL:have] you [SUB:ever-&gt;have] been transfused with blood no [SUB:ok-&gt;okay] [DEL:erm] are you married no [SUB:ok-&gt;okay] are you sexually active no [SUB:ok-&gt;okay] that is that is that is [SUB:that-&gt;it] [DEL:is] [DEL:ok] and what do you do for work i am a student [SUB:oh-&gt;okay] [DEL:ok] where do you [INS:go] [INS:you] [SUB:school-&gt;know] [SUB:unilag-&gt;i] [SUB:ok-&gt;okay] now i am most i would like to ask for this [DEL:erm] consultation are you paying out of pocket or [INS:are] you [DEL:are] under insurance i am paying out of pocket and how are your finances like you know well depend i am depending on my [SUB:parents-&gt;okay] [SUB:ok-&gt;okay] [SUB:ok-&gt;okay] [DEL:ok] alright that [SUB:is-&gt;sounds] [DEL:that] [DEL:is] very good so [SUB:erm-&gt;um] [SUB:asides-&gt;aside] [SUB:this-&gt;to] is [INS:it] [INS:is] there any other thing that you think [SUB:its-&gt;is] important that i [SUB:might-&gt;must] have missed out in the [SUB:course-&gt;because] of this conversation none for now [SUB:ok-&gt;okay] alright thank you very much so id like to examine you now ill do a general examination and [DEL:for] [DEL:and] [DEL:focus] [DEL:and] systemic examinations so [INS:um] well from what you have told me so far let us just you know do a quick recap [DEL:you] said you have been having headache body pains and fever for about [DEL:a] week [SUB:with-&gt;were] vomiting so and [SUB:this-&gt;its] [SUB:it-&gt;causing] [DEL:occurs] more in the evenings so i am thinking you are having a condition you are having malaria so but what [SUB:what-&gt;we] [DEL:would] need to do is [SUB:well-&gt;we] need to confirm well take [INS:um] blood samples to the lab well do [DEL:erm] malaria parasite [SUB:test-&gt;tests] so if it comes out positive well give you medications for malaria but for now [SUB:wed-&gt;well] give you [INS:um] paracetamol for the fever and the [SUB:erm-&gt;um] headache and the body pains so [DEL:wed] also like you to you know bed rest if you need [SUB:erm-&gt;um] notes for school to maybe exempt you from school we can also issue that for you do you have any other thing [DEL:you] would like you know like me to help with so ill direct you to the lab [SUB:where-&gt;and] [SUB:they-&gt;well] [DEL:will] do the test and [SUB:while-&gt;well] [SUB:we-&gt;i] [SUB:await-&gt;wish] the test results alright have any other thing no alright thank you so much for your time thank you very much alright have a lovely day you too bye</t>
+895     870     852     lovely     lovely         =            &lt;NA&gt;
+896     871     853        day        day         =            &lt;NA&gt;
+897     872     854        you        you         =            &lt;NA&gt;
+898     873     855        too        too         =            &lt;NA&gt;
+899     874     856        bye        bye         =            &lt;NA&gt;
+[900 rows x 6 columns]</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     ref_ix  hyp_ix  reference hypothesis operation  index_edit_ops
+0         0       0      hello      hello         =            &lt;NA&gt;
+1         1       1      hello      hello         =            &lt;NA&gt;
+2         2       2       good       good         =            &lt;NA&gt;
+3         3       3  afternoon  afternoon         =            &lt;NA&gt;
+4         4       4       good       good         =            &lt;NA&gt;
+..      ...     ...        ...        ...       ...             ...
+892     870     854     lovely     lovely         =            &lt;NA&gt;
+893     871     855        day        day         =            &lt;NA&gt;
+894     872    &lt;NA&gt;        you          _       del             108
+895     873    &lt;NA&gt;        too          _       del             109
+896     874     856        bye        bye         =            &lt;NA&gt;
+[897 rows x 6 columns]</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>hello hello good afternoon good afternoon i am doctor yemi and i will be the one attending to you this afternoon [SUB:all-&gt;alright] [DEL:right] so can you tell me what brought you to the hospital i have been [SUB:havingerm-&gt;having] my body has been feeling hot for a while now [SUB:as-&gt;it] [SUB:in-&gt;is] very hot oh i am so sorry to hear about that so i would like to know more about this so i would know how best to [INS:help] you [INS:when] [INS:did] [INS:it] [INS:start] [INS:it] [INS:started] [INS:a] [INS:week] [INS:ago] [INS:sorry] [INS:to] [INS:hear] [INS:about] [INS:that] [INS:so] [INS:i] [INS:would] [INS:like] [INS:to] know [INS:more] [INS:about] [INS:this] [INS:so] [INS:i] [INS:would] [INS:know] [INS:how] [INS:best] [INS:to] [INS:you] [INS:know] help you so when did it start started a week ago was [SUB:is-&gt;this] sudden [DEL:in] onset [DEL:or] it was gradual it was gradual and how has it been since then has it progressed has it gotten better [DEL:or] it has gotten worse it has gotten worse okay aside from this high body temperature do you have any other associated [SUB:symptom-&gt;dead] yes i have been having this very bad headache okay body pains okay [INS:and] [INS:sometimes] [INS:i] [INS:shiver] okay okay so all these symptoms [SUB:now-&gt;do] [SUB:did-&gt;they] [SUB:it-&gt;start] [DEL:starts] with the high body temperature yes and it especially [DEL:it] gets worse at night at night okay okay so you feel like what [DEL:of] during the day how [DEL:how] do you feel during the day during the day i vomit like i vomited for example today [SUB:now-&gt;and] i vomited like four times okay [DEL:this] [DEL:morning] okay so the headache what part of your head are you [DEL:have] having this headache [DEL:the] my front part of my [DEL:head] front part of your head i will [DEL:do] [DEL:you] describe it like [INS:in] any [SUB:associated-&gt;actual] eye pain no okay [INS:i] [INS:would] [INS:like] [INS:to] [INS:ask] [INS:you] [INS:when] [INS:was] [SUB:hmm-&gt;your] last [INS:menstrual] [INS:period] [INS:last] [SUB:month-&gt;morning] okay so you have [SUB:not-&gt;done] you have [SUB:not-&gt;all] had [SUB:a-&gt;the] missed [INS:period] yeah okay [INS:all] [SUB:alright-&gt;right] thank you very much so aside from this i would like to [SUB:ermso-&gt;so] what have you done since it started so far i have not done i [SUB:have-&gt;am] i [SUB:have-&gt;will] [SUB:only-&gt;not] [SUB:taken-&gt;take] [DEL:paracetamol] you [SUB:have-&gt;first] [DEL:only] [DEL:taken] [DEL:para] [DEL:and] [DEL:any] [DEL:any] [DEL:any] [DEL:relief] with paracetamol just for a short while okay okay okay so i would just like to ask some other systemic questions to be sure that everything is fine with [SUB:other-&gt;our] systems so from any neck pain or stiffness no any cough or chest pain [INS:have] [INS:pain] no have you been going to have you any urinary symptoms no any diarrhea no okay so like from what you told me so far you said you have been having high body temperature yes there was headache and body pain and you [SUB:shiver-&gt;shivered] for about a week now am i correct [INS:i] [INS:correct] and also this happens more in the evenings okay and there is also been vomiting how about your appetite [INS:are] [INS:you] [SUB:has-&gt;ever] [SUB:your-&gt;tired] [SUB:appetite-&gt;of] [SUB:been-&gt;being] fine [SUB:it-&gt;that] [SUB:has-&gt;is] reduced reduced appetite okay okay so are you being [INS:me] i would like to ask for your past medical history now [SUB:are-&gt;i] [SUB:you-&gt;have] been [SUB:managed-&gt;married] [SUB:for-&gt;to] any medical condition [DEL:no] in the past are you on any routine medications [DEL:no] do you drink alcohol [DEL:no] do you smoke cigarettes [DEL:no] have you had surgery before in the past [DEL:no] have you ever been [SUB:admitted-&gt;addicted] in the hospital no [DEL:have] you [SUB:ever-&gt;have] been transfused with blood [DEL:no] okay are you married no okay are you sexually active no okay that is that is that is [DEL:that] [DEL:is] okay and what do you do for work i am a student oh okay where do you school [INS:you] [SUB:unilag-&gt;know] okay now i [DEL:am] [DEL:most] [DEL:i] would like to ask for this consultation are you paying out of pocket or [SUB:you-&gt;yeah] [DEL:are] under insurance i am paying out of pocket and how are your finances like you know well depend i am depending on my parents okay okay okay [INS:all] [SUB:alright-&gt;right] that is that is very good so [DEL:asides] [DEL:this] is there any other thing that you think [DEL:it] is important that i [SUB:might-&gt;must] have missed out in the course of this conversation none for now okay [INS:all] [SUB:alright-&gt;right] thank you very much so i would like to examine you now i will do a general examination and [DEL:for] and [DEL:focus] [DEL:and] systemic examinations so well from what you have told me so far let us just you know do a quick recap [SUB:you-&gt;he] said you have been having headache body pains and fever for about a week [INS:you] [SUB:with-&gt;are] vomiting so and [INS:it] [SUB:this-&gt;is] [SUB:it-&gt;your] [SUB:occurs-&gt;because] more in the evenings so i am thinking you are having a condition you are having malaria so but what [SUB:what-&gt;we] [DEL:would] need to do is we [DEL:will] need to confirm we [DEL:will] take blood samples to the lab we will do [INS:a] malaria parasite test so if it comes out positive we will give you medications for malaria but for now we [SUB:would-&gt;will] give you paracetamol for the fever and the headache and the body pains so [SUB:we-&gt;i] would also like you to you know bed rest if you need notes for school to maybe exempt you from school we can also issue that for you do you have any other thing [DEL:you] would like you know like me to help with so i will direct you to the lab where they will do the test and [SUB:while-&gt;well] [SUB:we-&gt;which] [DEL:await] the test results [INS:all] [SUB:alright-&gt;right] have any other thing no [INS:all] [SUB:alright-&gt;right] thank you so much for your time [SUB:thank-&gt;all] [SUB:you-&gt;right] [DEL:very] [DEL:much] [DEL:alright] have a lovely day [DEL:you] [DEL:too] bye</t>
+        </is>
+      </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>hello hello good afternoon good afternoon i am doctor yemi and i will be the one attending to you this afternoon all right so can you tell me what brought you to the hospital i have been [SUB:havingerm-&gt;having] my body has been feeling hot for a while now [SUB:as-&gt;it] [SUB:in-&gt;is] very hot oh i am so sorry to hear about that so i would like to know more about this so i [DEL:would] know how best to you know help you so when did it start started a week ago was [SUB:is-&gt;this] sudden [SUB:in-&gt;or] [SUB:onset-&gt;was] [DEL:or] it [DEL:was] gradual it was gradual and how has it been since then has it progressed has it gotten better [DEL:or] it has gotten worse it has gotten worse okay aside from this high body temperature do you have any other associated symptom yes i have been having this very bad headache okay body pains okay [INS:and] [INS:sometimes] [INS:i] [INS:shiver] okay okay so all these symptoms [SUB:now-&gt;are] [SUB:did-&gt;do] [SUB:it-&gt;they] [SUB:starts-&gt;start] with the high body temperature yes and it especially [DEL:it] gets worse at night at night okay okay so you feel like what of during the day how how do you feel during the day during the day i vomit [SUB:like-&gt;okay] i vomited for example today [SUB:now-&gt;and] i vomited like four times [DEL:okay] this morning okay so the headache what part of your head are you [DEL:have] having this headache [DEL:the] my front part of my head front part of your head [SUB:i-&gt;are] [DEL:will] [DEL:do] you [SUB:describe-&gt;describing] it like [INS:in] any [INS:as] [SUB:associated-&gt;your] eye pain no okay [INS:i] [INS:would] [INS:like] [INS:to] [INS:ask] [INS:you] [INS:when] [INS:was] [SUB:hmm-&gt;your] last [INS:menstrual] [INS:period] [INS:last] month okay so you have [DEL:not] [DEL:you] [DEL:have] [DEL:not] had a missed [INS:period] yeah okay alright thank you very much so aside from this i would like to [SUB:ermso-&gt;so] what have you done since it started so far i have not done i have [SUB:i-&gt;not] [DEL:have] [DEL:only] taken [DEL:paracetamol] [DEL:you] [DEL:have] [DEL:only] [DEL:taken] [DEL:para] [DEL:and] any [SUB:any-&gt;paracetamol] any relief with paracetamol just for a short while okay okay okay so i would just like to ask some other systemic questions to be sure that everything is fine with [SUB:other-&gt;our] systems so from any [INS:any] neck pain or stiffness no any cough or chest pain no have you been going to have you any urinary symptoms no any diarrhea no okay so like from what you told me so far you said you have been having high body temperature yes there was headache and body pain and you shiver for about a week now am i correct and also this happens more in the evenings okay and there is also been vomiting how about [DEL:your] appetite [SUB:has-&gt;i] your [SUB:appetite-&gt;appetites] been fine it [SUB:has-&gt;does] reduced reduced appetite okay okay so are you being [INS:me] i would like to ask for your past medical history now [SUB:are-&gt;have] you been [SUB:managed-&gt;married] for any medical condition no in the past are you on any routine medications no do you drink alcohol no do you smoke cigarettes no have you had surgery before in the past no have you ever been admitted in the hospital no [DEL:have] you [SUB:ever-&gt;have] been transfused with blood no okay are you married no okay are you sexually active no okay that is that is that is [SUB:that-&gt;it] [DEL:is] [DEL:okay] and what do you do for work i am a student [DEL:oh] okay where do you [INS:go] [INS:you] [SUB:school-&gt;know] [SUB:unilag-&gt;i] okay now i am most i would like to ask for this consultation are you paying out of pocket or [INS:are] you [DEL:are] under insurance i am paying out of pocket and how are your finances like you know well depend i am depending on my [DEL:parents] okay okay okay alright that [SUB:is-&gt;sounds] [DEL:that] [DEL:is] very good so [SUB:asides-&gt;aside] [SUB:this-&gt;to] is [INS:it] [INS:is] there any other thing that you think [DEL:it] is important that i [SUB:might-&gt;must] have missed out in the [SUB:course-&gt;because] of this conversation none for now okay alright thank you very much so i would like to examine you now i will do a general examination and [DEL:for] [DEL:and] [DEL:focus] [DEL:and] systemic examinations so well from what you have told me so far let us just you know do a quick recap [DEL:you] said you have been having headache body pains and fever for about [SUB:a-&gt;week] [SUB:week-&gt;we] [SUB:with-&gt;are] vomiting so and [SUB:this-&gt;it] [SUB:it-&gt;is] [SUB:occurs-&gt;causing] more in the evenings so i am thinking you are having a condition you are having malaria so but what [SUB:what-&gt;we] [DEL:would] need to do is we [DEL:will] need to confirm we will take blood samples to the lab we will do malaria parasite [SUB:test-&gt;tests] so if it comes out positive we will give you medications for malaria but for now we [SUB:would-&gt;will] give you paracetamol for the fever and the headache and the body pains so [DEL:we] [DEL:would] also like you to you know bed rest if you need notes for school to maybe exempt you from school we can also issue that for you do you have any other thing [DEL:you] would like you know like me to help with so i will direct you to the lab [SUB:where-&gt;and] [SUB:they-&gt;we] will do the test and [SUB:while-&gt;well] [SUB:we-&gt;i] [SUB:await-&gt;wish] the test results alright have any other thing no alright thank you so much for your time thank you very much alright have a lovely day you too bye</t>
+        </is>
+      </c>
+      <c r="AM3" t="inlineStr">
+        <is>
+          <t>hello hello good afternoon good afternoon i am doctor yemi and i will be the one attending to you this afternoon [SUB:all-&gt;alright] [DEL:right] so can you tell me what brought you to the hospital i have been [SUB:havingerm-&gt;having] my body has been feeling hot for a while now [SUB:as-&gt;it] [SUB:in-&gt;is] very hot oh i am so sorry to hear about that so i would like to know more about this so i would know how best to you know help you so when did it start started a week ago was [SUB:is-&gt;it] [SUB:sudden-&gt;suddenly] [SUB:in-&gt;also] [SUB:onset-&gt;that] [DEL:or] it was gradual it was gradual and how has it been since then has it progressed has it gotten better [DEL:or] it has gotten worse it has gotten worse okay aside from this high body temperature do you have any other associated [SUB:symptom-&gt;symptoms] yes i have been having this very bad headache okay body pains okay [INS:and] [INS:sometimes] [INS:i] [INS:shiver] okay okay so all these symptoms now [SUB:did-&gt;this] [DEL:it] starts with the high body temperature yes and it especially [DEL:it] gets worse at night at night okay okay so you feel like what of during the day how [DEL:how] do you feel during the day during the day i vomit like i [INS:have] vomited for example today [DEL:now] i vomited like four times [DEL:okay] this morning okay so the headache what part of your head are you [DEL:have] having this headache the [DEL:my] front part of my head front part of your head [SUB:i-&gt;did] [DEL:will] [DEL:do] you describe it like [INS:in] any associated eye pain no okay [INS:i] [INS:would] [INS:like] [INS:to] [INS:ask] [INS:you] [INS:when] [INS:was] [SUB:hmm-&gt;your] last [SUB:month-&gt;menstrual] [SUB:okay-&gt;period] [SUB:so-&gt;last] [SUB:you-&gt;morning] [SUB:have-&gt;okay] [SUB:not-&gt;so] you have not had a missed [INS:period] [SUB:yeah-&gt;yes] okay [INS:all] [SUB:alright-&gt;right] thank you very much so aside from this i would like to [SUB:ermso-&gt;so] what have you done since it started so far i have not done i [SUB:have-&gt;will] [SUB:i-&gt;not] [SUB:have-&gt;take] [SUB:only-&gt;parasitomol] [SUB:taken-&gt;if] [DEL:paracetamol] you [SUB:have-&gt;need] [DEL:only] [DEL:taken] [DEL:para] [DEL:and] any [DEL:any] [DEL:any] relief with paracetamol just for a short while okay okay okay so i would just like to ask some other systemic questions to be sure that everything is fine with other systems so from any neck pain or stiffness no any cough or chest pain no have you been going to have you any urinary symptoms no any diarrhea no okay so like from what you told me so far you said you have been having high body temperature yes there was headache and body pain and you shiver for about a week now am i correct and also this happens more in the evenings okay and there is also been vomiting how about [DEL:your] appetite [SUB:has-&gt;appetites] [DEL:your] [DEL:appetite] been fine [DEL:it] [DEL:has] reduced reduced appetite okay okay so are you being i would like to ask for your past medical history now [SUB:are-&gt;have] you been [SUB:managed-&gt;married] for any medical condition [DEL:no] in the past are you on any routine medications no do you drink alcohol no do you smoke cigarettes [DEL:no] have you had surgery before in the past no have you ever been admitted in the hospital no have you ever been transfused with blood no okay are you married no okay are you sexually active no okay that is that is that is that is okay and what do you do for work i am a student [DEL:oh] okay where do you school [INS:you] [SUB:unilag-&gt;know] okay now [SUB:i-&gt;who] [SUB:am-&gt;is] [DEL:most] i would like to ask for this consultation are you paying out of pocket or [SUB:you-&gt;yeah] [DEL:are] under insurance i am paying out of pocket and how are your finances like you know well depend i am depending on my parents okay okay okay [INS:all] [SUB:alright-&gt;right] that is that is very good so [SUB:asides-&gt;aside] [DEL:this] is there any other thing that you think [DEL:it] is important that i [SUB:might-&gt;must] have missed out in the course of this conversation none for now okay [INS:all] [SUB:alright-&gt;right] thank you very much so i would like to examine you now i will do a general examination and [DEL:for] [DEL:and] focus and systemic examinations so well from what you have told me so far let us just you know do a quick recap you said you have been having headache body pains and fever for about a week [INS:you] [SUB:with-&gt;are] vomiting so and this [SUB:it-&gt;because] [DEL:occurs] more in the evenings so i am thinking you are having a condition you are having malaria so but what [SUB:what-&gt;we] would need to do is we will need to confirm we will take blood samples to the lab we will do malaria parasite [SUB:test-&gt;tests] so if it comes out positive we will give you medications for malaria but for now we [SUB:would-&gt;will] give you paracetamol for the fever and the headache and the body pains so [DEL:we] [DEL:would] also like you to you know bed rest if you need notes for school to maybe exempt you from school we can also issue that for you do you have any other thing [DEL:you] would like you know like me to help with so i will direct you to the lab where [SUB:they-&gt;you] will do the test and while we await the test results [INS:all] [SUB:alright-&gt;right] have any other thing no [INS:all] [SUB:alright-&gt;right] thank you so much for your time thank you [SUB:very-&gt;all] [SUB:much-&gt;right] [DEL:alright] have a lovely day [DEL:you] [DEL:too] bye</t>
         </is>
       </c>
     </row>
@@ -1001,74 +1174,111 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> would you mind by starting with what brought you in  yeah so over the last week i have just been feeling some symptoms it kind of first started with like a runny nose that was around like five days ago and then it turned into just a lot of congestion like around my nose and like my throat and now over the last two days i have been just feeling so much pressure around my nose and around my jaw so i have been getting a lot of pain there as well  ok is your nose still running  yeah i am still getting some discharge and i also feel like i am getting some dripping at the back of my throat too especially when i wake up  ok and could you describe the discharge is it clear yellow greenish  uh its fairly clear and sometimes like a bit white but like its not like green or yellow  ok uh and have you felt that its difficult to breathe in through either of your nostrils like its obstructed  yeah so at night sometimes i have to like turn because one side of my nose gets difficult to breathe from and then it kind of balances out on the other side so yeah i do have some obstruction  ok and have you had any changes to your sense of smell  yeah so just in the last three days when the congestion got really bad i started losing the ability to smell  ok have you had any changes to your sense of taste  no taste is fine  ok and have you had any cough or sore throat  uh no no cough or sore throat  ok and the symptoms have gone on for five days have you had a period of time where you got better and then got sick again  i did kind of have a runny nose last week as well so probably like eight days ago but then the runny nose discontinued a little bit but really got worse five days ago but all these other symptoms just happened in the last few days  ok and you have pain do you feel it in your jaw or do you feel it in the in the front of your nose  yes i would say mainly over the cheeks it can kind of go near the front of my teeth as well so like i would say like mostly around the cheeks jaws and up to the front of my teeth  ok and do you grind your teeth at all at night or have you had tmj issues before  no nothing like that i think its not so much on and around my teeth its more so just to right below my nose above my teeth and just around my cheeks  ok so no pain in your mouth or anything like that  no not inside my mouth  ok have you had any fevers or chills  uhm i do not think i have had a fever i did feel some chills over the last few days but just very brief episodes  ok and over the last few weeks have you had any weight loss  no  ok and you said you did not have a cough or a sore throat but have you had any wheezing  no wheezing  how about any shortness of breath  uh not shortness of breath just sometimes when my nose gets like really congested i just turn into like a mouth breather but that is about it  i see ok and have you had any chest pain  no no chest pain  alright and any lightheadedness or feeling dizzy  no  ok have you had any nausea or vomiting  nope  any abdominal pain  no  have you had any diarrhea  sorry what was that  have you had any diarrhea  no diarrhea  ok and have you had any urinary problems  uh no  and have you had any rashes or skin changes  no not that i know  ok then how about any muscle aches or joint aches  uh no  ok and have you had any muscle weakness  no  and how has your energy been any fatigue  uhm its been mainly ok just maybe sometimes difficult to get to sleep with all the all the congestion but i do not think my energy has been affected too much no  ok and uh sorry to go back to this i do not think i asked did you notice any discharge from your eyes or any eye redness  not discharge but yeah maybe a little bit of redness  ok have your eyes been itchy  uhm yeah a little bit i would say they have been a bit itchy  ok alright then do you have any medical conditions that you see a physician for regularly  uh just uhm its called dyslipidemia  ok i see and any medications you take for that  just like a statin medication  ok do you take any other medications over the counter prescribed  no other than that i take multivitamins  ok and do you have any allergies to medications or like environmental allergies that might be getting worse  uh no not that i know  ok so you do not experience any symptoms like this when the seasons change  i do not think so i have had this happen to me uh i would say like once before it happened like two years ago it was pretty similar  ok uhm and what was done at that time  at that time it kind of just went away on its own it got better i feel its definitely worse this time but at that time i did not even go to the doctor it kind of just went away  ok i see any recent hospitalizations  no hospitalizations  any surgeries  nope  alright and could you tell me where abouts you are living currently and who you are living with  yeah so i am currently living in an apartment by myself just outside of london  ok and anybody that you have been around who is had any symptoms  uh no not that i know of  ok so no sick contacts and have you traveled anywhere out of the city or province  no i have tried to stay home besides going to work i just work at the grocery store besides that no nowhere else  ok and any of your coworkers have any symptoms or any coworkers being off sick  no were pretty careful right now with the pandemic  i see yeah that is great ok and do you smoke cigarettes  no i quit just a couple of years ago  oh that is great its not easy to quit so that is awesome and do you drink alcohol  just maybe like red wine a couple of times a week  i see ok and do you use any recreational drugs  uh just in a month maybe once or twice i smoke a joint  ok uh and anybody in the family have any lung or heart conditions  no not that i know of  alright and how about any cancer in the family  uh no no cancers  ok i think i that was everything i wanted to ask about today was there any other symptoms or anything else that you wanted to make sure i knew about today  no i think that is all i just did not know if i needed any like medications or if i needed to get tested i just wanted to make sure  yeah so well certainly check your temperature to see if you have a fever and if you do and its high enough that will increase the chance that you have a bacterial sinusitis and if so with some of your symptoms including the discharge obstruction loss of smell and facial pain that all fits the picture for it and also you had a period where you felt a little bit better and then worse again so that might require antibiotics but we will check your temperature and go from there  alright sounds good thank you so much  thank you</t>
+          <t>Would you mind my starting with what brought you in? Yeah, so over the last week, I've just been feeling some symptoms of so it kind of first started with just like I had like a runny nose. And then so that was around like five days ago, and then it turned into just a lot of congestion like around my nose and like my throat. And now over the last two days, I've been just feeling so much pressure around my nose, around my jaw. So I've been getting a lot of pain there as well. Okay. Is your nose still running? Yeah, I'm still getting some discharge. And I also feel like I'm getting some dripping at the back of my throat too, especially when I wake up. Okay. And could you describe the discharge? Is it clear, yellow, greenish? It's fairly clear and sometimes like a bit white, but like it's not like green or yellow. Okay. And have you felt that it's difficult to breathe through either of your nostrils? Like it's obstructed? Yeah, so at night sometimes I have to like turn because one side of my nose gets difficult to breathe from and then it kind of balances out on the other side. So I do have some obstruction. Okay. And have you had any changes to your sense of smell? Yeah, so just in the last three days when the congestion got really bad, I started losing the ability to smell. Okay. Have you had any changes to your sense of taste? No, taste is fine. Okay. And have you had any cough or sore throat? No, no cough or sore throat. Okay. And the symptoms have gone on for five days. Have you had a period of time where you got better and then got sick again? I did. I did kind of have a runny nose last week as well. So probably like eight days ago. But the runny nose has continued a little bit, but really got worse five days ago. But all these other symptoms just happened in the last few days. Okay. And you have pain. Is it you feel it in your jaw or do you feel it in the front of your nose? Yeah, so I would say mainly over the cheeks. It can kind of go near the front of my teeth as well. So like I would say like mostly around the cheeks, jaws, and up to the front of my teeth. Okay. And do you grind your teeth at all at night or have you had like TMJ issues before? No, nothing like that. I think it's not so more like on and around my teeth. It's more so just right below my nose above my teeth and just around my cheeks. Okay. So no pain in your mouth or anything like that. No, not inside my mouth. Okay. Have you had any fevers or chills? I don't think I've had a fever. I did feel some chills over the last few days, but just very brief episodes. Okay. And over the last few weeks, have you had any weight loss? No. Okay. And so you didn't have a cough or a sore throat, but have you had any wheezing? No wheezing. How about any shortness of breath? Not shortness of breath. Just sometimes when my nose gets really congested, I just turn into like a mouth breather, but that's about it. I see, okay. And have you had any chest pain? No, no chest pain. All right. And any lightheadedness or feeling dizzy? No. Okay. Have you had any nausea or vomiting? Nope. Any abdominal pain? Nope. Have you had any diarrhea? Sorry, what was that? Have you had any diarrhea? No diarrhea. Okay. And have you had any urinary problems? Nope. And have you had any rashes or skin changes? No, not that I know of. Okay, and then how about any muscle aches or joint aches? Nope. Okay. And any muscle weakness? No. And how's your energy been? Have you any fatigue? It's been mainly okay. Just maybe sometimes difficult to get to sleep with all the congestion. But I don't think it's my energy's been affected too much, no? Okay. And sorry to go back to this. I don't think I asked. Did you have noticed any discharge from your eyes or any eye redness? Not discharge, but yeah, maybe a little bit of redness. Okay. Have your eyes been itchy? Yeah, a little bit. I would say they have been a bit itchy. Okay. All right. Do you have any medical conditions that you see a physician for regularly? Just I have what's it called? It's called high like dyslipidemia. Okay, I see. And any medications you take for that? Just like a statin medication. Okay. Do you take any other medications over the counter prescribed? No, just other than that, I take multivitamins. Okay. And do you have any allergies to medications or like environmental allergies that might be getting worse? No, not that I know of. Okay, so you don't experience any symptoms like this when the seasons change? I don't think so. I have had this happen to me, I would say, like once before. It happened like two years ago. Yeah. It was pretty similar. Okay. And did you have any time? At that time, it kind of just went away on its own. It got better. Like, I feel it's definitely worse this time. But at that time, I didn't even go to the doctor. I kind of just went away. Okay. I see. And any reasons for hospitalizations? No hospitalizations. No. Any surgeries? Nope. All right. And could you tell me whereabouts you're living currently and who you're living with? Yeah, so I'm currently living in an apartment by myself just outside of London. Okay. And anybody that you've been around who's had any symptoms? No, not that I know of. Okay, so no sick contacts. And have you traveled anywhere out of the city or province? No, I've tried to stay home. Besides going to work, I just work at the grocery store. Besides that, nowhere else. Okay. And any of your co-workers have any symptoms or any co-workers being off sick? No, we're pretty careful right now with the pandemic. I see. Yeah, no, that's great. Okay. And do you smoke cigarettes? No. I quit just a couple years ago. Oh, that's great. It's not, yeah, it's not easy to quit, so that's awesome. And do you drink alcohol? Just maybe like red wine a couple of times a week. I see, okay. And do you use any recreational drugs? Just in a month, maybe once or twice, I smoke a joint. Okay. And anybody in the family have any lung or heart conditions? No, not that I know of. All right. And how about any cancer in the family? No, no, no cancers. Okay. I think that was everything I wanted to ask about today. Was there any other symptoms or anything else that you wanted to make sure I knew about today? No, I think that's all. I just didn't know if I needed any medications or if I needed to get tested. I just wanted to make sure. Yeah, so we'll certainly check your temperature to see if you have a fever. And if you do, and it's high enough, that will increase the chance that you have a bacterial sinusitis with, and if so, with some of your symptoms, including the discharge, obstruction, loss of smell, and facial pain, that all fits the picture for it. And also you had a period where you felt a little bit better and then worse again. So that might require antibiotics, but we will check your temperature and go from there. All right, sounds good. Thank you so much. Thank you.</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>would you mind by starting with what brought you in yeah so over the last week i have just been feeling some symptoms of so it kind of first started with just like i had like a runny nose and then so that was around like five days ago and then it turned into just a lot of congestion like nose and my throat and now over the last two days i have been just feeling so much pressure around my nose around my jaw so i have been getting a lot of pain there as well okay your nose still running yeah i am still getting some discharge and i also feel like i am getting some dripping at the back of my throat too especially when i wake up okay um and uh could you describe the the discharge is it clear yellow yellow greenish its fairly clear and sometimes a bit white but its not green or yellow okay and have you felt that its difficult to breathe through either of your nostrilsrils like its uh obstructed yeah so i at night sometimes i have to like um turn because one side of my nose gets uh difficult to breathe from and then it kind of balances around the other side so i do have some obstruction okay and uh have you had any changes to your sense of smell i do not know have some obstruction okay and have you had any changes to your sense of smell yeah so just in the last three days when the congestion got really bad i started losing the ability to smell okay have you had any changes to your sense of taste no taste is fine okay and have you had any cough or sore throat uh no no cough or sore throat okay um and the symptoms have gone on for five days have you had a period of time where you got better and then got sick again i did i did kind of have a runny nose last week as well so probably like eight days ago and but the runny nose has continued a little bit but really got worse five days ago but all these other symptoms just happened in the last few days okay and you have pain is it you feel it in your jaw or do you feel it in the front of your nose so i would say mainly over the cheeks it can kind of go near the front of my teeth as well so like i would say like mostly around the cheeks jaws and up to the front of my teeth okay and do you grind your teeth at all at night or have you had like tmj issues before no nothing like that i think its not so more like on and around my teeth its more so just right below my nose above my teeth and just around my cheeks okay so no pain in your mouth or anything like that no not inside my mouth okay have you had any fevers or chills i do not think i have had a fever i did feel some chills over the last few days but just very brief episodes okay and over the last few weeks have you had any weight loss no okay and so you did not have a cough or a sore throat but have you had any wheezing no wheezing how about any shortness of breath um not shortness of breath just sometimes when my nose gets like really congested its i i just i just turn into like a mouth breather but that is about it i see okay and have you had um any uh chest pain no no chest pain all right and any lightheadedness or feeling dizzy no okay have you had any nausea or vomiting nope any abdominal pain nope have you had any diarrhea sorry what was that have you had any diarrhea no diarrhea okay and have you had any urinary problems no and have you had any rashes or skin changes no not that i know of okay and then how um any muscle aches or joint aches uh nope okay um and uh have you any muscle weakness no and how is your energy been have you any had any fatigue its been mainly okay just maybe sometimes difficult to get to sleep with all the congestion but i do not think my energys been affected too much no okay and sorry to go back to this i do not think i asked did you notice any discharge from your eyes or any eye redness not discharge but yeah maybe a little bit of redness okay have your eyes been itchy yeah a little bit i would say they have been a bit itchy okay all right do you have any medical conditions that you see a physician for regularly just i have what is it called its called high like dyslipidemia okay i see and any medications you take for that just like a statin medication okay do you take any other medications over the counter prescribed no just other than that i take multivitamins okay and do you have any allergies to medications or maybe like environmental allergies that might be getting worse no not that i know of okay so you do not experience any symptoms like this when the seasons change i do not think so i have had this happen to me i would say like once before it happened like two years ago yeah it was pretty similar okay and did you have any what was done at that time at that time it kind of just went away on its own it got better like i feel its definitely worse this time but at that time i did not even go to the doctor i kind of just went away okay i see any reasons for hospitalizations no hospitalizations no any surgeries nope all right and could you tell me whereabouts you are living currently and who you are living with yeah so i am currently living in an apartment by myself in just outside of london okay and anybody that you have been around who is had any symptoms no not that i know of okay so no sick contacts and have you traveled anywhere out of the city or province no i have tried to stay home besides going to work i just work at the grocery store um besides that nowhere else okay and anybody any of your coworkers have any symptoms or any coworkers been off sick no were pretty careful right now with the pandemic i see yeah no that that is great um okay and do you smoke cigarettes no i see yeah no that that is great um okay and uh do you smoke cigarettes no uh i quit just a couple years ago oh that is great um all right its not yeah its not easy to quit so that is awesome um and uh do you drink alcohol uh just just uh maybe like uh red wine a couple of times a week i see okay and do you use any recreational drugs um just in a month maybe once or twice i smoke a joint okay and anybody in the family have any lung or heart conditions no not that i know of all right and how about any cancer in the family uh no no no cancers okay um i think uh that was everything i wanted to ask about today um was there any other symptoms or um anything else that that you wanted to make sure i knew about today uh no i think that is all i i just did not know if i needed i needed any medications or if i needed to get tested i just wanted to make sure yeah so well certainly check your temperature to see if you have a fever and if you do and its high enough that will increase the chance that you have a bacterial sinusitis and if so with some of your symptoms including the discharge obstruction loss of smell and facial pain that all fits the picture for it and also you you felt you had a period where you felt a little bit better and then worse again so that might require antibiotics but we will yeah check your temperature and go from there alright sounds good thank you so much thank you</t>
+          <t>would you mind by starting with what brought you in yeah so over the last week i have just been feeling some symptoms it kind of first started with like a runny nose that was around like five days ago and then it turned into just a lot of congestion like around my nose and like my throat and now over the last two days i have been just feeling so much pressure around my nose and around my jaw so i have been getting a lot of pain there as well okay is your nose still running yeah i am still getting some discharge and i also feel like i am getting some dripping at the back of my throat too especially when i wake up okay and could you describe the discharge is it clear yellow greenish  it is fairly clear and sometimes like a bit white but like it is not like green or yellow okay  and have you felt that it is difficult to breathe in through either of your nostrils like it is obstructed yeah so at night sometimes i have to like turn because one side of my nose gets difficult to breathe from and then it kind of balances out on the other side so yeah i do have some obstruction okay and have you had any changes to your sense of smell yeah so just in the last three days when the congestion got really bad i started losing the ability to smell okay have you had any changes to your sense of taste no taste is fine okay and have you had any cough or sore throat  no no cough or sore throat okay and the symptoms have gone on for five days have you had a period of time where you got better and then got sick again i did kind of have a runny nose last week as well so probably like eight days ago but then the runny nose discontinued a little bit but really got worse five days ago but all these other symptoms just happened in the last few days okay and you have pain do you feel it in your jaw or do you feel it in the in the front of your nose yes i would say mainly over the cheeks it can kind of go near the front of my teeth as well so like i would say like mostly around the cheeks jaws and up to the front of my teeth okay and do you grind your teeth at all at night or have you had tmj issues before no nothing like that i think it is not so much on and around my teeth it is more so just to right below my nose above my teeth and just around my cheeks okay so no pain in your mouth or anything like that no not inside my mouth okay have you had any fevers or chills  i do not think i have had a fever i did feel some chills over the last few days but just very brief episodes okay and over the last few weeks have you had any weight loss no okay and you said you did not have a cough or a sore throat but have you had any wheezing no wheezing how about any shortness of breath  not shortness of breath just sometimes when my nose gets like really congested i just turn into like a mouth breather but that is about it i see okay and have you had any chest pain no no chest pain alright and any lightheadedness or feeling dizzy no okay have you had any nausea or vomiting nope any abdominal pain no have you had any diarrhea sorry what was that have you had any diarrhea no diarrhea okay and have you had any urinary problems  no and have you had any rashes or skin changes no not that i know okay then how about any muscle aches or joint aches  no okay and have you had any muscle weakness no and how has your energy been any fatigue  it is been mainly okay just maybe sometimes difficult to get to sleep with all the all the congestion but i do not think my energy has been affected too much no okay and  sorry to go back to this i do not think i asked did you notice any discharge from your eyes or any eye redness not discharge but yeah maybe a little bit of redness okay have your eyes been itchy  yeah a little bit i would say they have been a bit itchy okay alright then do you have any medical conditions that you see a physician for regularly  just  its called dyslipidemia okay i see and any medications you take for that just like a statin medication okay do you take any other medications over the counter prescribed no other than that i take multivitamins okay and do you have any allergies to medications or like environmental allergies that might be getting worse  no not that i know okay so you do not experience any symptoms like this when the seasons change i do not think so i have had this happen to me  i would say like once before it happened like two years ago it was pretty similar okay  and what was done at that time at that time it kind of just went away on it is own it got better i feel it is definitely worse this time but at that time i did not even go to the doctor it kind of just went away okay i see any recent hospitalizations no hospitalizations any surgeries nope alright and could you tell me where abouts you are living currently and who you are living with yeah so i am currently living in an apartment by myself just outside of london okay and anybody that you have been around who is had any symptoms  no not that i know of okay so no sick contacts and have you traveled anywhere out of the city or province no i have tried to stay home besides going to work i just work at the grocery store besides that no nowhere else okay and any of your coworkers have any symptoms or any coworkers being off sick no we are pretty careful right now with the pandemic i see yeah that is great okay and do you smoke cigarettes no i quit just a couple of years ago oh that is great it is not easy to quit so that is awesome and do you drink alcohol just maybe like red wine a couple of times a week i see okay and do you use any recreational drugs  just in a month maybe once or twice i smoke a joint okay  and anybody in the family have any lung or heart conditions no not that i know of alright and how about any cancer in the family  no no cancers okay i think i that was everything i wanted to ask about today was there any other symptoms or anything else that you wanted to make sure i knew about today no i think that is all i just did not know if i needed any like medications or if i needed to get tested i just wanted to make sure yeah so well certainly check your temperature to see if you have a fever and if you do and it is high enough that will increase the chance that you have a bacterial sinusitis and if so with some of your symptoms including the discharge obstruction loss of smell and facial pain that all fits the picture for it and also you had a period where you felt a little bit better and then worse again so that might require antibiotics but we will check your temperature and go from there alright sounds good thank you so much thank you</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>would you mind by starting with what brought you in yeah so over the last week i have just been feeling some symptoms of so it kind of first started with just like i had like a runny nose and then so that was around like five days ago and then it turned into just a lot of congestion like around my nose and like my throat and now over the last two days i have been just feeling so much pressure around around my nose around my jaw so having having getting a lot of pain there as well okay is your nose still running yeah i am still getting some discharge and i also feel like i am getting some dripping at the back of my throat too especially when i wake up okay and could you describe the discharge is it clear yellow greenish its fairly clear and sometimes like a bit white but like its not like green or yellow okay and have you felt that its difficult to breathe in through either of your nostrils like its obstructed yeah so i at night sometimes i i have to like turn because one side of my nose gets difficult to breathe from and then it kind of balances around the other side so i do have some obstruction okay and have you had any changes to your sense of smell yeah so just in the last three days when the congestion got really bad i started losing the ability to smell okay have you had any changes to your sense of taste no taste is fine okay and have you had any cough or sore throat no no cough or sore throat okay and the symptoms have gone on for five days have you had a period of time where you got better and then got sick again again i did kind of have a runny nose last week as well so probably like eight days ago and but that the runny nose has continued a little bit but really got worse five days ago but all these other symptoms just happened in the last few days okay and you have pain is it you feel it in your jaw or do you feel it in the in the front of your nose or yes i would say mainly over the cheeks it can kind of go near the front of my teeth as well so i would say like mostly around the cheeks jaws and up to the front of my teeth okay do you grind your teeth at all at night or have you had tmj issues before no nothing like that i think its not so more like on and around my teeth its more so just right below my nose above my teeth and just around my cheeks okay so no pain in your mouth or anything like that no not inside my mouth okay have you had any fevers or chills i do not think i have had a fever i did feel feel some chills over the last few days but just very brief episodes okay and over the last few weeks have you had any weight loss no okay and so you did not have a cough or a sore throat but have you had any wheezing no wheezing how about any shortness of breath not shortness of breath just sometimes in my neck nose gets like really congested its i just i just turn into like a mouth breather but that is about it i see okay and have you had any chest pain no no chest pain all right and any lightheadedness or feeling dizzy no okay have you had any nausea or vomiting nope any abdominal pain no have you had any diarrhea sorry what was that have you had any diarrhea no diarrhea okay and have you had any urinary problems no and have you had any rashes or skin changes no not that i know of okay and then how about any muscle aches or joint aches no no okay and have you any muscle weakness no and how is your energy been have you any fatigue its been mainly okay just maybe sometimes difficult to get to sleep with all the congestion but i do not think my energys been affected too much okay and sorry to go back to this i do not think i asked did you have notice any discharge from your eyes or any eye redness not discharge but yeah maybe a little bit of redness okay have your eyes been itchy yeah a little bit i would say they have been a bit itchy okay all right then do you have any medical conditions that you see a physician for regularly just a i have what is it called its its called high like dyslipidemia okay i see and any medications you take for that just a like a statin medication okay do you take any other medications over the counter or prescribed no just other than that i take multivitamins okay and do you have any allergies to medications or maybe like environmental allergies that might be getting worse no not that i know of okay so you do not experience any symptoms like this when the seasons change i do not i do not think so i have had this happen to me i would say like once before it happened like two years ago yeah it was pretty similar okay and did you have any and what was done at that time at that time it kind of just went away on its own it got better like i feel its definitely worse this time but at that time i did not even go to the doctor i kind of just went away okay i see and have any reasons for hospitalizations no hospitalizations and no any surgeries nope alright and could you tell me whereabouts you are living currently and who you are living with yeah so i am currently living in an apartment by myself and just outside of london okay and anybody that you have been around who is had any symptoms no not that i know of okay so no sick contacts and have you traveled anywhere out of the city or province no i have tried to stay home i besides going to work i just work at the grocery store besides that nowhere else okay and anybody any of your coworkers have any symptoms or any coworkers been off sick no were pretty careful right now with the pandemic i see yeah no that is great okay and do you smoke cigarettes no i quit just a couple of years ago oh that is great its not easy to quit so that is awesome and do you drink alcohol just maybe like red wine a couple of times a week i see okay and do you use any recreational drugs just in a month maybe or twice i smoke a joint okay and anybody in the family have any lung or heart conditions no not that i know of all right and how about any cancer in the family no no no cancers okay i think that was everything wanted to ask about today was there any other symptoms or anything else that you wanted to make sure i knew about today no i think that is all i just did not know if i needed any medications or if i needed to get tested i just wanted to make sure yeah so well certainly check your temperature to see if you have a fever and if you do and its high enough that will increase the chance that you have a bacterial sinusitis with and if so with some of your symptoms including the discharge obstruction loss of smell and facial pain that all fits the picture for it and also you you felt you had a period where you felt a little bit better and then worse again so that might require antibiotics but we will check your temperature and go from there all right sounds good thank you so much thank you</t>
-        </is>
-      </c>
-      <c r="K4" t="n">
-        <v>0.1676602086438152</v>
-      </c>
-      <c r="L4" t="n">
-        <v>126</v>
+          <t>would you mind by starting with what brought you in yeah so over the last week i have just been feeling some symptoms of so it kind of first started with just like i had like a runny nose and then so that was around like five days ago and then it turned into just a lot of congestion like nose and my throat and now over the last two days i have been just feeling so much pressure around my nose around my jaw so i have been getting a lot of pain there as well okay your nose still running yeah i am still getting some discharge and i also feel like i am getting some dripping at the back of my throat too especially when i wake up okay  and  could you describe the the discharge is it clear yellow yellow greenish it is fairly clear and sometimes a bit white but it is not green or yellow okay and have you felt that it is difficult to breathe through either of your nostrilsrils like it is  obstructed yeah so i at night sometimes i have to like  turn because one side of my nose gets  difficult to breathe from and then it kind of balances around the other side so i do have some obstruction okay and  have you had any changes to your sense of smell i do not know have some obstruction okay and have you had any changes to your sense of smell yeah so just in the last three days when the congestion got really bad i started losing the ability to smell okay have you had any changes to your sense of taste no taste is fine okay and have you had any cough or sore throat  no no cough or sore throat okay  and the symptoms have gone on for five days have you had a period of time where you got better and then got sick again i did i did kind of have a runny nose last week as well so probably like eight days ago and but the runny nose has continued a little bit but really got worse five days ago but all these other symptoms just happened in the last few days okay and you have pain is it you feel it in your jaw or do you feel it in the front of your nose so i would say mainly over the cheeks it can kind of go near the front of my teeth as well so like i would say like mostly around the cheeks jaws and up to the front of my teeth okay and do you grind your teeth at all at night or have you had like tmj issues before no nothing like that i think it is not so more like on and around my teeth it is more so just right below my nose above my teeth and just around my cheeks okay so no pain in your mouth or anything like that no not inside my mouth okay have you had any fevers or chills i do not think i have had a fever i did feel some chills over the last few days but just very brief episodes okay and over the last few weeks have you had any weight loss no okay and so you did not have a cough or a sore throat but have you had any wheezing no wheezing how about any shortness of breath  not shortness of breath just sometimes when my nose gets like really congested it is i i just i just turn into like a mouth breather but that is about it i see okay and have you had  any  chest pain no no chest pain all right and any lightheadedness or feeling dizzy no okay have you had any nausea or vomiting nope any abdominal pain nope have you had any diarrhea sorry what was that have you had any diarrhea no diarrhea okay and have you had any urinary problems no and have you had any rashes or skin changes no not that i know of okay and then how  any muscle aches or joint aches  nope okay  and  have you any muscle weakness no and how is your energy been have you any had any fatigue it is been mainly okay just maybe sometimes difficult to get to sleep with all the congestion but i do not think my energys been affected too much no okay and sorry to go back to this i do not think i asked did you notice any discharge from your eyes or any eye redness not discharge but yeah maybe a little bit of redness okay have your eyes been itchy yeah a little bit i would say they have been a bit itchy okay all right do you have any medical conditions that you see a physician for regularly just i have what is it called it is called high like dyslipidemia okay i see and any medications you take for that just like a statin medication okay do you take any other medications over the counter prescribed no just other than that i take multivitamins okay and do you have any allergies to medications or maybe like environmental allergies that might be getting worse no not that i know of okay so you do not experience any symptoms like this when the seasons change i do not think so i have had this happen to me i would say like once before it happened like two years ago yeah it was pretty similar okay and did you have any what was done at that time at that time it kind of just went away on its own it got better like i feel it is definitely worse this time but at that time i did not even go to the doctor i kind of just went away okay i see any reasons for hospitalizations no hospitalizations no any surgeries nope all right and could you tell me whereabouts you are living currently and who you are living with yeah so i am currently living in an apartment by myself in just outside of london okay and anybody that you have been around who is had any symptoms no not that i know of okay so no sick contacts and have you traveled anywhere out of the city or province no i have tried to stay home besides going to work i just work at the grocery store  besides that nowhere else okay and anybody any of your coworkers have any symptoms or any coworkers been off sick no we are pretty careful right now with the pandemic i see yeah no that that is great  okay and do you smoke cigarettes no i see yeah no that that is great  okay and  do you smoke cigarettes no  i quit just a couple years ago oh that is great  all right it is not yeah it is not easy to quit so that is awesome  and  do you drink alcohol  just just  maybe like  red wine a couple of times a week i see okay and do you use any recreational drugs  just in a month maybe once or twice i smoke a joint okay and anybody in the family have any lung or heart conditions no not that i know of all right and how about any cancer in the family  no no no cancers okay  i think  that was everything i wanted to ask about today  was there any other symptoms or  anything else that that you wanted to make sure i knew about today  no i think that is all i i just did not know if i needed i needed any medications or if i needed to get tested i just wanted to make sure yeah so we will certainly check your temperature to see if you have a fever and if you do and it is high enough that will increase the chance that you have a bacterial sinusitis and if so with some of your symptoms including the discharge obstruction loss of smell and facial pain that all fits the picture for it and also you you felt you had a period where you felt a little bit better and then worse again so that might require antibiotics but we will yeah check your temperature and go from there alright sounds good thank you so much thank you</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>would you mind by starting with what brought you in yeah so over the last week i have just been feeling some symptoms of so it kind of first started with just like i had like a runny nose and then so that was around like five days ago and then it turned into just a lot of congestion like around my nose and like my throat and now over the last two days i have been just feeling so much pressure around around my nose around my jaw so having having getting a lot of pain there as well okay is your nose still running yeah i am still getting some discharge and i also feel like i am getting some dripping at the back of my throat too especially when i wake up okay and could you describe the discharge is it clear yellow greenish it is fairly clear and sometimes like a bit white but like it is not like green or yellow okay and have you felt that it is difficult to breathe in through either of your nostrils like it is obstructed yeah so i at night sometimes i i have to like turn because one side of my nose gets difficult to breathe from and then it kind of balances around the other side so i do have some obstruction okay and have you had any changes to your sense of smell yeah so just in the last three days when the congestion got really bad i started losing the ability to smell okay have you had any changes to your sense of taste no taste is fine okay and have you had any cough or sore throat no no cough or sore throat okay and the symptoms have gone on for five days have you had a period of time where you got better and then got sick again again i did kind of have a runny nose last week as well so probably like eight days ago and but that the runny nose has continued a little bit but really got worse five days ago but all these other symptoms just happened in the last few days okay and you have pain is it you feel it in your jaw or do you feel it in the in the front of your nose or yes i would say mainly over the cheeks it can kind of go near the front of my teeth as well so i would say like mostly around the cheeks jaws and up to the front of my teeth okay do you grind your teeth at all at night or have you had tmj issues before no nothing like that i think it is not so more like on and around my teeth it is more so just right below my nose above my teeth and just around my cheeks okay so no pain in your mouth or anything like that no not inside my mouth okay have you had any fevers or chills i do not think i have had a fever i did feel feel some chills over the last few days but just very brief episodes okay and over the last few weeks have you had any weight loss no okay and so you did not have a cough or a sore throat but have you had any wheezing no wheezing how about any shortness of breath not shortness of breath just sometimes in my neck nose gets like really congested it is i just i just turn into like a mouth breather but that is about it i see okay and have you had any chest pain no no chest pain all right and any lightheadedness or feeling dizzy no okay have you had any nausea or vomiting nope any abdominal pain no have you had any diarrhea sorry what was that have you had any diarrhea no diarrhea okay and have you had any urinary problems no and have you had any rashes or skin changes no not that i know of okay and then how about any muscle aches or joint aches no no okay and have you any muscle weakness no and how is your energy been have you any fatigue it is been mainly okay just maybe sometimes difficult to get to sleep with all the congestion but i do not think my energys been affected too much okay and sorry to go back to this i do not think i asked did you have notice any discharge from your eyes or any eye redness not discharge but yeah maybe a little bit of redness okay have your eyes been itchy yeah a little bit i would say they have been a bit itchy okay all right then do you have any medical conditions that you see a physician for regularly just a i have what is it called it is it is called high like dyslipidemia okay i see and any medications you take for that just a like a statin medication okay do you take any other medications over the counter or prescribed no just other than that i take multivitamins okay and do you have any allergies to medications or maybe like environmental allergies that might be getting worse no not that i know of okay so you do not experience any symptoms like this when the seasons change i do not i do not think so i have had this happen to me i would say like once before it happened like two years ago yeah it was pretty similar okay and did you have any and what was done at that time at that time it kind of just went away on its own it got better like i feel it is definitely worse this time but at that time i did not even go to the doctor i kind of just went away okay i see and have any reasons for hospitalizations no hospitalizations and no any surgeries nope alright and could you tell me whereabouts you are living currently and who you are living with yeah so i am currently living in an apartment by myself and just outside of london okay and anybody that you have been around who is had any symptoms no not that i know of okay so no sick contacts and have you traveled anywhere out of the city or province no i have tried to stay home i besides going to work i just work at the grocery store besides that nowhere else okay and anybody any of your coworkers have any symptoms or any coworkers been off sick no we are pretty careful right now with the pandemic i see yeah no that is great okay and do you smoke cigarettes no i quit just a couple of years ago oh that is great it is not easy to quit so that is awesome and do you drink alcohol just maybe like red wine a couple of times a week i see okay and do you use any recreational drugs just in a month maybe or twice i smoke a joint okay and anybody in the family have any lung or heart conditions no not that i know of all right and how about any cancer in the family no no no cancers okay i think that was everything wanted to ask about today was there any other symptoms or anything else that you wanted to make sure i knew about today no i think that is all i just did not know if i needed any medications or if i needed to get tested i just wanted to make sure yeah so we will certainly check your temperature to see if you have a fever and if you do and it is high enough that will increase the chance that you have a bacterial sinusitis with and if so with some of your symptoms including the discharge obstruction loss of smell and facial pain that all fits the picture for it and also you you felt you had a period where you felt a little bit better and then worse again so that might require antibiotics but we will check your temperature and go from there all right sounds good thank you so much thank you</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>would you mind my starting with what brought you in yeah so over the last week i have just been feeling some symptoms of so it kind of first started with just like i had like a runny nose and then so that was around like five days ago and then it turned into just a lot of congestion like around my nose and like my throat and now over the last two days i have been just feeling so much pressure around my nose around my jaw so i have been getting a lot of pain there as well okay is your nose still running yeah i am still getting some discharge and i also feel like i am getting some dripping at the back of my throat too especially when i wake up okay and could you describe the discharge is it clear yellow greenish it is fairly clear and sometimes like a bit white but like it is not like green or yellow okay and have you felt that it is difficult to breathe through either of your nostrils like it is obstructed yeah so at night sometimes i have to like turn because one side of my nose gets difficult to breathe from and then it kind of balances out on the other side so i do have some obstruction okay and have you had any changes to your sense of smell yeah so just in the last three days when the congestion got really bad i started losing the ability to smell okay have you had any changes to your sense of taste no taste is fine okay and have you had any cough or sore throat no no cough or sore throat okay and the symptoms have gone on for five days have you had a period of time where you got better and then got sick again i did i did kind of have a runny nose last week as well so probably like eight days ago but the runny nose has continued a little bit but really got worse five days ago but all these other symptoms just happened in the last few days okay and you have pain is it you feel it in your jaw or do you feel it in the front of your nose yeah so i would say mainly over the cheeks it can kind of go near the front of my teeth as well so like i would say like mostly around the cheeks jaws and up to the front of my teeth okay and do you grind your teeth at all at night or have you had like tmj issues before no nothing like that i think it is not so more like on and around my teeth it is more so just right below my nose above my teeth and just around my cheeks okay so no pain in your mouth or anything like that no not inside my mouth okay have you had any fevers or chills i do not think i have had a fever i did feel some chills over the last few days but just very brief episodes okay and over the last few weeks have you had any weight loss no okay and so you did not have a cough or a sore throat but have you had any wheezing no wheezing how about any shortness of breath not shortness of breath just sometimes when my nose gets really congested i just turn into like a mouth breather but that is about it i see okay and have you had any chest pain no no chest pain all right and any lightheadedness or feeling dizzy no okay have you had any nausea or vomiting nope any abdominal pain nope have you had any diarrhea sorry what was that have you had any diarrhea no diarrhea okay and have you had any urinary problems nope and have you had any rashes or skin changes no not that i know of okay and then how about any muscle aches or joint aches nope okay and any muscle weakness no and how is your energy been have you any fatigue it is been mainly okay just maybe sometimes difficult to get to sleep with all the congestion but i do not think it is my energys been affected too much no okay and sorry to go back to this i do not think i asked did you have noticed any discharge from your eyes or any eye redness not discharge but yeah maybe a little bit of redness okay have your eyes been itchy yeah a little bit i would say they have been a bit itchy okay all right do you have any medical conditions that you see a physician for regularly just i have what is it called it is called high like dyslipidemia okay i see and any medications you take for that just like a statin medication okay do you take any other medications over the counter prescribed no just other than that i take multivitamins okay and do you have any allergies to medications or like environmental allergies that might be getting worse no not that i know of okay so you do not experience any symptoms like this when the seasons change i do not think so i have had this happen to me i would say like once before it happened like two years ago yeah it was pretty similar okay and did you have any time at that time it kind of just went away on its own it got better like i feel it is definitely worse this time but at that time i did not even go to the doctor i kind of just went away okay i see and any reasons for hospitalizations no hospitalizations no any surgeries nope all right and could you tell me whereabouts you are living currently and who you are living with yeah so i am currently living in an apartment by myself just outside of london okay and anybody that you have been around who is had any symptoms no not that i know of okay so no sick contacts and have you traveled anywhere out of the city or province no i have tried to stay home besides going to work i just work at the grocery store besides that nowhere else okay and any of your coworkers have any symptoms or any coworkers being off sick no we are pretty careful right now with the pandemic i see yeah no that is great okay and do you smoke cigarettes no i quit just a couple years ago oh that is great it is not yeah it is not easy to quit so that is awesome and do you drink alcohol just maybe like red wine a couple of times a week i see okay and do you use any recreational drugs just in a month maybe once or twice i smoke a joint okay and anybody in the family have any lung or heart conditions no not that i know of all right and how about any cancer in the family no no no cancers okay i think that was everything i wanted to ask about today was there any other symptoms or anything else that you wanted to make sure i knew about today no i think that is all i just did not know if i needed any medications or if i needed to get tested i just wanted to make sure yeah so we will certainly check your temperature to see if you have a fever and if you do and it is high enough that will increase the chance that you have a bacterial sinusitis with and if so with some of your symptoms including the discharge obstruction loss of smell and facial pain that all fits the picture for it and also you had a period where you felt a little bit better and then worse again so that might require antibiotics but we will check your temperature and go from there all right sounds good thank you so much thank you</t>
+        </is>
       </c>
       <c r="M4" t="n">
-        <v>34</v>
+        <v>0.1176029962546817</v>
       </c>
       <c r="N4" t="n">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="O4" t="n">
-        <v>0.1192250372578241</v>
+        <v>26</v>
       </c>
       <c r="P4" t="n">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="Q4" t="n">
-        <v>33</v>
+        <v>0.08838951310861423</v>
       </c>
       <c r="R4" t="n">
-        <v>60</v>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>['around', 'my', 'like', 'and', 'is', 'uh', 'like', 'like', 'like', 'uh', 'in', 'on', 'then', 'in', 'the', 'to', 'uhm', 'said', 'uh', 'had', 'uhm', 'all', 'the', 'has', 'uh', 'uhm', 'uh', 'uh', 'abouts', 'uh', 'no', 'of', 'uh', 'like']</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>['of', 'so', 'just', 'i', 'had', 'like', 'and', 'then', 'so', 'okay', 'uh', 'the', 'yellow', 'uh', 'i', 'um', 'uh', 'i', 'do', 'have', 'some', 'obstruction', 'okay', 'and', 'uh', 'have', 'you', 'had', 'any', 'changes', 'to', 'your', 'sense', 'of', 'not', 'know', 'okay', 'i', 'did', 'and', 'has', 'is', 'like', 'more', 'its', 'i', 'i', 'just', 'um', 'uh', 'all', 'of', 'okay', 'nope', 'uh', 'have', 'you', 'had', 'any', 'just', 'i', 'have', 'what', 'high', 'like', 'just', 'maybe', 'of', 'yeah', 'okay', 'and', 'did', 'like', 'reasons', 'no', 'all', 'in', 'um', 'anybody', 'no', 'that', 'um', 'see', 'yeah', 'no', 'that', 'that', 'is', 'great', 'um', 'okay', 'and', 'uh', 'do', 'you', 'smoke', 'cigarettes', 'no', 'uh', 'i', 'um', 'all', 'right', 'yeah', 'its', 'not', 'um', 'uh', 'uh', 'just', 'uh', 'uh', 'all', 'no', 'okay', 'um', 'um', 'that', 'uh', 'i', 'i', 'needed', 'you', 'felt', 'you', 'yeah']</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>['ok', 'ok', 'ok', 'nostrils', 'out', 'yeah', 'ok', 'ok', 'ok', 'ok', 'discontinued', 'ok', 'do', 'yes', 'ok', 'much', 'ok', 'ok', 'ok', 'ok', 'you', 'uh', 'ok', 'alright', 'ok', 'no', 'ok', 'ok', 'about', 'no', 'ok', 'has', 'ok', 'energy', 'ok', 'ok', 'ok', 'alright', 'then', 'uh', 'just', 'uhm', 'ok', 'ok', 'ok', 'ok', 'ok', 'uhm', 'and', 'it', 'ok', 'recent', 'alright', 'where', 'ok', 'ok', 'ok', 'being', 'ok', 'ok', 'uh', 'ok', 'alright', 'ok', 'i']</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>['and', 'been', 'uh', 'uh', 'on', 'yeah', 'uh', 'like', 'and', 'to', 'uhm', 'said', 'uh', 'uh', 'had', 'uhm', 'all', 'the', 'has', 'ok', 'uh', 'uhm', 'uh', 'uh', 'abouts', 'uh', 'no', 'uh', 'once', 'uh', 'i', 'i', 'like']</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>['of', 'so', 'just', 'i', 'had', 'like', 'and', 'then', 'so', 'around', 'i', 'i', 'again', 'and', 'has', 'is', 'or', 'more', 'feel', 'neck', 'its', 'i', 'just', 'all', 'of', 'okay', 'have', 'you', 'have', 'okay', 'just', 'a', 'i', 'have', 'what', 'its', 'high', 'like', 'a', 'or', 'just', 'maybe', 'of', 'i', 'do', 'not', 'yeah', 'okay', 'and', 'did', 'you', 'like', 'and', 'have', 'reasons', 'and', 'no', 'and', 'i', 'anybody', 'no', 'all', 'with', 'you', 'felt', 'you', 'all']</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>['i', 'have', 'ok', 'ok', 'ok', 'out', 'ok', 'ok', 'ok', 'ok', 'then', 'discontinued', 'ok', 'do', 'ok', 'much', 'ok', 'ok', 'ok', 'ok', 'you', 'when', 'ok', 'alright', 'ok', 'ok', 'ok', 'uh', 'ok', 'has', 'ok', 'energy', 'no', 'ok', 'ok', 'alright', 'uh', 'just', 'uhm', 'ok', 'ok', 'ok', 'ok', 'ok', 'uhm', 'it', 'ok', 'recent', 'where', 'ok', 'ok', 'ok', 'being', 'ok', 'ok', 'ok', 'alright', 'uh', 'ok', 'alright']</t>
-        </is>
+        <v>76</v>
+      </c>
+      <c r="S4" t="n">
+        <v>20</v>
+      </c>
+      <c r="T4" t="n">
+        <v>22</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.07565543071161049</v>
+      </c>
+      <c r="V4" t="n">
+        <v>51</v>
+      </c>
+      <c r="W4" t="n">
+        <v>22</v>
+      </c>
+      <c r="X4" t="n">
+        <v>28</v>
       </c>
       <c r="Y4" t="inlineStr">
+        <is>
+          <t>['around', 'my', 'like', 'and', 'is', 'like', 'like', 'like', 'in', 'on', 'then', 'in', 'the', 'to', 'said', 'about', 'had', 'all', 'the', 'has', 'is', 'abouts', 'no', 'of', 'i', 'like']</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>['of', 'so', 'just', 'i', 'had', 'like', 'and', 'then', 'so', 'the', 'yellow', 'i', 'i', 'do', 'have', 'some', 'obstruction', 'okay', 'and', 'have', 'you', 'had', 'any', 'changes', 'to', 'your', 'sense', 'of', 'not', 'know', 'i', 'did', 'and', 'has', 'is', 'like', 'more', 'it', 'is', 'i', 'i', 'just', 'all', 'of', 'and', 'have', 'you', 'had', 'any', 'i', 'have', 'what', 'is', 'it', 'is', 'called', 'high', 'like', 'just', 'maybe', 'of', 'yeah', 'did', 'you', 'have', 'any', 'like', 'reasons', 'no', 'all', 'in', 'anybody', 'no', 'that', 'see', 'yeah', 'no', 'that', 'that', 'is', 'great', 'okay', 'and', 'do', 'you', 'smoke', 'cigarettes', 'no', 'i', 'all', 'right', 'yeah', 'it', 'is', 'not', 'just', 'all', 'no', 'that', 'i', 'i', 'needed', 'we', 'you', 'felt', 'you', 'yeah']</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>['nostrils', 'out', 'yeah', 'discontinued', 'do', 'yes', 'much', 'you', 'alright', 'no', 'no', 'has', 'energy', 'alright', 'then', 'its', 'it', 'it', 'recent', 'alright', 'where', 'being', 'alright', 'well']</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>['and', 'been', 'on', 'yeah', 'like', 'and', 'to', 'said', 'had', 'all', 'the', 'has', 'no', 'is', 'abouts', 'no', 'once', 'i', 'i', 'like']</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>['of', 'so', 'just', 'i', 'had', 'like', 'and', 'then', 'so', 'around', 'i', 'i', 'again', 'and', 'has', 'is', 'or', 'more', 'feel', 'neck', 'it', 'is', 'i', 'just', 'all', 'of', 'and', 'no', 'have', 'you', 'have', 'all', 'a', 'i', 'have', 'what', 'is', 'it', 'is', 'it', 'is', 'called', 'high', 'like', 'a', 'or', 'just', 'maybe', 'of', 'i', 'do', 'not', 'yeah', 'did', 'you', 'have', 'any', 'and', 'like', 'and', 'have', 'reasons', 'and', 'no', 'and', 'i', 'anybody', 'no', 'all', 'no', 'we', 'with', 'you', 'felt', 'you', 'all']</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>['i', 'have', 'out', 'then', 'discontinued', 'do', 'much', 'you', 'when', 'alright', 'has', 'energy', 'alright', 'its', 'it', 'it', 'recent', 'where', 'being', 'alright', 'well', 'alright']</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>['and', 'in', 'yeah', 'then', 'in', 'the', 'to', 'said', 'like', 'have', 'you', 'had', 'all', 'the', 'has', 'that', 'is', 'abouts', 'no', 'of', 'i', 'like']</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>['of', 'so', 'just', 'i', 'had', 'like', 'and', 'then', 'so', 'i', 'did', 'has', 'is', 'yeah', 'like', 'more', 'all', 'of', 'and', 'have', 'you', 'it', 'is', 'have', 'i', 'have', 'what', 'is', 'it', 'is', 'called', 'high', 'like', 'just', 'of', 'yeah', 'like', 'and', 'reasons', 'no', 'all', 'no', 'yeah', 'it', 'is', 'not', 'all', 'no', 'we', 'with', 'all']</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>['by', 'discontinued', 'do', 'yes', 'much', 'you', 'alright', 'no', 'no', 'no', 'has', 'energy', 'notice', 'alright', 'then', 'its', 'what', 'was', 'done', 'at', 'it', 'it', 'recent', 'alright', 'where', 'alright', 'well', 'alright']</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
         <is>
           <t xml:space="preserve">      ref_ix  hyp_ix reference hypothesis operation  index_edit_ops
 0          0       0     would      would         =            &lt;NA&gt;
@@ -1077,15 +1287,15 @@
 3          3       3        by         by         =            &lt;NA&gt;
 4          4       4  starting   starting         =            &lt;NA&gt;
 ...      ...     ...       ...        ...       ...             ...
-1463    1337    1429       you        you         =            &lt;NA&gt;
-1464    1338    1430        so         so         =            &lt;NA&gt;
-1465    1339    1431      much       much         =            &lt;NA&gt;
-1466    1340    1432     thank      thank         =            &lt;NA&gt;
-1467    1341    1433       you        you         =            &lt;NA&gt;
-[1468 rows x 6 columns]</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
+1437    1330    1411       you        you         =            &lt;NA&gt;
+1438    1331    1412        so         so         =            &lt;NA&gt;
+1439    1332    1413      much       much         =            &lt;NA&gt;
+1440    1333    1414     thank      thank         =            &lt;NA&gt;
+1441    1334    1415       you        you         =            &lt;NA&gt;
+[1442 rows x 6 columns]</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
         <is>
           <t xml:space="preserve">      ref_ix  hyp_ix reference hypothesis operation  index_edit_ops
 0          0       0     would      would         =            &lt;NA&gt;
@@ -1094,22 +1304,44 @@
 3          3       3        by         by         =            &lt;NA&gt;
 4          4       4  starting   starting         =            &lt;NA&gt;
 ...      ...     ...       ...        ...       ...             ...
-1404    1337    1371       you        you         =            &lt;NA&gt;
-1405    1338    1372        so         so         =            &lt;NA&gt;
-1406    1339    1373      much       much         =            &lt;NA&gt;
-1407    1340    1374     thank      thank         =            &lt;NA&gt;
-1408    1341    1375       you        you         =            &lt;NA&gt;
-[1409 rows x 6 columns]</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>would you mind by starting with what brought you in yeah so over the last week i have just been feeling some symptoms [INS:of] [INS:so] it kind of first started with [INS:just] like [INS:i] [INS:had] [INS:like] a runny nose [INS:and] [INS:then] [INS:so] that was around like five days ago and then it turned into just a lot of congestion like [DEL:around] [DEL:my] nose and [DEL:like] my throat and now over the last two days i have been just feeling so much pressure around my nose [DEL:and] around my jaw so i have been getting a lot of pain there as well [SUB:ok-&gt;okay] [DEL:is] your nose still running yeah i am still getting some discharge and i also feel like i am getting some dripping at the back of my throat too especially when i wake up [INS:okay] [SUB:ok-&gt;um] and [INS:uh] could you describe the [INS:the] discharge is it clear yellow [INS:yellow] greenish [DEL:uh] its fairly clear and sometimes [DEL:like] a bit white but [DEL:like] its not [DEL:like] green or yellow [SUB:ok-&gt;okay] [DEL:uh] and have you felt that its difficult to breathe [DEL:in] through either of your [SUB:nostrils-&gt;nostrilsrils] like its [INS:uh] obstructed yeah so [INS:i] at night sometimes i have to like [INS:um] turn because one side of my nose gets [INS:uh] difficult to breathe from and then it kind of balances [SUB:out-&gt;around] [DEL:on] the other side so [INS:i] [INS:do] [INS:have] [INS:some] [INS:obstruction] [INS:okay] [INS:and] [INS:uh] [INS:have] [INS:you] [INS:had] [INS:any] [INS:changes] [INS:to] [INS:your] [INS:sense] [INS:of] [SUB:yeah-&gt;smell] i do [INS:not] [INS:know] have some obstruction [SUB:ok-&gt;okay] and have you had any changes to your sense of smell yeah so just in the last three days when the congestion got really bad i started losing the ability to smell [SUB:ok-&gt;okay] have you had any changes to your sense of taste no taste is fine [SUB:ok-&gt;okay] and have you had any cough or sore throat uh no no cough or sore throat [INS:okay] [SUB:ok-&gt;um] and the symptoms have gone on for five days have you had a period of time where you got better and then got sick again i did [INS:i] [INS:did] kind of have a runny nose last week as well so probably like eight days ago [INS:and] but [DEL:then] the runny nose [INS:has] [SUB:discontinued-&gt;continued] a little bit but really got worse five days ago but all these other symptoms just happened in the last few days [SUB:ok-&gt;okay] and you have pain [INS:is] [SUB:do-&gt;it] you feel it in your jaw or do you feel it in the [DEL:in] [DEL:the] front of your nose [SUB:yes-&gt;so] i would say mainly over the cheeks it can kind of go near the front of my teeth as well so like i would say like mostly around the cheeks jaws and up to the front of my teeth [SUB:ok-&gt;okay] and do you grind your teeth at all at night or have you had [INS:like] tmj issues before no nothing like that i think its not so [INS:more] [SUB:much-&gt;like] on and around my teeth its more so just [DEL:to] right below my nose above my teeth and just around my cheeks [SUB:ok-&gt;okay] so no pain in your mouth or anything like that no not inside my mouth [SUB:ok-&gt;okay] have you had any fevers or chills [DEL:uhm] i do not think i have had a fever i did feel some chills over the last few days but just very brief episodes [SUB:ok-&gt;okay] and over the last few weeks have you had any weight loss no [SUB:ok-&gt;okay] and [SUB:you-&gt;so] [DEL:said] you did not have a cough or a sore throat but have you had any wheezing no wheezing how about any shortness of breath [SUB:uh-&gt;um] not shortness of breath just sometimes when my nose gets like really congested [INS:its] i [INS:i] just [INS:i] [INS:just] turn into like a mouth breather but that is about it i see [SUB:ok-&gt;okay] and have you had [INS:um] any [INS:uh] chest pain no no chest pain [INS:all] [SUB:alright-&gt;right] and any lightheadedness or feeling dizzy no [SUB:ok-&gt;okay] have you had any nausea or vomiting nope any abdominal pain [SUB:no-&gt;nope] have you had any diarrhea sorry what was that have you had any diarrhea no diarrhea [SUB:ok-&gt;okay] and have you had any urinary problems [DEL:uh] no and have you had any rashes or skin changes no not that i know [INS:of] [INS:okay] [SUB:ok-&gt;and] then how [SUB:about-&gt;um] any muscle aches or joint aches uh [INS:nope] [SUB:no-&gt;okay] [SUB:ok-&gt;um] and [INS:uh] have you [DEL:had] any muscle weakness no and how [SUB:has-&gt;is] your energy been [INS:have] [INS:you] any [INS:had] [INS:any] fatigue [DEL:uhm] its been mainly [SUB:ok-&gt;okay] just maybe sometimes difficult to get to sleep with all the [DEL:all] [DEL:the] congestion but i do not think my [SUB:energy-&gt;energys] [DEL:has] been affected too much no [SUB:ok-&gt;okay] and [DEL:uh] sorry to go back to this i do not think i asked did you notice any discharge from your eyes or any eye redness not discharge but yeah maybe a little bit of redness [SUB:ok-&gt;okay] have your eyes been itchy [DEL:uhm] yeah a little bit i would say they have been a bit itchy [SUB:ok-&gt;okay] [SUB:alright-&gt;all] [SUB:then-&gt;right] do you have any medical conditions that you see a physician for regularly [INS:just] [INS:i] [INS:have] [INS:what] [SUB:uh-&gt;is] [SUB:just-&gt;it] [SUB:uhm-&gt;called] its called [INS:high] [INS:like] dyslipidemia [SUB:ok-&gt;okay] i see and any medications you take for that just like a statin medication [SUB:ok-&gt;okay] do you take any other medications over the counter prescribed no [INS:just] other than that i take multivitamins [SUB:ok-&gt;okay] and do you have any allergies to medications or [INS:maybe] like environmental allergies that might be getting worse [DEL:uh] no not that i know [INS:of] [SUB:ok-&gt;okay] so you do not experience any symptoms like this when the seasons change i do not think so i have had this happen to me [DEL:uh] i would say like once before it happened like two years ago [INS:yeah] it was pretty similar [INS:okay] [INS:and] [INS:did] [SUB:ok-&gt;you] [SUB:uhm-&gt;have] [SUB:and-&gt;any] what was done at that time at that time it kind of just went away on its own it got better [INS:like] i feel its definitely worse this time but at that time i did not even go to the doctor [SUB:it-&gt;i] kind of just went away [SUB:ok-&gt;okay] i see any [INS:reasons] [SUB:recent-&gt;for] hospitalizations no hospitalizations [INS:no] any surgeries nope [INS:all] [SUB:alright-&gt;right] and could you tell me [SUB:where-&gt;whereabouts] [DEL:abouts] you are living currently and who you are living with yeah so i am currently living in an apartment by myself [INS:in] just outside of london [SUB:ok-&gt;okay] and anybody that you have been around who is had any symptoms [DEL:uh] no not that i know of [SUB:ok-&gt;okay] so no sick contacts and have you traveled anywhere out of the city or province no i have tried to stay home besides going to work i just work at the grocery store [INS:um] besides that [DEL:no] nowhere else [SUB:ok-&gt;okay] and [INS:anybody] any of your coworkers have any symptoms or any coworkers [SUB:being-&gt;been] off sick no were pretty careful right now with the pandemic i see yeah [INS:no] that [INS:that] is great [INS:um] [SUB:ok-&gt;okay] and do you smoke cigarettes no i [INS:see] [INS:yeah] [INS:no] [INS:that] [INS:that] [INS:is] [INS:great] [INS:um] [INS:okay] [INS:and] [INS:uh] [INS:do] [INS:you] [INS:smoke] [INS:cigarettes] [INS:no] [INS:uh] [INS:i] quit just a couple [DEL:of] years ago oh that is great [INS:um] [INS:all] [INS:right] its not [INS:yeah] [INS:its] [INS:not] easy to quit so that is awesome [INS:um] and [INS:uh] do you drink alcohol [INS:uh] just [INS:just] [INS:uh] maybe like [INS:uh] red wine a couple of times a week i see [SUB:ok-&gt;okay] and do you use any recreational drugs [SUB:uh-&gt;um] just in a month maybe once or twice i smoke a joint [SUB:ok-&gt;okay] [DEL:uh] and anybody in the family have any lung or heart conditions no not that i know of [INS:all] [SUB:alright-&gt;right] and how about any cancer in the family uh no no [INS:no] cancers [INS:okay] [SUB:ok-&gt;um] i think [SUB:i-&gt;uh] that was everything i wanted to ask about today [INS:um] was there any other symptoms or [INS:um] anything else that [INS:that] you wanted to make sure i knew about today [INS:uh] no i think that is all i [INS:i] just did not know if i needed [INS:i] [INS:needed] any [DEL:like] medications or if i needed to get tested i just wanted to make sure yeah so well certainly check your temperature to see if you have a fever and if you do and its high enough that will increase the chance that you have a bacterial sinusitis and if so with some of your symptoms including the discharge obstruction loss of smell and facial pain that all fits the picture for it and also you [INS:you] [INS:felt] [INS:you] had a period where you felt a little bit better and then worse again so that might require antibiotics but we will [INS:yeah] check your temperature and go from there alright sounds good thank you so much thank you</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>would you mind by starting with what brought you in yeah so over the last week i have just been feeling some symptoms [INS:of] [INS:so] it kind of first started with [INS:just] like [INS:i] [INS:had] [INS:like] a runny nose [INS:and] [INS:then] [INS:so] that was around like five days ago and then it turned into just a lot of congestion like around my nose and like my throat and now over the last two days i have been just feeling so much pressure around [INS:around] my nose [DEL:and] around my jaw so [SUB:i-&gt;having] [SUB:have-&gt;having] [DEL:been] getting a lot of pain there as well [SUB:ok-&gt;okay] is your nose still running yeah i am still getting some discharge and i also feel like i am getting some dripping at the back of my throat too especially when i wake up [SUB:ok-&gt;okay] and could you describe the discharge is it clear yellow greenish [DEL:uh] its fairly clear and sometimes like a bit white but like its not like green or yellow [SUB:ok-&gt;okay] [DEL:uh] and have you felt that its difficult to breathe in through either of your nostrils like its obstructed yeah so [INS:i] at night sometimes i [INS:i] have to like turn because one side of my nose gets difficult to breathe from and then it kind of balances [SUB:out-&gt;around] [DEL:on] the other side so [DEL:yeah] i do have some obstruction [SUB:ok-&gt;okay] and have you had any changes to your sense of smell yeah so just in the last three days when the congestion got really bad i started losing the ability to smell [SUB:ok-&gt;okay] have you had any changes to your sense of taste no taste is fine [SUB:ok-&gt;okay] and have you had any cough or sore throat [DEL:uh] no no cough or sore throat [SUB:ok-&gt;okay] and the symptoms have gone on for five days have you had a period of time where you got better and then got sick again [INS:again] i did kind of have a runny nose last week as well so probably like eight days ago [INS:and] but [SUB:then-&gt;that] the runny nose [INS:has] [SUB:discontinued-&gt;continued] a little bit but really got worse five days ago but all these other symptoms just happened in the last few days [SUB:ok-&gt;okay] and you have pain [INS:is] [SUB:do-&gt;it] you feel it in your jaw or do you feel it in the in the front of your nose [INS:or] yes i would say mainly over the cheeks it can kind of go near the front of my teeth as well so [DEL:like] i would say like mostly around the cheeks jaws and up to the front of my teeth [SUB:ok-&gt;okay] [DEL:and] do you grind your teeth at all at night or have you had tmj issues before no nothing like that i think its not so [INS:more] [SUB:much-&gt;like] on and around my teeth its more so just [DEL:to] right below my nose above my teeth and just around my cheeks [SUB:ok-&gt;okay] so no pain in your mouth or anything like that no not inside my mouth [SUB:ok-&gt;okay] have you had any fevers or chills [DEL:uhm] i do not think i have had a fever i did feel [INS:feel] some chills over the last few days but just very brief episodes [SUB:ok-&gt;okay] and over the last few weeks have you had any weight loss no [SUB:ok-&gt;okay] and [SUB:you-&gt;so] [DEL:said] you did not have a cough or a sore throat but have you had any wheezing no wheezing how about any shortness of breath [DEL:uh] not shortness of breath just sometimes [SUB:when-&gt;in] my [INS:neck] nose gets like really congested [INS:its] i just [INS:i] [INS:just] turn into like a mouth breather but that is about it i see [SUB:ok-&gt;okay] and have you had any chest pain no no chest pain [INS:all] [SUB:alright-&gt;right] and any lightheadedness or feeling dizzy no [SUB:ok-&gt;okay] have you had any nausea or vomiting nope any abdominal pain no have you had any diarrhea sorry what was that have you had any diarrhea no diarrhea [SUB:ok-&gt;okay] and have you had any urinary problems [DEL:uh] no and have you had any rashes or skin changes no not that i know [INS:of] [INS:okay] [SUB:ok-&gt;and] then how about any muscle aches or joint aches [SUB:uh-&gt;no] no [SUB:ok-&gt;okay] and have you [DEL:had] any muscle weakness no and how [SUB:has-&gt;is] your energy been [INS:have] [INS:you] any fatigue [DEL:uhm] its been mainly [SUB:ok-&gt;okay] just maybe sometimes difficult to get to sleep with all the [DEL:all] [DEL:the] congestion but i do not think my [SUB:energy-&gt;energys] [DEL:has] been affected too much [SUB:no-&gt;okay] [DEL:ok] and [DEL:uh] sorry to go back to this i do not think i asked did you [INS:have] notice any discharge from your eyes or any eye redness not discharge but yeah maybe a little bit of redness [SUB:ok-&gt;okay] have your eyes been itchy [DEL:uhm] yeah a little bit i would say they have been a bit itchy [INS:okay] [SUB:ok-&gt;all] [SUB:alright-&gt;right] then do you have any medical conditions that you see a physician for regularly [INS:just] [INS:a] [INS:i] [INS:have] [INS:what] [SUB:uh-&gt;is] [SUB:just-&gt;it] [SUB:uhm-&gt;called] its [INS:its] called [INS:high] [INS:like] dyslipidemia [SUB:ok-&gt;okay] i see and any medications you take for that just [INS:a] like a statin medication [SUB:ok-&gt;okay] do you take any other medications over the counter [INS:or] prescribed no [INS:just] other than that i take multivitamins [SUB:ok-&gt;okay] and do you have any allergies to medications or [INS:maybe] like environmental allergies that might be getting worse [DEL:uh] no not that i know [INS:of] [SUB:ok-&gt;okay] so you do not experience any symptoms like this when the seasons change i do not [INS:i] [INS:do] [INS:not] think so i have had this happen to me [DEL:uh] i would say like once before it happened like two years ago [INS:yeah] it was pretty similar [INS:okay] [INS:and] [INS:did] [INS:you] [SUB:ok-&gt;have] [SUB:uhm-&gt;any] and what was done at that time at that time it kind of just went away on its own it got better [INS:like] i feel its definitely worse this time but at that time i did not even go to the doctor [SUB:it-&gt;i] kind of just went away [SUB:ok-&gt;okay] i see [INS:and] [INS:have] any [INS:reasons] [SUB:recent-&gt;for] hospitalizations no hospitalizations [INS:and] [INS:no] any surgeries nope alright and could you tell me [SUB:where-&gt;whereabouts] [DEL:abouts] you are living currently and who you are living with yeah so i am currently living in an apartment by myself [INS:and] just outside of london [SUB:ok-&gt;okay] and anybody that you have been around who is had any symptoms [DEL:uh] no not that i know of [SUB:ok-&gt;okay] so no sick contacts and have you traveled anywhere out of the city or province no i have tried to stay home [INS:i] besides going to work i just work at the grocery store besides that [DEL:no] nowhere else [SUB:ok-&gt;okay] and [INS:anybody] any of your coworkers have any symptoms or any coworkers [SUB:being-&gt;been] off sick no were pretty careful right now with the pandemic i see yeah [INS:no] that is great [SUB:ok-&gt;okay] and do you smoke cigarettes no i quit just a couple of years ago oh that is great its not easy to quit so that is awesome and do you drink alcohol just maybe like red wine a couple of times a week i see [SUB:ok-&gt;okay] and do you use any recreational drugs [DEL:uh] just in a month maybe [DEL:once] or twice i smoke a joint [SUB:ok-&gt;okay] [DEL:uh] and anybody in the family have any lung or heart conditions no not that i know of [INS:all] [SUB:alright-&gt;right] and how about any cancer in the family [SUB:uh-&gt;no] no no cancers [SUB:ok-&gt;okay] i think [DEL:i] that was everything [DEL:i] wanted to ask about today was there any other symptoms or anything else that you wanted to make sure i knew about today no i think that is all i just did not know if i needed any [DEL:like] medications or if i needed to get tested i just wanted to make sure yeah so well certainly check your temperature to see if you have a fever and if you do and its high enough that will increase the chance that you have a bacterial sinusitis [INS:with] and if so with some of your symptoms including the discharge obstruction loss of smell and facial pain that all fits the picture for it and also you [INS:you] [INS:felt] [INS:you] had a period where you felt a little bit better and then worse again so that might require antibiotics but we will check your temperature and go from there [INS:all] [SUB:alright-&gt;right] sounds good thank you so much thank you</t>
+1406    1330    1386       you        you         =            &lt;NA&gt;
+1407    1331    1387        so         so         =            &lt;NA&gt;
+1408    1332    1388      much       much         =            &lt;NA&gt;
+1409    1333    1389     thank      thank         =            &lt;NA&gt;
+1410    1334    1390       you        you         =            &lt;NA&gt;
+[1411 rows x 6 columns]</t>
+        </is>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      ref_ix  hyp_ix reference hypothesis operation  index_edit_ops
+0          0       0     would      would         =            &lt;NA&gt;
+1          1       1       you        you         =            &lt;NA&gt;
+2          2       2      mind       mind         =            &lt;NA&gt;
+3          3       3        by         my       sub               0
+4          4       4  starting   starting         =            &lt;NA&gt;
+...      ...     ...       ...        ...       ...             ...
+1381    1330    1359       you        you         =            &lt;NA&gt;
+1382    1331    1360        so         so         =            &lt;NA&gt;
+1383    1332    1361      much       much         =            &lt;NA&gt;
+1384    1333    1362     thank      thank         =            &lt;NA&gt;
+1385    1334    1363       you        you         =            &lt;NA&gt;
+[1386 rows x 6 columns]</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>would you mind by starting with what brought you in yeah so over the last week i have just been feeling some symptoms [INS:of] [INS:so] it kind of first started with [INS:just] like [INS:i] [INS:had] [INS:like] a runny nose [INS:and] [INS:then] [INS:so] that was around like five days ago and then it turned into just a lot of congestion like [DEL:around] [DEL:my] nose and [DEL:like] my throat and now over the last two days i have been just feeling so much pressure around my nose [DEL:and] around my jaw so i have been getting a lot of pain there as well okay [DEL:is] your nose still running yeah i am still getting some discharge and i also feel like i am getting some dripping at the back of my throat too especially when i wake up okay and could you describe the [INS:the] discharge is it clear yellow [INS:yellow] greenish it is fairly clear and sometimes [DEL:like] a bit white but [DEL:like] it is not [DEL:like] green or yellow okay and have you felt that it is difficult to breathe [DEL:in] through either of your [SUB:nostrils-&gt;nostrilsrils] like it is obstructed yeah so [INS:i] at night sometimes i have to like turn because one side of my nose gets difficult to breathe from and then it kind of balances [SUB:out-&gt;around] [DEL:on] the other side so [INS:i] [INS:do] [INS:have] [INS:some] [INS:obstruction] [INS:okay] [INS:and] [INS:have] [INS:you] [INS:had] [INS:any] [INS:changes] [INS:to] [INS:your] [INS:sense] [INS:of] [SUB:yeah-&gt;smell] i do [INS:not] [INS:know] have some obstruction okay and have you had any changes to your sense of smell yeah so just in the last three days when the congestion got really bad i started losing the ability to smell okay have you had any changes to your sense of taste no taste is fine okay and have you had any cough or sore throat no no cough or sore throat okay and the symptoms have gone on for five days have you had a period of time where you got better and then got sick again i did [INS:i] [INS:did] kind of have a runny nose last week as well so probably like eight days ago [INS:and] but [DEL:then] the runny nose [INS:has] [SUB:discontinued-&gt;continued] a little bit but really got worse five days ago but all these other symptoms just happened in the last few days okay and you have pain [INS:is] [SUB:do-&gt;it] you feel it in your jaw or do you feel it in the [DEL:in] [DEL:the] front of your nose [SUB:yes-&gt;so] i would say mainly over the cheeks it can kind of go near the front of my teeth as well so like i would say like mostly around the cheeks jaws and up to the front of my teeth okay and do you grind your teeth at all at night or have you had [INS:like] tmj issues before no nothing like that i think it is not so [INS:more] [SUB:much-&gt;like] on and around my teeth it is more so just [DEL:to] right below my nose above my teeth and just around my cheeks okay so no pain in your mouth or anything like that no not inside my mouth okay have you had any fevers or chills i do not think i have had a fever i did feel some chills over the last few days but just very brief episodes okay and over the last few weeks have you had any weight loss no okay and [SUB:you-&gt;so] [DEL:said] you did not have a cough or a sore throat but have you had any wheezing no wheezing how about any shortness of breath not shortness of breath just sometimes when my nose gets like really congested [INS:it] [INS:is] i [INS:i] just [INS:i] [INS:just] turn into like a mouth breather but that is about it i see okay and have you had any chest pain no no chest pain [INS:all] [SUB:alright-&gt;right] and any lightheadedness or feeling dizzy no okay have you had any nausea or vomiting nope any abdominal pain [SUB:no-&gt;nope] have you had any diarrhea sorry what was that have you had any diarrhea no diarrhea okay and have you had any urinary problems no and have you had any rashes or skin changes no not that i know [INS:of] okay [INS:and] then how [DEL:about] any muscle aches or joint aches [SUB:no-&gt;nope] okay and have you [DEL:had] any muscle weakness no and how [SUB:has-&gt;is] your energy been [INS:have] [INS:you] any [INS:had] [INS:any] fatigue it is been mainly okay just maybe sometimes difficult to get to sleep with all the [DEL:all] [DEL:the] congestion but i do not think my [SUB:energy-&gt;energys] [DEL:has] been affected too much no okay and sorry to go back to this i do not think i asked did you notice any discharge from your eyes or any eye redness not discharge but yeah maybe a little bit of redness okay have your eyes been itchy yeah a little bit i would say they have been a bit itchy okay [SUB:alright-&gt;all] [SUB:then-&gt;right] do you have any medical conditions that you see a physician for regularly just [INS:i] [INS:have] [INS:what] [INS:is] [SUB:its-&gt;it] called [INS:it] [INS:is] [INS:called] [INS:high] [INS:like] dyslipidemia okay i see and any medications you take for that just like a statin medication okay do you take any other medications over the counter prescribed no [INS:just] other than that i take multivitamins okay and do you have any allergies to medications or [INS:maybe] like environmental allergies that might be getting worse no not that i know [INS:of] okay so you do not experience any symptoms like this when the seasons change i do not think so i have had this happen to me i would say like once before it happened like two years ago [INS:yeah] it was pretty similar okay and [INS:did] [INS:you] [INS:have] [INS:any] what was done at that time at that time it kind of just went away on [SUB:it-&gt;its] [DEL:is] own it got better [INS:like] i feel it is definitely worse this time but at that time i did not even go to the doctor [SUB:it-&gt;i] kind of just went away okay i see any [INS:reasons] [SUB:recent-&gt;for] hospitalizations no hospitalizations [INS:no] any surgeries nope [INS:all] [SUB:alright-&gt;right] and could you tell me [SUB:where-&gt;whereabouts] [DEL:abouts] you are living currently and who you are living with yeah so i am currently living in an apartment by myself [INS:in] just outside of london okay and anybody that you have been around who is had any symptoms no not that i know of okay so no sick contacts and have you traveled anywhere out of the city or province no i have tried to stay home besides going to work i just work at the grocery store besides that [DEL:no] nowhere else okay and [INS:anybody] any of your coworkers have any symptoms or any coworkers [SUB:being-&gt;been] off sick no we are pretty careful right now with the pandemic i see yeah [INS:no] that [INS:that] is great okay and do you smoke cigarettes no i [INS:see] [INS:yeah] [INS:no] [INS:that] [INS:that] [INS:is] [INS:great] [INS:okay] [INS:and] [INS:do] [INS:you] [INS:smoke] [INS:cigarettes] [INS:no] [INS:i] quit just a couple [DEL:of] years ago oh that is great [INS:all] [INS:right] it is not [INS:yeah] [INS:it] [INS:is] [INS:not] easy to quit so that is awesome and do you drink alcohol just [INS:just] maybe like red wine a couple of times a week i see okay and do you use any recreational drugs just in a month maybe once or twice i smoke a joint okay and anybody in the family have any lung or heart conditions no not that i know of [INS:all] [SUB:alright-&gt;right] and how about any cancer in the family no no [INS:no] cancers okay i think [DEL:i] that was everything i wanted to ask about today was there any other symptoms or anything else that [INS:that] you wanted to make sure i knew about today no i think that is all i [INS:i] just did not know if i needed [INS:i] [INS:needed] any [DEL:like] medications or if i needed to get tested i just wanted to make sure yeah so [INS:we] [SUB:well-&gt;will] certainly check your temperature to see if you have a fever and if you do and it is high enough that will increase the chance that you have a bacterial sinusitis and if so with some of your symptoms including the discharge obstruction loss of smell and facial pain that all fits the picture for it and also you [INS:you] [INS:felt] [INS:you] had a period where you felt a little bit better and then worse again so that might require antibiotics but we will [INS:yeah] check your temperature and go from there alright sounds good thank you so much thank you</t>
+        </is>
+      </c>
+      <c r="AL4" t="inlineStr">
+        <is>
+          <t>would you mind by starting with what brought you in yeah so over the last week i have just been feeling some symptoms [INS:of] [INS:so] it kind of first started with [INS:just] like [INS:i] [INS:had] [INS:like] a runny nose [INS:and] [INS:then] [INS:so] that was around like five days ago and then it turned into just a lot of congestion like around my nose and like my throat and now over the last two days i have been just feeling so much pressure around [INS:around] my nose [DEL:and] around my jaw so [SUB:i-&gt;having] [SUB:have-&gt;having] [DEL:been] getting a lot of pain there as well okay is your nose still running yeah i am still getting some discharge and i also feel like i am getting some dripping at the back of my throat too especially when i wake up okay and could you describe the discharge is it clear yellow greenish it is fairly clear and sometimes like a bit white but like it is not like green or yellow okay and have you felt that it is difficult to breathe in through either of your nostrils like it is obstructed yeah so [INS:i] at night sometimes i [INS:i] have to like turn because one side of my nose gets difficult to breathe from and then it kind of balances [SUB:out-&gt;around] [DEL:on] the other side so [DEL:yeah] i do have some obstruction okay and have you had any changes to your sense of smell yeah so just in the last three days when the congestion got really bad i started losing the ability to smell okay have you had any changes to your sense of taste no taste is fine okay and have you had any cough or sore throat no no cough or sore throat okay and the symptoms have gone on for five days have you had a period of time where you got better and then got sick again [INS:again] i did kind of have a runny nose last week as well so probably like eight days ago [INS:and] but [SUB:then-&gt;that] the runny nose [INS:has] [SUB:discontinued-&gt;continued] a little bit but really got worse five days ago but all these other symptoms just happened in the last few days okay and you have pain [INS:is] [SUB:do-&gt;it] you feel it in your jaw or do you feel it in the in the front of your nose [INS:or] yes i would say mainly over the cheeks it can kind of go near the front of my teeth as well so [DEL:like] i would say like mostly around the cheeks jaws and up to the front of my teeth okay [DEL:and] do you grind your teeth at all at night or have you had tmj issues before no nothing like that i think it is not so [INS:more] [SUB:much-&gt;like] on and around my teeth it is more so just [DEL:to] right below my nose above my teeth and just around my cheeks okay so no pain in your mouth or anything like that no not inside my mouth okay have you had any fevers or chills i do not think i have had a fever i did feel [INS:feel] some chills over the last few days but just very brief episodes okay and over the last few weeks have you had any weight loss no okay and [SUB:you-&gt;so] [DEL:said] you did not have a cough or a sore throat but have you had any wheezing no wheezing how about any shortness of breath not shortness of breath just sometimes [SUB:when-&gt;in] my [INS:neck] nose gets like really congested [INS:it] [INS:is] i just [INS:i] [INS:just] turn into like a mouth breather but that is about it i see okay and have you had any chest pain no no chest pain [INS:all] [SUB:alright-&gt;right] and any lightheadedness or feeling dizzy no okay have you had any nausea or vomiting nope any abdominal pain no have you had any diarrhea sorry what was that have you had any diarrhea no diarrhea okay and have you had any urinary problems no and have you had any rashes or skin changes no not that i know [INS:of] okay [INS:and] then how about any muscle aches or joint aches no [INS:no] okay and have you [DEL:had] any muscle weakness no and how [SUB:has-&gt;is] your energy been [INS:have] [INS:you] any fatigue it is been mainly okay just maybe sometimes difficult to get to sleep with all the [DEL:all] [DEL:the] congestion but i do not think my [SUB:energy-&gt;energys] [DEL:has] been affected too much [DEL:no] okay and sorry to go back to this i do not think i asked did you [INS:have] notice any discharge from your eyes or any eye redness not discharge but yeah maybe a little bit of redness okay have your eyes been itchy yeah a little bit i would say they have been a bit itchy okay [INS:all] [SUB:alright-&gt;right] then do you have any medical conditions that you see a physician for regularly just [INS:a] [INS:i] [INS:have] [INS:what] [INS:is] [SUB:its-&gt;it] called [INS:it] [INS:is] [INS:it] [INS:is] [INS:called] [INS:high] [INS:like] dyslipidemia okay i see and any medications you take for that just [INS:a] like a statin medication okay do you take any other medications over the counter [INS:or] prescribed no [INS:just] other than that i take multivitamins okay and do you have any allergies to medications or [INS:maybe] like environmental allergies that might be getting worse no not that i know [INS:of] okay so you do not experience any symptoms like this when the seasons change i do not [INS:i] [INS:do] [INS:not] think so i have had this happen to me i would say like once before it happened like two years ago [INS:yeah] it was pretty similar okay and [INS:did] [INS:you] [INS:have] [INS:any] [INS:and] what was done at that time at that time it kind of just went away on [SUB:it-&gt;its] [DEL:is] own it got better [INS:like] i feel it is definitely worse this time but at that time i did not even go to the doctor [SUB:it-&gt;i] kind of just went away okay i see [INS:and] [INS:have] any [INS:reasons] [SUB:recent-&gt;for] hospitalizations no hospitalizations [INS:and] [INS:no] any surgeries nope alright and could you tell me [SUB:where-&gt;whereabouts] [DEL:abouts] you are living currently and who you are living with yeah so i am currently living in an apartment by myself [INS:and] just outside of london okay and anybody that you have been around who is had any symptoms no not that i know of okay so no sick contacts and have you traveled anywhere out of the city or province no i have tried to stay home [INS:i] besides going to work i just work at the grocery store besides that [DEL:no] nowhere else okay and [INS:anybody] any of your coworkers have any symptoms or any coworkers [SUB:being-&gt;been] off sick no we are pretty careful right now with the pandemic i see yeah [INS:no] that is great okay and do you smoke cigarettes no i quit just a couple of years ago oh that is great it is not easy to quit so that is awesome and do you drink alcohol just maybe like red wine a couple of times a week i see okay and do you use any recreational drugs just in a month maybe [DEL:once] or twice i smoke a joint okay and anybody in the family have any lung or heart conditions no not that i know of [INS:all] [SUB:alright-&gt;right] and how about any cancer in the family no no [INS:no] cancers okay i think [DEL:i] that was everything [DEL:i] wanted to ask about today was there any other symptoms or anything else that you wanted to make sure i knew about today no i think that is all i just did not know if i needed any [DEL:like] medications or if i needed to get tested i just wanted to make sure yeah so [INS:we] [SUB:well-&gt;will] certainly check your temperature to see if you have a fever and if you do and it is high enough that will increase the chance that you have a bacterial sinusitis [INS:with] and if so with some of your symptoms including the discharge obstruction loss of smell and facial pain that all fits the picture for it and also you [INS:you] [INS:felt] [INS:you] had a period where you felt a little bit better and then worse again so that might require antibiotics but we will check your temperature and go from there [INS:all] [SUB:alright-&gt;right] sounds good thank you so much thank you</t>
+        </is>
+      </c>
+      <c r="AM4" t="inlineStr">
+        <is>
+          <t>would you mind [SUB:by-&gt;my] starting with what brought you in yeah so over the last week i have just been feeling some symptoms [INS:of] [INS:so] it kind of first started with [INS:just] like [INS:i] [INS:had] [INS:like] a runny nose [INS:and] [INS:then] [INS:so] that was around like five days ago and then it turned into just a lot of congestion like around my nose and like my throat and now over the last two days i have been just feeling so much pressure around my nose [DEL:and] around my jaw so i have been getting a lot of pain there as well okay is your nose still running yeah i am still getting some discharge and i also feel like i am getting some dripping at the back of my throat too especially when i wake up okay and could you describe the discharge is it clear yellow greenish it is fairly clear and sometimes like a bit white but like it is not like green or yellow okay and have you felt that it is difficult to breathe [DEL:in] through either of your nostrils like it is obstructed yeah so at night sometimes i have to like turn because one side of my nose gets difficult to breathe from and then it kind of balances out on the other side so [DEL:yeah] i do have some obstruction okay and have you had any changes to your sense of smell yeah so just in the last three days when the congestion got really bad i started losing the ability to smell okay have you had any changes to your sense of taste no taste is fine okay and have you had any cough or sore throat no no cough or sore throat okay and the symptoms have gone on for five days have you had a period of time where you got better and then got sick again i did [INS:i] [INS:did] kind of have a runny nose last week as well so probably like eight days ago but [DEL:then] the runny nose [INS:has] [SUB:discontinued-&gt;continued] a little bit but really got worse five days ago but all these other symptoms just happened in the last few days okay and you have pain [INS:is] [SUB:do-&gt;it] you feel it in your jaw or do you feel it in the [DEL:in] [DEL:the] front of your nose [INS:yeah] [SUB:yes-&gt;so] i would say mainly over the cheeks it can kind of go near the front of my teeth as well so like i would say like mostly around the cheeks jaws and up to the front of my teeth okay and do you grind your teeth at all at night or have you had [INS:like] tmj issues before no nothing like that i think it is not so [INS:more] [SUB:much-&gt;like] on and around my teeth it is more so just [DEL:to] right below my nose above my teeth and just around my cheeks okay so no pain in your mouth or anything like that no not inside my mouth okay have you had any fevers or chills i do not think i have had a fever i did feel some chills over the last few days but just very brief episodes okay and over the last few weeks have you had any weight loss no okay and [SUB:you-&gt;so] [DEL:said] you did not have a cough or a sore throat but have you had any wheezing no wheezing how about any shortness of breath not shortness of breath just sometimes when my nose gets [DEL:like] really congested i just turn into like a mouth breather but that is about it i see okay and have you had any chest pain no no chest pain [INS:all] [SUB:alright-&gt;right] and any lightheadedness or feeling dizzy no okay have you had any nausea or vomiting nope any abdominal pain [SUB:no-&gt;nope] have you had any diarrhea sorry what was that have you had any diarrhea no diarrhea okay and have you had any urinary problems [SUB:no-&gt;nope] and have you had any rashes or skin changes no not that i know [INS:of] okay [INS:and] then how about any muscle aches or joint aches [SUB:no-&gt;nope] okay and [DEL:have] [DEL:you] [DEL:had] any muscle weakness no and how [SUB:has-&gt;is] your energy been [INS:have] [INS:you] any fatigue it is been mainly okay just maybe sometimes difficult to get to sleep with all the [DEL:all] [DEL:the] congestion but i do not think [INS:it] [INS:is] my [SUB:energy-&gt;energys] [DEL:has] been affected too much no okay and sorry to go back to this i do not think i asked did you [INS:have] [SUB:notice-&gt;noticed] any discharge from your eyes or any eye redness not discharge but yeah maybe a little bit of redness okay have your eyes been itchy yeah a little bit i would say they have been a bit itchy okay [SUB:alright-&gt;all] [SUB:then-&gt;right] do you have any medical conditions that you see a physician for regularly just [INS:i] [INS:have] [INS:what] [INS:is] [SUB:its-&gt;it] called [INS:it] [INS:is] [INS:called] [INS:high] [INS:like] dyslipidemia okay i see and any medications you take for that just like a statin medication okay do you take any other medications over the counter prescribed no [INS:just] other than that i take multivitamins okay and do you have any allergies to medications or like environmental allergies that might be getting worse no not that i know [INS:of] okay so you do not experience any symptoms like this when the seasons change i do not think so i have had this happen to me i would say like once before it happened like two years ago [INS:yeah] it was pretty similar okay and [SUB:what-&gt;did] [SUB:was-&gt;you] [SUB:done-&gt;have] [SUB:at-&gt;any] [DEL:that] time at that time it kind of just went away on [SUB:it-&gt;its] [DEL:is] own it got better [INS:like] i feel it is definitely worse this time but at that time i did not even go to the doctor [SUB:it-&gt;i] kind of just went away okay i see [INS:and] any [INS:reasons] [SUB:recent-&gt;for] hospitalizations no hospitalizations [INS:no] any surgeries nope [INS:all] [SUB:alright-&gt;right] and could you tell me [SUB:where-&gt;whereabouts] [DEL:abouts] you are living currently and who you are living with yeah so i am currently living in an apartment by myself just outside of london okay and anybody that you have been around who is had any symptoms no not that i know of okay so no sick contacts and have you traveled anywhere out of the city or province no i have tried to stay home besides going to work i just work at the grocery store besides that [DEL:no] nowhere else okay and any of your coworkers have any symptoms or any coworkers being off sick no we are pretty careful right now with the pandemic i see yeah [INS:no] that is great okay and do you smoke cigarettes no i quit just a couple [DEL:of] years ago oh that is great it is not [INS:yeah] [INS:it] [INS:is] [INS:not] easy to quit so that is awesome and do you drink alcohol just maybe like red wine a couple of times a week i see okay and do you use any recreational drugs just in a month maybe once or twice i smoke a joint okay and anybody in the family have any lung or heart conditions no not that i know of [INS:all] [SUB:alright-&gt;right] and how about any cancer in the family no no [INS:no] cancers okay i think [DEL:i] that was everything i wanted to ask about today was there any other symptoms or anything else that you wanted to make sure i knew about today no i think that is all i just did not know if i needed any [DEL:like] medications or if i needed to get tested i just wanted to make sure yeah so [INS:we] [SUB:well-&gt;will] certainly check your temperature to see if you have a fever and if you do and it is high enough that will increase the chance that you have a bacterial sinusitis [INS:with] and if so with some of your symptoms including the discharge obstruction loss of smell and facial pain that all fits the picture for it and also you had a period where you felt a little bit better and then worse again so that might require antibiotics but we will check your temperature and go from there [INS:all] [SUB:alright-&gt;right] sounds good thank you so much thank you</t>
         </is>
       </c>
     </row>

</xml_diff>